<commit_message>
Significant edits to remove option to read management via input Excel file - simplifies code
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ORATOR\setup\lookup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADCEA18-AF7B-421B-8B2A-5A4C53851523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B8CCAB-301B-437C-A07B-2FC15BEC661F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="-30" windowWidth="27060" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29175" yWindow="-105" windowWidth="24870" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="498">
   <si>
     <t>PyOrator variable</t>
   </si>
@@ -1787,9 +1787,6 @@
     <t xml:space="preserve"> (eq.2.4.13)</t>
   </si>
   <si>
-    <t>n2o_release</t>
-  </si>
-  <si>
     <t>(eq.2.4.15)</t>
   </si>
   <si>
@@ -1893,30 +1890,6 @@
   </si>
   <si>
     <t>Optimum N supply</t>
-  </si>
-  <si>
-    <r>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>O released</t>
-    </r>
   </si>
   <si>
     <r>
@@ -2452,6 +2425,69 @@
   </si>
   <si>
     <t>n_denit_max</t>
+  </si>
+  <si>
+    <t>n2o_relse_denit</t>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>O released from denitrified N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>O released from nitrified N</t>
+    </r>
+  </si>
+  <si>
+    <t>n2o_relse_nitrif</t>
+  </si>
+  <si>
+    <t>prop_n2o_fc</t>
+  </si>
+  <si>
+    <t>prop_nitrif_gas</t>
+  </si>
+  <si>
+    <t>k_c_rate</t>
   </si>
 </sst>
 </file>
@@ -2707,7 +2743,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -10715,8 +10758,8 @@
   <dimension ref="A1:H235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E157" sqref="E157"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
@@ -10737,10 +10780,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -10775,7 +10818,7 @@
         <v>286</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -10829,10 +10872,10 @@
         <v>276</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
@@ -10847,10 +10890,10 @@
     </row>
     <row r="8" spans="1:8" ht="18" customHeight="1">
       <c r="A8" s="28" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
@@ -10865,10 +10908,10 @@
     </row>
     <row r="9" spans="1:8" ht="18" customHeight="1">
       <c r="A9" s="28" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
@@ -10883,10 +10926,10 @@
     </row>
     <row r="10" spans="1:8" ht="18" customHeight="1">
       <c r="A10" s="28" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
@@ -10904,10 +10947,10 @@
         <v>275</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
@@ -10922,10 +10965,10 @@
     </row>
     <row r="12" spans="1:8" ht="18" customHeight="1">
       <c r="A12" s="28" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
@@ -10940,19 +10983,19 @@
     </row>
     <row r="13" spans="1:8" ht="18" customHeight="1">
       <c r="A13" s="28" t="s">
+        <v>383</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="C13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>385</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>476</v>
-      </c>
-      <c r="C13" t="s">
-        <v>388</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>387</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>12</v>
@@ -10963,19 +11006,19 @@
     </row>
     <row r="14" spans="1:8" ht="18" customHeight="1">
       <c r="A14" s="28" t="s">
+        <v>387</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="C14" t="s">
+        <v>388</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>389</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>476</v>
-      </c>
-      <c r="C14" t="s">
-        <v>390</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>391</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>12</v>
@@ -10986,19 +11029,19 @@
     </row>
     <row r="15" spans="1:8" ht="18" customHeight="1">
       <c r="A15" s="28" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C15" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>12</v>
@@ -11009,19 +11052,19 @@
     </row>
     <row r="16" spans="1:8" ht="18" customHeight="1">
       <c r="A16" s="28" t="s">
+        <v>395</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="C16" t="s">
+        <v>396</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>397</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>476</v>
-      </c>
-      <c r="C16" t="s">
-        <v>398</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>386</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>399</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>12</v>
@@ -11035,7 +11078,7 @@
         <v>274</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>20</v>
@@ -11116,10 +11159,10 @@
         <v>26</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
@@ -11137,10 +11180,10 @@
         <v>28</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
@@ -11158,10 +11201,10 @@
         <v>30</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
@@ -11176,13 +11219,13 @@
     </row>
     <row r="26" spans="1:7" ht="18" customHeight="1">
       <c r="A26" s="28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
@@ -11261,13 +11304,13 @@
     </row>
     <row r="32" spans="1:7" ht="18" customHeight="1">
       <c r="A32" s="28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C32" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
@@ -11282,13 +11325,13 @@
     </row>
     <row r="33" spans="1:7" ht="18" customHeight="1">
       <c r="A33" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C33" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
@@ -11306,10 +11349,10 @@
         <v>273</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C34" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
@@ -11364,17 +11407,17 @@
     </row>
     <row r="38" spans="1:7" ht="18" customHeight="1">
       <c r="A38" s="28" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>12</v>
@@ -11385,17 +11428,17 @@
     </row>
     <row r="39" spans="1:7" ht="18" customHeight="1">
       <c r="A39" s="28" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C39" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>12</v>
@@ -11406,7 +11449,7 @@
     </row>
     <row r="40" spans="1:7" ht="18" customHeight="1">
       <c r="B40" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
@@ -11421,17 +11464,17 @@
     </row>
     <row r="41" spans="1:7" ht="18" customHeight="1">
       <c r="A41" s="28" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="4" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>12</v>
@@ -11442,17 +11485,17 @@
     </row>
     <row r="42" spans="1:7" ht="18" customHeight="1">
       <c r="A42" s="28" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F42" s="5" t="s">
         <v>12</v>
@@ -11463,17 +11506,17 @@
     </row>
     <row r="43" spans="1:7" ht="18" customHeight="1">
       <c r="A43" s="28" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="4" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>12</v>
@@ -11484,17 +11527,17 @@
     </row>
     <row r="44" spans="1:7" ht="18" customHeight="1">
       <c r="A44" s="28" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>12</v>
@@ -11505,13 +11548,13 @@
     </row>
     <row r="45" spans="1:7" ht="18" customHeight="1">
       <c r="A45" s="28" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
@@ -11538,7 +11581,7 @@
     </row>
     <row r="47" spans="1:7" ht="18" customHeight="1">
       <c r="A47" s="28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4" t="s">
@@ -11637,13 +11680,13 @@
     </row>
     <row r="55" spans="1:8" ht="18" customHeight="1">
       <c r="A55" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
@@ -11658,13 +11701,13 @@
     </row>
     <row r="56" spans="1:8" ht="18" customHeight="1">
       <c r="A56" s="28" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
@@ -11679,10 +11722,10 @@
     </row>
     <row r="57" spans="1:8" ht="18" customHeight="1">
       <c r="D57" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="F57" s="5" t="s">
         <v>9</v>
@@ -11707,10 +11750,10 @@
     </row>
     <row r="59" spans="1:8" ht="18" customHeight="1">
       <c r="A59" s="28" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>62</v>
@@ -11727,6 +11770,9 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="18" customHeight="1">
+      <c r="A60" s="28" t="s">
+        <v>497</v>
+      </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
         <v>63</v>
@@ -11779,10 +11825,10 @@
         <v>312</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
@@ -11803,10 +11849,10 @@
         <v>309</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
@@ -11827,10 +11873,10 @@
         <v>308</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
@@ -12087,7 +12133,7 @@
         <v>291</v>
       </c>
       <c r="B85" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
@@ -12102,13 +12148,13 @@
     </row>
     <row r="86" spans="1:8" ht="18" customHeight="1">
       <c r="A86" s="28" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
@@ -12126,7 +12172,7 @@
         <v>314</v>
       </c>
       <c r="B87" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
@@ -12141,13 +12187,13 @@
     </row>
     <row r="88" spans="1:8" ht="18" customHeight="1">
       <c r="A88" s="28" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="B88" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
@@ -12165,13 +12211,13 @@
     </row>
     <row r="89" spans="1:8" ht="18" customHeight="1">
       <c r="A89" s="28" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C89" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
@@ -12189,13 +12235,13 @@
     </row>
     <row r="90" spans="1:8" ht="18" customHeight="1">
       <c r="A90" s="28" t="s">
-        <v>318</v>
+        <v>491</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C90" t="s">
-        <v>354</v>
+        <v>492</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
@@ -12267,13 +12313,13 @@
     </row>
     <row r="95" spans="1:8" ht="18" customHeight="1">
       <c r="A95" s="28" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
@@ -12291,10 +12337,10 @@
         <v>293</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
@@ -12309,13 +12355,13 @@
     </row>
     <row r="97" spans="1:8" ht="18" customHeight="1">
       <c r="A97" s="28" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C97" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
@@ -12333,10 +12379,10 @@
         <v>297</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4" t="s">
@@ -12354,10 +12400,10 @@
         <v>298</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D99" s="10" t="s">
         <v>303</v>
@@ -12374,17 +12420,17 @@
     </row>
     <row r="100" spans="1:8" ht="18" customHeight="1">
       <c r="A100" s="28" t="s">
+        <v>428</v>
+      </c>
+      <c r="B100" s="25" t="s">
+        <v>473</v>
+      </c>
+      <c r="C100" t="s">
         <v>430</v>
-      </c>
-      <c r="B100" s="25" t="s">
-        <v>475</v>
-      </c>
-      <c r="C100" t="s">
-        <v>432</v>
       </c>
       <c r="D100" s="10"/>
       <c r="E100" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F100" s="5" t="s">
         <v>92</v>
@@ -12395,17 +12441,17 @@
     </row>
     <row r="101" spans="1:8" ht="18" customHeight="1">
       <c r="A101" s="28" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C101" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D101" s="10"/>
       <c r="E101" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="F101" s="5" t="s">
         <v>92</v>
@@ -12416,10 +12462,10 @@
     </row>
     <row r="102" spans="1:8" ht="18" customHeight="1">
       <c r="A102" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
@@ -12437,10 +12483,10 @@
         <v>299</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D103" s="10" t="s">
         <v>302</v>
@@ -12460,10 +12506,10 @@
         <v>301</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
@@ -12478,17 +12524,17 @@
     </row>
     <row r="105" spans="1:8" ht="18" customHeight="1">
       <c r="A105" s="28" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="F105" s="5" t="s">
         <v>92</v>
@@ -12499,17 +12545,17 @@
     </row>
     <row r="106" spans="1:8" ht="18" customHeight="1">
       <c r="A106" s="28" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>92</v>
@@ -12523,10 +12569,10 @@
         <v>300</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4" t="s">
@@ -12539,18 +12585,18 @@
         <v>7</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="18" customHeight="1">
       <c r="A108" s="28" t="s">
+        <v>427</v>
+      </c>
+      <c r="B108" s="25" t="s">
+        <v>473</v>
+      </c>
+      <c r="C108" s="4" t="s">
         <v>429</v>
-      </c>
-      <c r="B108" s="25" t="s">
-        <v>475</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>431</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4" t="s">
@@ -12563,10 +12609,19 @@
         <v>7</v>
       </c>
       <c r="H108" s="13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="18" customHeight="1">
+      <c r="A109" s="28" t="s">
+        <v>494</v>
+      </c>
+      <c r="B109" s="25" t="s">
+        <v>473</v>
+      </c>
+      <c r="C109" t="s">
+        <v>493</v>
+      </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4" t="s">
         <v>111</v>
@@ -12595,10 +12650,10 @@
         <v>292</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4" t="s">
@@ -12613,13 +12668,13 @@
     </row>
     <row r="112" spans="1:8" ht="18" customHeight="1">
       <c r="A112" s="28" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C112" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
@@ -12637,10 +12692,10 @@
         <v>283</v>
       </c>
       <c r="B113" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4" t="s">
@@ -12658,10 +12713,10 @@
         <v>284</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>255</v>
@@ -12678,13 +12733,13 @@
     </row>
     <row r="115" spans="1:8" ht="18" customHeight="1">
       <c r="A115" s="28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B115" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C115" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4" t="s">
@@ -12697,7 +12752,7 @@
         <v>7</v>
       </c>
       <c r="H115" s="13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="18" customHeight="1">
@@ -12705,10 +12760,10 @@
         <v>285</v>
       </c>
       <c r="B116" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>256</v>
@@ -12725,17 +12780,17 @@
     </row>
     <row r="117" spans="1:8" ht="18" customHeight="1">
       <c r="A117" s="28" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B117" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D117" s="9"/>
       <c r="E117" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="F117" s="5" t="s">
         <v>92</v>
@@ -12746,13 +12801,13 @@
     </row>
     <row r="118" spans="1:8" ht="18" customHeight="1">
       <c r="A118" s="28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B118" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
@@ -12767,17 +12822,17 @@
     </row>
     <row r="119" spans="1:8" ht="18" customHeight="1">
       <c r="A119" s="28" t="s">
+        <v>411</v>
+      </c>
+      <c r="B119" s="25" t="s">
+        <v>473</v>
+      </c>
+      <c r="C119" s="4" t="s">
         <v>413</v>
-      </c>
-      <c r="B119" s="25" t="s">
-        <v>475</v>
-      </c>
-      <c r="C119" s="4" t="s">
-        <v>415</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F119" s="5" t="s">
         <v>92</v>
@@ -12788,10 +12843,10 @@
     </row>
     <row r="120" spans="1:8" ht="18" customHeight="1">
       <c r="A120" s="28" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B120" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4" t="s">
@@ -12809,10 +12864,10 @@
         <v>282</v>
       </c>
       <c r="B121" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4" t="s">
@@ -12830,10 +12885,10 @@
         <v>295</v>
       </c>
       <c r="B122" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4" t="s">
@@ -12848,17 +12903,17 @@
     </row>
     <row r="123" spans="1:8" ht="18" customHeight="1">
       <c r="A123" s="28" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B123" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="F123" s="5" t="s">
         <v>92</v>
@@ -12872,10 +12927,10 @@
         <v>294</v>
       </c>
       <c r="B124" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4" t="s">
@@ -12890,10 +12945,10 @@
     </row>
     <row r="125" spans="1:8" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A125" s="30" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B125" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>123</v>
@@ -12915,7 +12970,7 @@
         <v>306</v>
       </c>
       <c r="B126" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4" t="s">
@@ -13050,7 +13105,7 @@
         <v>304</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4" t="s">
@@ -13066,10 +13121,10 @@
     </row>
     <row r="137" spans="1:8" ht="18" customHeight="1">
       <c r="A137" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B137" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4" t="s">
@@ -13085,10 +13140,10 @@
     </row>
     <row r="138" spans="1:8" ht="18" customHeight="1">
       <c r="A138" s="28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B138" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4" t="s">
@@ -13133,7 +13188,7 @@
         <v>305</v>
       </c>
       <c r="B141" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4" t="s">
@@ -13152,7 +13207,7 @@
         <v>296</v>
       </c>
       <c r="B142" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D142" s="4"/>
       <c r="E142" s="4" t="s">
@@ -13182,6 +13237,9 @@
       <c r="H143"/>
     </row>
     <row r="144" spans="1:8" ht="18" customHeight="1">
+      <c r="A144" s="8" t="s">
+        <v>496</v>
+      </c>
       <c r="D144" s="4"/>
       <c r="E144" s="4" t="s">
         <v>142</v>
@@ -13199,10 +13257,10 @@
         <v>281</v>
       </c>
       <c r="B145" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D145" s="4"/>
       <c r="E145" s="4" t="s">
@@ -13217,6 +13275,12 @@
       <c r="H145"/>
     </row>
     <row r="146" spans="1:8" ht="18" customHeight="1">
+      <c r="A146" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="B146" s="25" t="s">
+        <v>473</v>
+      </c>
       <c r="D146" s="4"/>
       <c r="E146" s="4" t="s">
         <v>144</v>
@@ -13257,13 +13321,13 @@
     </row>
     <row r="149" spans="1:8" ht="18" customHeight="1">
       <c r="A149" s="28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B149" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C149" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
@@ -13276,7 +13340,7 @@
         <v>7</v>
       </c>
       <c r="H149" s="13" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="150" spans="1:8" ht="18" customHeight="1">
@@ -13293,10 +13357,10 @@
     </row>
     <row r="151" spans="1:8" ht="18" customHeight="1">
       <c r="A151" s="28" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B151" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4" t="s">
@@ -13323,16 +13387,16 @@
     </row>
     <row r="153" spans="1:8" ht="18" customHeight="1">
       <c r="A153" s="28" t="s">
+        <v>376</v>
+      </c>
+      <c r="B153" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="D153" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="E153" s="4" t="s">
         <v>378</v>
-      </c>
-      <c r="B153" s="25" t="s">
-        <v>476</v>
-      </c>
-      <c r="D153" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="E153" s="4" t="s">
-        <v>380</v>
       </c>
       <c r="F153" s="5" t="s">
         <v>9</v>
@@ -13369,7 +13433,7 @@
     </row>
     <row r="156" spans="1:8" ht="18" customHeight="1">
       <c r="A156" s="28" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4" t="s">
@@ -13384,10 +13448,10 @@
     </row>
     <row r="157" spans="1:8" ht="18" customHeight="1">
       <c r="A157" s="28" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4" t="s">
@@ -13400,18 +13464,18 @@
         <v>7</v>
       </c>
       <c r="H157" s="13" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="158" spans="1:8" ht="18" customHeight="1">
       <c r="A158" s="28" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B158" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C158" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4" t="s">
@@ -13483,7 +13547,7 @@
         <v>279</v>
       </c>
       <c r="B163" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>163</v>
@@ -13579,10 +13643,10 @@
     </row>
     <row r="170" spans="1:8" ht="18" customHeight="1">
       <c r="A170" s="28" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4" t="s">
@@ -13595,7 +13659,7 @@
         <v>7</v>
       </c>
       <c r="H170" s="13" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="171" spans="1:8" ht="18" customHeight="1">
@@ -13603,10 +13667,10 @@
         <v>272</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C171" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D171" s="4"/>
       <c r="E171" s="4" t="s">
@@ -13729,14 +13793,14 @@
     </row>
     <row r="181" spans="1:8" s="15" customFormat="1" ht="18" customHeight="1">
       <c r="A181" s="31" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B181" s="27"/>
       <c r="D181" s="19" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E181" s="15" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F181" s="16"/>
       <c r="G181" s="17"/>
@@ -13860,7 +13924,7 @@
     </row>
     <row r="191" spans="1:8" ht="18" customHeight="1">
       <c r="A191" s="28" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D191" s="4"/>
       <c r="E191" s="4" t="s">
@@ -13911,13 +13975,13 @@
     </row>
     <row r="195" spans="1:7" ht="18" customHeight="1">
       <c r="A195" s="28" t="s">
+        <v>433</v>
+      </c>
+      <c r="B195" s="25" t="s">
+        <v>475</v>
+      </c>
+      <c r="C195" s="4" t="s">
         <v>435</v>
-      </c>
-      <c r="B195" s="25" t="s">
-        <v>477</v>
-      </c>
-      <c r="C195" s="4" t="s">
-        <v>437</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>267</v>
@@ -13934,13 +13998,13 @@
     </row>
     <row r="196" spans="1:7" ht="18" customHeight="1">
       <c r="A196" s="28" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B196" s="25" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D196" s="9"/>
       <c r="E196" s="4" t="s">
@@ -13955,17 +14019,17 @@
     </row>
     <row r="197" spans="1:7" ht="18" customHeight="1">
       <c r="A197" s="28" t="s">
+        <v>434</v>
+      </c>
+      <c r="B197" s="25" t="s">
+        <v>475</v>
+      </c>
+      <c r="C197" s="4" t="s">
         <v>436</v>
-      </c>
-      <c r="B197" s="25" t="s">
-        <v>477</v>
-      </c>
-      <c r="C197" s="4" t="s">
-        <v>438</v>
       </c>
       <c r="D197" s="9"/>
       <c r="E197" s="4" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F197" s="5" t="s">
         <v>53</v>
@@ -13976,13 +14040,13 @@
     </row>
     <row r="198" spans="1:7" ht="18" customHeight="1">
       <c r="A198" s="29" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B198" s="25" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D198" s="4"/>
       <c r="E198" s="4" t="s">
@@ -13997,7 +14061,7 @@
     </row>
     <row r="199" spans="1:7" ht="18" customHeight="1">
       <c r="A199" s="28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D199" s="4"/>
       <c r="E199" s="4" t="s">
@@ -14038,13 +14102,13 @@
     </row>
     <row r="202" spans="1:7" ht="18" customHeight="1">
       <c r="A202" s="28" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B202" s="25" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="D202" s="4"/>
       <c r="E202" s="4" t="s">
@@ -14059,7 +14123,7 @@
     </row>
     <row r="203" spans="1:7" ht="18" customHeight="1">
       <c r="A203" s="30" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D203" s="4"/>
       <c r="E203" s="4" t="s">
@@ -14110,13 +14174,13 @@
     </row>
     <row r="207" spans="1:7" ht="18" customHeight="1">
       <c r="A207" s="28" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B207" s="25" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C207" s="4" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4" t="s">
@@ -14149,14 +14213,14 @@
         <v>289</v>
       </c>
       <c r="B209" s="25" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C209" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D209" s="4"/>
       <c r="E209" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F209" s="5" t="s">
         <v>53</v>
@@ -14191,17 +14255,17 @@
     </row>
     <row r="212" spans="1:8" ht="18" customHeight="1">
       <c r="A212" s="28" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B212" s="25" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D212" s="4"/>
       <c r="E212" s="4" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F212" s="5" t="s">
         <v>53</v>
@@ -14212,17 +14276,17 @@
     </row>
     <row r="213" spans="1:8" ht="18" customHeight="1">
       <c r="A213" s="28" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B213" s="25" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C213" s="4" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D213" s="4"/>
       <c r="E213" s="4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F213" s="5" t="s">
         <v>53</v>
@@ -14236,10 +14300,10 @@
         <v>287</v>
       </c>
       <c r="B214" s="25" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D214" s="10" t="s">
         <v>288</v>
@@ -14254,7 +14318,7 @@
         <v>7</v>
       </c>
       <c r="H214" s="13" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="215" spans="1:8" ht="18" customHeight="1">
@@ -14344,10 +14408,10 @@
         <v>307</v>
       </c>
       <c r="B221" s="25" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C221" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D221" s="4"/>
       <c r="E221" s="4" t="s">
@@ -14389,7 +14453,7 @@
     </row>
     <row r="224" spans="1:8" ht="18" customHeight="1">
       <c r="A224" s="28" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D224" s="4"/>
       <c r="E224" s="4" t="s">
@@ -14405,7 +14469,7 @@
     </row>
     <row r="225" spans="1:8" ht="18" customHeight="1">
       <c r="A225" s="28" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D225" s="4"/>
       <c r="E225" s="4" t="s">
@@ -14551,62 +14615,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J150">
-    <cfRule type="expression" priority="12">
+    <cfRule type="expression" priority="13">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D198:XFD198 D115:XFD115 A181:C181 F181:XFD181 A182:XFD195 A111:A114 C111:XFD114 A116:A125 C116:XFD125 A126:XFD144 A146:XFD148 A145 C145:XFD145 A150:XFD150 A149 C149:XFD149 A151 C151:XFD151 A152:XFD156 A157 C157:XFD157 A158:XFD169 A172:XFD180 A170:A171 C170:XFD171 A196:A197 C196:XFD197 A199:XFD220 A222:XFD1048576 A221 C221:XFD221 A1:XFD110">
-    <cfRule type="expression" dxfId="0" priority="11">
+  <conditionalFormatting sqref="D198:XFD198 D115:XFD115 A181:C181 F181:XFD181 A182:XFD195 A111:A114 C111:XFD114 A116:A125 C116:XFD125 A126:XFD144 A147:XFD148 A150:XFD150 A149 C149:XFD149 A151 C151:XFD151 A152:XFD156 A157 C157:XFD157 A158:XFD169 A172:XFD180 A170:A171 C170:XFD171 A196:A197 C196:XFD197 A199:XFD220 A222:XFD1048576 A221 C221:XFD221 A1:XFD110 A145:A146 C145:XFD146">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C198">
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B111:B125">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B149">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B151">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B157">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B171">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B170">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B196:B198">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B221">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B146">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
improvements to Excel output files and experiments with fonts
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B8CCAB-301B-437C-A07B-2FC15BEC661F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0997FBCE-EA6D-4519-90F8-23C9504FFD71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29175" yWindow="-105" windowWidth="24870" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3090" yWindow="105" windowWidth="25710" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -2250,9 +2250,6 @@
     <t>NH4 loss adjusted ???</t>
   </si>
   <si>
-    <t>wat_stress_index</t>
-  </si>
-  <si>
     <t>aet</t>
   </si>
   <si>
@@ -2488,6 +2485,9 @@
   </si>
   <si>
     <t>k_c_rate</t>
+  </si>
+  <si>
+    <t>wat_strss_indx</t>
   </si>
 </sst>
 </file>
@@ -10758,8 +10758,8 @@
   <dimension ref="A1:H235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A60" sqref="A60"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1"/>
@@ -10780,7 +10780,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>349</v>
@@ -10818,7 +10818,7 @@
         <v>286</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -10872,7 +10872,7 @@
         <v>276</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C7" t="s">
         <v>353</v>
@@ -10893,7 +10893,7 @@
         <v>347</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
@@ -10911,7 +10911,7 @@
         <v>346</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
@@ -10929,7 +10929,7 @@
         <v>348</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
@@ -10947,7 +10947,7 @@
         <v>275</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>370</v>
@@ -10968,7 +10968,7 @@
         <v>343</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
@@ -10986,7 +10986,7 @@
         <v>383</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C13" t="s">
         <v>386</v>
@@ -11009,7 +11009,7 @@
         <v>387</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C14" t="s">
         <v>388</v>
@@ -11032,7 +11032,7 @@
         <v>393</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C15" t="s">
         <v>391</v>
@@ -11055,7 +11055,7 @@
         <v>395</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C16" t="s">
         <v>396</v>
@@ -11078,7 +11078,7 @@
         <v>274</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>20</v>
@@ -11159,7 +11159,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>379</v>
@@ -11180,7 +11180,7 @@
         <v>28</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>380</v>
@@ -11201,7 +11201,7 @@
         <v>30</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>381</v>
@@ -11222,7 +11222,7 @@
         <v>330</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>382</v>
@@ -11307,7 +11307,7 @@
         <v>331</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C32" t="s">
         <v>372</v>
@@ -11328,7 +11328,7 @@
         <v>332</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C33" t="s">
         <v>373</v>
@@ -11349,7 +11349,7 @@
         <v>273</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C34" t="s">
         <v>371</v>
@@ -11410,7 +11410,7 @@
         <v>398</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>402</v>
@@ -11431,7 +11431,7 @@
         <v>399</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C39" t="s">
         <v>403</v>
@@ -11449,7 +11449,7 @@
     </row>
     <row r="40" spans="1:7" ht="18" customHeight="1">
       <c r="B40" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
@@ -11467,7 +11467,7 @@
         <v>358</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>366</v>
@@ -11488,7 +11488,7 @@
         <v>359</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>367</v>
@@ -11509,7 +11509,7 @@
         <v>360</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>368</v>
@@ -11530,7 +11530,7 @@
         <v>365</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>369</v>
@@ -11551,7 +11551,7 @@
         <v>336</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>350</v>
@@ -11683,10 +11683,10 @@
         <v>334</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4" t="s">
@@ -11704,10 +11704,10 @@
         <v>333</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
@@ -11750,10 +11750,10 @@
     </row>
     <row r="59" spans="1:8" ht="18" customHeight="1">
       <c r="A59" s="28" t="s">
-        <v>432</v>
+        <v>497</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>62</v>
@@ -11771,7 +11771,7 @@
     </row>
     <row r="60" spans="1:8" ht="18" customHeight="1">
       <c r="A60" s="28" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
@@ -11825,10 +11825,10 @@
         <v>312</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
@@ -11849,10 +11849,10 @@
         <v>309</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
@@ -11873,10 +11873,10 @@
         <v>308</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
@@ -12133,7 +12133,7 @@
         <v>291</v>
       </c>
       <c r="B85" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4" t="s">
@@ -12148,13 +12148,13 @@
     </row>
     <row r="86" spans="1:8" ht="18" customHeight="1">
       <c r="A86" s="28" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
@@ -12172,7 +12172,7 @@
         <v>314</v>
       </c>
       <c r="B87" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
@@ -12187,13 +12187,13 @@
     </row>
     <row r="88" spans="1:8" ht="18" customHeight="1">
       <c r="A88" s="28" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B88" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
@@ -12211,13 +12211,13 @@
     </row>
     <row r="89" spans="1:8" ht="18" customHeight="1">
       <c r="A89" s="28" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C89" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
@@ -12235,13 +12235,13 @@
     </row>
     <row r="90" spans="1:8" ht="18" customHeight="1">
       <c r="A90" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="B90" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="C90" t="s">
         <v>491</v>
-      </c>
-      <c r="B90" s="25" t="s">
-        <v>473</v>
-      </c>
-      <c r="C90" t="s">
-        <v>492</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
@@ -12316,10 +12316,10 @@
         <v>338</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
@@ -12337,10 +12337,10 @@
         <v>293</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
@@ -12358,10 +12358,10 @@
         <v>337</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C97" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
@@ -12379,10 +12379,10 @@
         <v>297</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4" t="s">
@@ -12400,10 +12400,10 @@
         <v>298</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D99" s="10" t="s">
         <v>303</v>
@@ -12423,7 +12423,7 @@
         <v>428</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C100" t="s">
         <v>430</v>
@@ -12441,17 +12441,17 @@
     </row>
     <row r="101" spans="1:8" ht="18" customHeight="1">
       <c r="A101" s="28" t="s">
+        <v>437</v>
+      </c>
+      <c r="B101" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="C101" t="s">
         <v>438</v>
-      </c>
-      <c r="B101" s="25" t="s">
-        <v>473</v>
-      </c>
-      <c r="C101" t="s">
-        <v>439</v>
       </c>
       <c r="D101" s="10"/>
       <c r="E101" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F101" s="5" t="s">
         <v>92</v>
@@ -12465,7 +12465,7 @@
         <v>339</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
@@ -12483,10 +12483,10 @@
         <v>299</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D103" s="10" t="s">
         <v>302</v>
@@ -12506,10 +12506,10 @@
         <v>301</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
@@ -12527,7 +12527,7 @@
         <v>416</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>421</v>
@@ -12548,7 +12548,7 @@
         <v>417</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>420</v>
@@ -12569,10 +12569,10 @@
         <v>300</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D107" s="4"/>
       <c r="E107" s="4" t="s">
@@ -12593,7 +12593,7 @@
         <v>427</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>429</v>
@@ -12614,13 +12614,13 @@
     </row>
     <row r="109" spans="1:8" ht="18" customHeight="1">
       <c r="A109" s="28" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C109" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4" t="s">
@@ -12650,10 +12650,10 @@
         <v>292</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="4" t="s">
@@ -12671,7 +12671,7 @@
         <v>408</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C112" t="s">
         <v>409</v>
@@ -12692,10 +12692,10 @@
         <v>283</v>
       </c>
       <c r="B113" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4" t="s">
@@ -12713,10 +12713,10 @@
         <v>284</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D114" s="9" t="s">
         <v>255</v>
@@ -12736,10 +12736,10 @@
         <v>341</v>
       </c>
       <c r="B115" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C115" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4" t="s">
@@ -12760,10 +12760,10 @@
         <v>285</v>
       </c>
       <c r="B116" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D116" s="9" t="s">
         <v>256</v>
@@ -12783,7 +12783,7 @@
         <v>406</v>
       </c>
       <c r="B117" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>407</v>
@@ -12804,10 +12804,10 @@
         <v>340</v>
       </c>
       <c r="B118" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
@@ -12825,7 +12825,7 @@
         <v>411</v>
       </c>
       <c r="B119" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>413</v>
@@ -12846,7 +12846,7 @@
         <v>339</v>
       </c>
       <c r="B120" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4" t="s">
@@ -12864,10 +12864,10 @@
         <v>282</v>
       </c>
       <c r="B121" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4" t="s">
@@ -12885,7 +12885,7 @@
         <v>295</v>
       </c>
       <c r="B122" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>422</v>
@@ -12906,7 +12906,7 @@
         <v>414</v>
       </c>
       <c r="B123" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C123" s="4" t="s">
         <v>423</v>
@@ -12927,7 +12927,7 @@
         <v>294</v>
       </c>
       <c r="B124" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C124" s="4" t="s">
         <v>352</v>
@@ -12948,7 +12948,7 @@
         <v>404</v>
       </c>
       <c r="B125" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>123</v>
@@ -12970,7 +12970,7 @@
         <v>306</v>
       </c>
       <c r="B126" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D126" s="4"/>
       <c r="E126" s="4" t="s">
@@ -13105,7 +13105,7 @@
         <v>304</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4" t="s">
@@ -13124,7 +13124,7 @@
         <v>345</v>
       </c>
       <c r="B137" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D137" s="4"/>
       <c r="E137" s="4" t="s">
@@ -13143,7 +13143,7 @@
         <v>344</v>
       </c>
       <c r="B138" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4" t="s">
@@ -13188,7 +13188,7 @@
         <v>305</v>
       </c>
       <c r="B141" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4" t="s">
@@ -13207,7 +13207,7 @@
         <v>296</v>
       </c>
       <c r="B142" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D142" s="4"/>
       <c r="E142" s="4" t="s">
@@ -13238,7 +13238,7 @@
     </row>
     <row r="144" spans="1:8" ht="18" customHeight="1">
       <c r="A144" s="8" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D144" s="4"/>
       <c r="E144" s="4" t="s">
@@ -13257,10 +13257,10 @@
         <v>281</v>
       </c>
       <c r="B145" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D145" s="4"/>
       <c r="E145" s="4" t="s">
@@ -13276,10 +13276,10 @@
     </row>
     <row r="146" spans="1:8" ht="18" customHeight="1">
       <c r="A146" s="8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B146" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D146" s="4"/>
       <c r="E146" s="4" t="s">
@@ -13324,10 +13324,10 @@
         <v>319</v>
       </c>
       <c r="B149" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C149" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
@@ -13360,7 +13360,7 @@
         <v>329</v>
       </c>
       <c r="B151" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D151" s="4"/>
       <c r="E151" s="4" t="s">
@@ -13390,7 +13390,7 @@
         <v>376</v>
       </c>
       <c r="B153" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D153" s="10" t="s">
         <v>377</v>
@@ -13433,7 +13433,7 @@
     </row>
     <row r="156" spans="1:8" ht="18" customHeight="1">
       <c r="A156" s="28" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4" t="s">
@@ -13451,7 +13451,7 @@
         <v>321</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4" t="s">
@@ -13472,10 +13472,10 @@
         <v>405</v>
       </c>
       <c r="B158" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C158" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4" t="s">
@@ -13547,7 +13547,7 @@
         <v>279</v>
       </c>
       <c r="B163" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>163</v>
@@ -13646,7 +13646,7 @@
         <v>323</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4" t="s">
@@ -13667,7 +13667,7 @@
         <v>272</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C171" t="s">
         <v>351</v>
@@ -13793,7 +13793,7 @@
     </row>
     <row r="181" spans="1:8" s="15" customFormat="1" ht="18" customHeight="1">
       <c r="A181" s="31" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B181" s="27"/>
       <c r="D181" s="19" t="s">
@@ -13975,13 +13975,13 @@
     </row>
     <row r="195" spans="1:7" ht="18" customHeight="1">
       <c r="A195" s="28" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B195" s="25" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D195" s="9" t="s">
         <v>267</v>
@@ -13998,13 +13998,13 @@
     </row>
     <row r="196" spans="1:7" ht="18" customHeight="1">
       <c r="A196" s="28" t="s">
+        <v>448</v>
+      </c>
+      <c r="B196" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="C196" s="4" t="s">
         <v>449</v>
-      </c>
-      <c r="B196" s="25" t="s">
-        <v>475</v>
-      </c>
-      <c r="C196" s="4" t="s">
-        <v>450</v>
       </c>
       <c r="D196" s="9"/>
       <c r="E196" s="4" t="s">
@@ -14019,17 +14019,17 @@
     </row>
     <row r="197" spans="1:7" ht="18" customHeight="1">
       <c r="A197" s="28" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B197" s="25" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D197" s="9"/>
       <c r="E197" s="4" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F197" s="5" t="s">
         <v>53</v>
@@ -14043,10 +14043,10 @@
         <v>326</v>
       </c>
       <c r="B198" s="25" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D198" s="4"/>
       <c r="E198" s="4" t="s">
@@ -14105,7 +14105,7 @@
         <v>426</v>
       </c>
       <c r="B202" s="25" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>425</v>
@@ -14123,7 +14123,7 @@
     </row>
     <row r="203" spans="1:7" ht="18" customHeight="1">
       <c r="A203" s="30" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D203" s="4"/>
       <c r="E203" s="4" t="s">
@@ -14174,13 +14174,13 @@
     </row>
     <row r="207" spans="1:7" ht="18" customHeight="1">
       <c r="A207" s="28" t="s">
+        <v>440</v>
+      </c>
+      <c r="B207" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="C207" s="4" t="s">
         <v>441</v>
-      </c>
-      <c r="B207" s="25" t="s">
-        <v>475</v>
-      </c>
-      <c r="C207" s="4" t="s">
-        <v>442</v>
       </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4" t="s">
@@ -14213,7 +14213,7 @@
         <v>289</v>
       </c>
       <c r="B209" s="25" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C209" t="s">
         <v>354</v>
@@ -14255,17 +14255,17 @@
     </row>
     <row r="212" spans="1:8" ht="18" customHeight="1">
       <c r="A212" s="28" t="s">
+        <v>443</v>
+      </c>
+      <c r="B212" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="C212" s="4" t="s">
         <v>444</v>
-      </c>
-      <c r="B212" s="25" t="s">
-        <v>475</v>
-      </c>
-      <c r="C212" s="4" t="s">
-        <v>445</v>
       </c>
       <c r="D212" s="4"/>
       <c r="E212" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F212" s="5" t="s">
         <v>53</v>
@@ -14276,17 +14276,17 @@
     </row>
     <row r="213" spans="1:8" ht="18" customHeight="1">
       <c r="A213" s="28" t="s">
+        <v>445</v>
+      </c>
+      <c r="B213" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="C213" s="4" t="s">
         <v>446</v>
-      </c>
-      <c r="B213" s="25" t="s">
-        <v>475</v>
-      </c>
-      <c r="C213" s="4" t="s">
-        <v>447</v>
       </c>
       <c r="D213" s="4"/>
       <c r="E213" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F213" s="5" t="s">
         <v>53</v>
@@ -14300,7 +14300,7 @@
         <v>287</v>
       </c>
       <c r="B214" s="25" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C214" s="4" t="s">
         <v>424</v>
@@ -14408,10 +14408,10 @@
         <v>307</v>
       </c>
       <c r="B221" s="25" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C221" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D221" s="4"/>
       <c r="E221" s="4" t="s">
@@ -14453,7 +14453,7 @@
     </row>
     <row r="224" spans="1:8" ht="18" customHeight="1">
       <c r="A224" s="28" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D224" s="4"/>
       <c r="E224" s="4" t="s">
@@ -14469,7 +14469,7 @@
     </row>
     <row r="225" spans="1:8" ht="18" customHeight="1">
       <c r="A225" s="28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D225" s="4"/>
       <c r="E225" s="4" t="s">

</xml_diff>

<commit_message>
incremental improvements aimed at addressing transition issue between steady state and forward runs
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D64236-7E94-4865-A8FF-C4C224A1D44F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07E64B9-DDBF-4BD7-A3F7-859CEF34641A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="840" yWindow="540" windowWidth="27300" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2060,18 +2060,6 @@
     <t>Amount of ammonium available at the end of the month</t>
   </si>
   <si>
-    <t>NH4 available at month end</t>
-  </si>
-  <si>
-    <t>NH4 available at month start</t>
-  </si>
-  <si>
-    <t>NO3 available at month start</t>
-  </si>
-  <si>
-    <t>NO3 available at month end</t>
-  </si>
-  <si>
     <t>Water drained from soil</t>
   </si>
   <si>
@@ -2087,12 +2075,6 @@
     <t>nh4_loss_adj</t>
   </si>
   <si>
-    <t>NH4 volatilisation adjusted</t>
-  </si>
-  <si>
-    <t>NH4 loss adjusted</t>
-  </si>
-  <si>
     <t>NH4 loss adjusted ???</t>
   </si>
   <si>
@@ -2114,9 +2096,6 @@
     <t>nh4_total_loss</t>
   </si>
   <si>
-    <t>NH4 total loss</t>
-  </si>
-  <si>
     <t>NH4 total loss ???</t>
   </si>
   <si>
@@ -2156,54 +2135,9 @@
     <t>N to nitrate by nitrification</t>
   </si>
   <si>
-    <t>N lost from NH4 pool by nitrification</t>
-  </si>
-  <si>
     <t>N immobilised from nitrate pool</t>
   </si>
   <si>
-    <t>N immobilised from NH4 pool</t>
-  </si>
-  <si>
-    <t>Crop N demand NH4 pool</t>
-  </si>
-  <si>
-    <t>Volatilisation of NH4</t>
-  </si>
-  <si>
-    <t>NH4 input from mineralisation</t>
-  </si>
-  <si>
-    <t>NH4 available in soil</t>
-  </si>
-  <si>
-    <t>Fertiliser inputs to NH4 pool</t>
-  </si>
-  <si>
-    <t>Fertiliser inputs to NO3 pool</t>
-  </si>
-  <si>
-    <t>NH4 from atmospheric deposition</t>
-  </si>
-  <si>
-    <t>Loss adjustment factor for NH4</t>
-  </si>
-  <si>
-    <t>Loss adjustment factor for NO3</t>
-  </si>
-  <si>
-    <t>Sum of all NO3 losses</t>
-  </si>
-  <si>
-    <t>NO3 lost by leaching</t>
-  </si>
-  <si>
-    <t>Sum of all NO3 inputs</t>
-  </si>
-  <si>
-    <t>NO3 from atmospheric deposition</t>
-  </si>
-  <si>
     <t>Prop. of the optimum N supply</t>
   </si>
   <si>
@@ -2243,18 +2177,12 @@
     <t xml:space="preserve">N adjustment </t>
   </si>
   <si>
-    <t>Denitrific rate modifier NO3</t>
-  </si>
-  <si>
     <t>Denitrific rate modifier soil mointure</t>
   </si>
   <si>
     <t>Denitrific rate modifier BIO</t>
   </si>
   <si>
-    <t>Prop. of N2 from soil NO3 denitrif</t>
-  </si>
-  <si>
     <t>Max potential monthly denitrific</t>
   </si>
   <si>
@@ -2282,78 +2210,6 @@
     <t>C passed to HUM pool</t>
   </si>
   <si>
-    <r>
-      <t>CO</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> emission</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>O emission from denitrified N</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>N</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>O emission from nitrified N</t>
-    </r>
-  </si>
-  <si>
     <t>c_input_dpm</t>
   </si>
   <si>
@@ -2490,12 +2346,6 @@
   </si>
   <si>
     <t>no3_avail</t>
-  </si>
-  <si>
-    <t>NO3 available in soil</t>
-  </si>
-  <si>
-    <t>Sum of all NH4 inputs</t>
   </si>
   <si>
     <t>Sum of all ammonium-N inputs during the month</t>
@@ -2535,9 +2385,6 @@
     <t>Volatilisation of ammonium or urea-N adjusted</t>
   </si>
   <si>
-    <t>NH4 or urea-N in applied manure</t>
-  </si>
-  <si>
     <t>Amount of ammonium-N or urea-N in applied manure</t>
   </si>
   <si>
@@ -2584,6 +2431,96 @@
   </si>
   <si>
     <t>Crop Name</t>
+  </si>
+  <si>
+    <t>CO2-C emission</t>
+  </si>
+  <si>
+    <t>Loss adjustment factor for NO3-N</t>
+  </si>
+  <si>
+    <t>Denitrific rate modifier NO3-N</t>
+  </si>
+  <si>
+    <t>N2O-N emission from denitrified N</t>
+  </si>
+  <si>
+    <t>N2O-N emission from nitrified N</t>
+  </si>
+  <si>
+    <t>NO3-N available in soil</t>
+  </si>
+  <si>
+    <t>NO3-N from atmospheric deposition</t>
+  </si>
+  <si>
+    <t>Fertiliser inputs to NO3-N pool</t>
+  </si>
+  <si>
+    <t>Sum of all NO3-N inputs</t>
+  </si>
+  <si>
+    <t>NO3-N lost by leaching</t>
+  </si>
+  <si>
+    <t>Sum of all NO3-N losses</t>
+  </si>
+  <si>
+    <t>NO3-N available at month start</t>
+  </si>
+  <si>
+    <t>NO3-N available at month end</t>
+  </si>
+  <si>
+    <t>Prop. of N2 from soil NO3-N denitrif</t>
+  </si>
+  <si>
+    <t>NH4-N available in soil</t>
+  </si>
+  <si>
+    <t>NH4-N from atmospheric deposition</t>
+  </si>
+  <si>
+    <t>Crop N demand NH4-N pool</t>
+  </si>
+  <si>
+    <t>Fertiliser inputs to NH4-N pool</t>
+  </si>
+  <si>
+    <t>N immobilised from NH4-N pool</t>
+  </si>
+  <si>
+    <t>Sum of all NH4-N inputs</t>
+  </si>
+  <si>
+    <t>NH4-N loss adjusted</t>
+  </si>
+  <si>
+    <t>NH4-N total loss</t>
+  </si>
+  <si>
+    <t>NH4-N or urea-N in applied manure</t>
+  </si>
+  <si>
+    <t>NH4-N input from mineralisation</t>
+  </si>
+  <si>
+    <t>N lost from NH4-N pool by nitrification</t>
+  </si>
+  <si>
+    <t>NH4-N available at month start</t>
+  </si>
+  <si>
+    <t>NH4-N available at month end</t>
+  </si>
+  <si>
+    <t>Volatilisation of NH4-N</t>
+  </si>
+  <si>
+    <t>NH4-N volatilisation adjusted</t>
+  </si>
+  <si>
+    <t>Loss adjustment factor for NH4-N</t>
   </si>
 </sst>
 </file>
@@ -2718,7 +2655,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF663300"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2847,34 +2784,20 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <fill>
         <patternFill>
@@ -10910,8 +10833,8 @@
   <dimension ref="A1:H249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C103" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -10932,7 +10855,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>455</v>
+        <v>433</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>338</v>
@@ -10970,7 +10893,7 @@
         <v>277</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -11001,7 +10924,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>7</v>
@@ -11013,7 +10936,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>7</v>
@@ -11021,20 +10944,20 @@
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="28" t="s">
-        <v>505</v>
+        <v>478</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C7" t="s">
-        <v>480</v>
+        <v>526</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>7</v>
@@ -11045,14 +10968,14 @@
         <v>336</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>7</v>
@@ -11063,14 +10986,14 @@
         <v>335</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>7</v>
@@ -11081,14 +11004,14 @@
         <v>337</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>7</v>
@@ -11099,7 +11022,7 @@
         <v>268</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>358</v>
@@ -11109,7 +11032,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>7</v>
@@ -11120,14 +11043,14 @@
         <v>332</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>7</v>
@@ -11138,7 +11061,7 @@
         <v>371</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C13" t="s">
         <v>374</v>
@@ -11150,7 +11073,7 @@
         <v>373</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>7</v>
@@ -11161,7 +11084,7 @@
         <v>375</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C14" t="s">
         <v>376</v>
@@ -11173,7 +11096,7 @@
         <v>377</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>7</v>
@@ -11184,7 +11107,7 @@
         <v>381</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C15" t="s">
         <v>379</v>
@@ -11196,7 +11119,7 @@
         <v>380</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>7</v>
@@ -11207,7 +11130,7 @@
         <v>383</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C16" t="s">
         <v>384</v>
@@ -11219,7 +11142,7 @@
         <v>385</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>7</v>
@@ -11230,7 +11153,7 @@
         <v>267</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
@@ -11240,7 +11163,7 @@
         <v>19</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>7</v>
@@ -11252,7 +11175,7 @@
         <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>7</v>
@@ -11260,17 +11183,17 @@
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="28" t="s">
-        <v>545</v>
+        <v>515</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>547</v>
+        <v>517</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>543</v>
+        <v>513</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>7</v>
@@ -11278,17 +11201,17 @@
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="28" t="s">
-        <v>546</v>
+        <v>516</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>548</v>
+        <v>518</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>544</v>
+        <v>514</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>7</v>
@@ -11300,10 +11223,10 @@
       <c r="E21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="34" t="s">
-        <v>497</v>
-      </c>
-      <c r="G21" s="35" t="s">
+      <c r="F21" s="33" t="s">
+        <v>470</v>
+      </c>
+      <c r="G21" s="34" t="s">
         <v>7</v>
       </c>
       <c r="H21" s="21"/>
@@ -11314,7 +11237,7 @@
         <v>22</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>7</v>
@@ -11326,7 +11249,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>7</v>
@@ -11338,7 +11261,7 @@
         <v>24</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>7</v>
@@ -11349,7 +11272,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>367</v>
@@ -11359,7 +11282,7 @@
         <v>26</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>7</v>
@@ -11370,7 +11293,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>368</v>
@@ -11380,7 +11303,7 @@
         <v>28</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>7</v>
@@ -11391,7 +11314,7 @@
         <v>29</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>369</v>
@@ -11401,7 +11324,7 @@
         <v>30</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>7</v>
@@ -11412,7 +11335,7 @@
         <v>319</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>370</v>
@@ -11422,7 +11345,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>7</v>
@@ -11434,7 +11357,7 @@
         <v>32</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>7</v>
@@ -11448,7 +11371,7 @@
         <v>34</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>7</v>
@@ -11462,7 +11385,7 @@
         <v>35</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>7</v>
@@ -11474,7 +11397,7 @@
         <v>36</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>7</v>
@@ -11486,7 +11409,7 @@
         <v>37</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>7</v>
@@ -11497,7 +11420,7 @@
         <v>320</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C34" t="s">
         <v>360</v>
@@ -11507,7 +11430,7 @@
         <v>38</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>7</v>
@@ -11518,7 +11441,7 @@
         <v>321</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C35" t="s">
         <v>361</v>
@@ -11528,7 +11451,7 @@
         <v>39</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>7</v>
@@ -11539,7 +11462,7 @@
         <v>266</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C36" t="s">
         <v>359</v>
@@ -11549,7 +11472,7 @@
         <v>40</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>7</v>
@@ -11563,7 +11486,7 @@
         <v>41</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>7</v>
@@ -11577,7 +11500,7 @@
         <v>42</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>7</v>
@@ -11589,7 +11512,7 @@
         <v>43</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>7</v>
@@ -11600,17 +11523,17 @@
         <v>386</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>478</v>
+        <v>454</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
         <v>388</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>7</v>
@@ -11618,20 +11541,20 @@
     </row>
     <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="28" t="s">
-        <v>483</v>
+        <v>456</v>
       </c>
       <c r="B41" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="C41" t="s">
         <v>457</v>
-      </c>
-      <c r="C41" t="s">
-        <v>484</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>7</v>
@@ -11642,17 +11565,17 @@
         <v>387</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C42" t="s">
-        <v>479</v>
+        <v>455</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
         <v>389</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>7</v>
@@ -11660,14 +11583,14 @@
     </row>
     <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B43" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>7</v>
@@ -11678,7 +11601,7 @@
         <v>346</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>354</v>
@@ -11688,7 +11611,7 @@
         <v>349</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>7</v>
@@ -11699,7 +11622,7 @@
         <v>347</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>355</v>
@@ -11709,7 +11632,7 @@
         <v>350</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>7</v>
@@ -11720,7 +11643,7 @@
         <v>348</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>356</v>
@@ -11730,7 +11653,7 @@
         <v>351</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>7</v>
@@ -11741,7 +11664,7 @@
         <v>353</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>357</v>
@@ -11751,7 +11674,7 @@
         <v>352</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>7</v>
@@ -11762,7 +11685,7 @@
         <v>325</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>339</v>
@@ -11772,7 +11695,7 @@
         <v>45</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>7</v>
@@ -11780,10 +11703,10 @@
     </row>
     <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="28" t="s">
-        <v>554</v>
+        <v>524</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>555</v>
+        <v>525</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -11795,7 +11718,7 @@
         <v>46</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>7</v>
@@ -11813,7 +11736,7 @@
         <v>47</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>7</v>
@@ -11833,7 +11756,7 @@
     </row>
     <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="28" t="s">
-        <v>486</v>
+        <v>459</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>50</v>
@@ -11914,10 +11837,10 @@
         <v>323</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>448</v>
+        <v>555</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
@@ -11935,10 +11858,10 @@
         <v>322</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>449</v>
+        <v>527</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
@@ -11981,10 +11904,10 @@
     </row>
     <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="28" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>61</v>
@@ -12002,7 +11925,7 @@
     </row>
     <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="28" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
@@ -12056,10 +11979,10 @@
         <v>302</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>469</v>
+        <v>446</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
@@ -12080,10 +12003,10 @@
         <v>299</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>467</v>
+        <v>528</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
@@ -12104,10 +12027,10 @@
         <v>298</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>468</v>
+        <v>445</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
@@ -12129,7 +12052,7 @@
         <v>71</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G71" s="6" t="s">
         <v>7</v>
@@ -12141,7 +12064,7 @@
         <v>72</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>497</v>
+        <v>470</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>7</v>
@@ -12155,7 +12078,7 @@
         <v>73</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G73" s="6" t="s">
         <v>7</v>
@@ -12169,7 +12092,7 @@
         <v>74</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G74" s="6" t="s">
         <v>7</v>
@@ -12183,7 +12106,7 @@
         <v>75</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>7</v>
@@ -12197,7 +12120,7 @@
         <v>76</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G76" s="6" t="s">
         <v>7</v>
@@ -12211,7 +12134,7 @@
         <v>77</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>7</v>
@@ -12225,7 +12148,7 @@
         <v>78</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>7</v>
@@ -12237,7 +12160,7 @@
         <v>79</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>7</v>
@@ -12251,7 +12174,7 @@
         <v>80</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>7</v>
@@ -12265,7 +12188,7 @@
         <v>81</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>7</v>
@@ -12364,14 +12287,14 @@
         <v>282</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
         <v>89</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>7</v>
@@ -12379,20 +12302,20 @@
     </row>
     <row r="90" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A90" s="28" t="s">
-        <v>460</v>
+        <v>438</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>465</v>
+        <v>443</v>
       </c>
       <c r="D90" s="4"/>
-      <c r="E90" s="33" t="s">
-        <v>519</v>
+      <c r="E90" s="35" t="s">
+        <v>492</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>7</v>
@@ -12400,20 +12323,20 @@
     </row>
     <row r="91" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A91" s="28" t="s">
-        <v>518</v>
+        <v>491</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>521</v>
+        <v>494</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
-        <v>520</v>
+        <v>493</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>7</v>
@@ -12424,14 +12347,14 @@
         <v>304</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
         <v>90</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G92" s="6" t="s">
         <v>7</v>
@@ -12439,20 +12362,20 @@
     </row>
     <row r="93" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A93" s="28" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>525</v>
+        <v>498</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
         <v>91</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G93" s="6" t="s">
         <v>7</v>
@@ -12463,20 +12386,20 @@
     </row>
     <row r="94" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="28" t="s">
-        <v>523</v>
+        <v>496</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>524</v>
+        <v>497</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>526</v>
+        <v>499</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G94" s="6" t="s">
         <v>7</v>
@@ -12487,20 +12410,20 @@
     </row>
     <row r="95" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="28" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C95" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G95" s="6" t="s">
         <v>7</v>
@@ -12511,20 +12434,20 @@
     </row>
     <row r="96" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A96" s="28" t="s">
-        <v>506</v>
+        <v>479</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C96" t="s">
-        <v>481</v>
+        <v>529</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G96" s="6" t="s">
         <v>7</v>
@@ -12541,7 +12464,7 @@
         <v>94</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>7</v>
@@ -12555,7 +12478,7 @@
         <v>95</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G98" s="6" t="s">
         <v>7</v>
@@ -12569,7 +12492,7 @@
         <v>96</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>498</v>
+        <v>471</v>
       </c>
       <c r="G99" s="6" t="s">
         <v>7</v>
@@ -12581,7 +12504,7 @@
         <v>97</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>7</v>
@@ -12589,20 +12512,20 @@
     </row>
     <row r="101" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A101" s="28" t="s">
-        <v>508</v>
+        <v>481</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C101" t="s">
-        <v>513</v>
+        <v>486</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
-        <v>510</v>
+        <v>483</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>7</v>
@@ -12610,20 +12533,20 @@
     </row>
     <row r="102" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A102" s="28" t="s">
-        <v>509</v>
+        <v>482</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C102" t="s">
-        <v>512</v>
+        <v>485</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
-        <v>511</v>
+        <v>484</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G102" s="6" t="s">
         <v>7</v>
@@ -12631,20 +12554,20 @@
     </row>
     <row r="103" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A103" s="28" t="s">
-        <v>527</v>
+        <v>500</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>444</v>
+        <v>540</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
         <v>98</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G103" s="6" t="s">
         <v>7</v>
@@ -12655,17 +12578,17 @@
         <v>284</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>447</v>
+        <v>541</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G104" s="6" t="s">
         <v>7</v>
@@ -12676,17 +12599,17 @@
         <v>326</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C105" t="s">
-        <v>441</v>
+        <v>542</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
         <v>100</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G105" s="6" t="s">
         <v>7</v>
@@ -12694,20 +12617,20 @@
     </row>
     <row r="106" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A106" s="28" t="s">
-        <v>492</v>
+        <v>465</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>445</v>
+        <v>543</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4" t="s">
         <v>101</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G106" s="6" t="s">
         <v>7</v>
@@ -12718,10 +12641,10 @@
         <v>288</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>440</v>
+        <v>544</v>
       </c>
       <c r="D107" s="10" t="s">
         <v>293</v>
@@ -12730,7 +12653,7 @@
         <v>102</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G107" s="6" t="s">
         <v>7</v>
@@ -12741,17 +12664,17 @@
         <v>327</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C108" t="s">
-        <v>530</v>
+        <v>545</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4" t="s">
-        <v>531</v>
+        <v>502</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G108" s="6" t="s">
         <v>7</v>
@@ -12762,20 +12685,20 @@
     </row>
     <row r="109" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A109" s="28" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C109" t="s">
-        <v>416</v>
+        <v>546</v>
       </c>
       <c r="D109" s="10"/>
       <c r="E109" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G109" s="6" t="s">
         <v>7</v>
@@ -12783,20 +12706,20 @@
     </row>
     <row r="110" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A110" s="28" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
       <c r="B110" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C110" t="s">
-        <v>424</v>
+        <v>547</v>
       </c>
       <c r="D110" s="10"/>
       <c r="E110" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G110" s="6" t="s">
         <v>7</v>
@@ -12804,22 +12727,22 @@
     </row>
     <row r="111" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A111" s="28" t="s">
-        <v>537</v>
+        <v>508</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C111" t="s">
-        <v>539</v>
+        <v>548</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>536</v>
+        <v>507</v>
       </c>
       <c r="E111" t="s">
-        <v>540</v>
+        <v>510</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G111" s="6" t="s">
         <v>7</v>
@@ -12830,14 +12753,14 @@
         <v>328</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
         <v>103</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G112" s="6" t="s">
         <v>7</v>
@@ -12848,10 +12771,10 @@
         <v>289</v>
       </c>
       <c r="B113" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>443</v>
+        <v>549</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>292</v>
@@ -12860,7 +12783,7 @@
         <v>104</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G113" s="6" t="s">
         <v>7</v>
@@ -12871,17 +12794,17 @@
         <v>291</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>438</v>
+        <v>550</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4" t="s">
         <v>105</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G114" s="6" t="s">
         <v>7</v>
@@ -12889,20 +12812,20 @@
     </row>
     <row r="115" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A115" s="28" t="s">
-        <v>551</v>
+        <v>521</v>
       </c>
       <c r="B115" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>552</v>
+        <v>522</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4" t="s">
-        <v>553</v>
+        <v>523</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G115" s="6" t="s">
         <v>7</v>
@@ -12913,17 +12836,17 @@
         <v>402</v>
       </c>
       <c r="B116" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>407</v>
+        <v>551</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4" t="s">
         <v>404</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G116" s="6" t="s">
         <v>7</v>
@@ -12934,17 +12857,17 @@
         <v>403</v>
       </c>
       <c r="B117" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>406</v>
+        <v>552</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4" t="s">
         <v>405</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G117" s="6" t="s">
         <v>7</v>
@@ -12955,17 +12878,17 @@
         <v>290</v>
       </c>
       <c r="B118" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>442</v>
+        <v>553</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
         <v>106</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G118" s="6" t="s">
         <v>7</v>
@@ -12976,20 +12899,20 @@
     </row>
     <row r="119" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A119" s="28" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="B119" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>415</v>
+        <v>554</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4" t="s">
-        <v>538</v>
+        <v>509</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G119" s="6" t="s">
         <v>7</v>
@@ -13000,20 +12923,20 @@
     </row>
     <row r="120" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A120" s="28" t="s">
-        <v>507</v>
+        <v>480</v>
       </c>
       <c r="B120" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C120" t="s">
-        <v>482</v>
+        <v>530</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G120" s="6" t="s">
         <v>7</v>
@@ -13021,20 +12944,20 @@
     </row>
     <row r="121" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A121" s="28" t="s">
-        <v>534</v>
+        <v>505</v>
       </c>
       <c r="B121" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>535</v>
+        <v>506</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4" t="s">
-        <v>533</v>
+        <v>504</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G121" s="6" t="s">
         <v>7</v>
@@ -13042,20 +12965,20 @@
     </row>
     <row r="122" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A122" s="28" t="s">
-        <v>528</v>
+        <v>501</v>
       </c>
       <c r="B122" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4" t="s">
         <v>108</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G122" s="6" t="s">
         <v>7</v>
@@ -13066,17 +12989,17 @@
         <v>283</v>
       </c>
       <c r="B123" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>453</v>
+        <v>532</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4" t="s">
         <v>109</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G123" s="6" t="s">
         <v>7</v>
@@ -13087,7 +13010,7 @@
         <v>394</v>
       </c>
       <c r="B124" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C124" t="s">
         <v>395</v>
@@ -13097,7 +13020,7 @@
         <v>110</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G124" s="6" t="s">
         <v>7</v>
@@ -13105,20 +13028,20 @@
     </row>
     <row r="125" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A125" s="28" t="s">
-        <v>491</v>
+        <v>464</v>
       </c>
       <c r="B125" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>446</v>
+        <v>533</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G125" s="6" t="s">
         <v>7</v>
@@ -13129,10 +13052,10 @@
         <v>275</v>
       </c>
       <c r="B126" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>248</v>
@@ -13141,7 +13064,7 @@
         <v>112</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G126" s="6" t="s">
         <v>7</v>
@@ -13152,17 +13075,17 @@
         <v>330</v>
       </c>
       <c r="B127" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C127" t="s">
-        <v>452</v>
+        <v>534</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4" t="s">
         <v>113</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G127" s="6" t="s">
         <v>7</v>
@@ -13176,10 +13099,10 @@
         <v>276</v>
       </c>
       <c r="B128" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>451</v>
+        <v>535</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>249</v>
@@ -13188,7 +13111,7 @@
         <v>250</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G128" s="6" t="s">
         <v>7</v>
@@ -13199,7 +13122,7 @@
         <v>392</v>
       </c>
       <c r="B129" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>393</v>
@@ -13209,7 +13132,7 @@
         <v>396</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G129" s="6" t="s">
         <v>7</v>
@@ -13220,17 +13143,17 @@
         <v>329</v>
       </c>
       <c r="B130" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>450</v>
+        <v>536</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4" t="s">
         <v>114</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G130" s="6" t="s">
         <v>7</v>
@@ -13241,7 +13164,7 @@
         <v>397</v>
       </c>
       <c r="B131" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>399</v>
@@ -13251,7 +13174,7 @@
         <v>398</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G131" s="6" t="s">
         <v>7</v>
@@ -13262,14 +13185,14 @@
         <v>328</v>
       </c>
       <c r="B132" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4" t="s">
         <v>115</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G132" s="6" t="s">
         <v>7</v>
@@ -13280,17 +13203,17 @@
         <v>274</v>
       </c>
       <c r="B133" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4" t="s">
         <v>116</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G133" s="6" t="s">
         <v>7</v>
@@ -13301,17 +13224,17 @@
         <v>286</v>
       </c>
       <c r="B134" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>408</v>
+        <v>537</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G134" s="6" t="s">
         <v>7</v>
@@ -13322,17 +13245,17 @@
         <v>400</v>
       </c>
       <c r="B135" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>409</v>
+        <v>538</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4" t="s">
         <v>401</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G135" s="6" t="s">
         <v>7</v>
@@ -13343,7 +13266,7 @@
         <v>285</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>341</v>
@@ -13353,7 +13276,7 @@
         <v>118</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G136" s="6" t="s">
         <v>7</v>
@@ -13364,7 +13287,7 @@
         <v>390</v>
       </c>
       <c r="B137" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>119</v>
@@ -13374,7 +13297,7 @@
         <v>119</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G137" s="6" t="s">
         <v>7</v>
@@ -13386,7 +13309,7 @@
         <v>296</v>
       </c>
       <c r="B138" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4" t="s">
@@ -13401,10 +13324,10 @@
     </row>
     <row r="139" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A139" s="28" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4" t="s">
@@ -13433,10 +13356,10 @@
     </row>
     <row r="141" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A141" s="28" t="s">
-        <v>493</v>
+        <v>466</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>489</v>
+        <v>462</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4" t="s">
@@ -13465,10 +13388,10 @@
     </row>
     <row r="143" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A143" s="28" t="s">
-        <v>494</v>
+        <v>467</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="D143" s="4"/>
       <c r="E143" s="4" t="s">
@@ -13539,7 +13462,7 @@
         <v>294</v>
       </c>
       <c r="B148" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4" t="s">
@@ -13558,7 +13481,7 @@
         <v>334</v>
       </c>
       <c r="B149" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
@@ -13577,7 +13500,7 @@
         <v>333</v>
       </c>
       <c r="B150" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4" t="s">
@@ -13622,7 +13545,7 @@
         <v>295</v>
       </c>
       <c r="B153" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4" t="s">
@@ -13641,7 +13564,7 @@
         <v>287</v>
       </c>
       <c r="B154" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4" t="s">
@@ -13672,7 +13595,7 @@
     </row>
     <row r="156" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A156" s="8" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4" t="s">
@@ -13691,10 +13614,10 @@
         <v>273</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>454</v>
+        <v>432</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4" t="s">
@@ -13710,10 +13633,10 @@
     </row>
     <row r="158" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A158" s="8" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="B158" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4" t="s">
@@ -13758,10 +13681,10 @@
         <v>309</v>
       </c>
       <c r="B161" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C161" t="s">
-        <v>470</v>
+        <v>539</v>
       </c>
       <c r="D161" s="4"/>
       <c r="E161" s="4" t="s">
@@ -13794,7 +13717,7 @@
         <v>318</v>
       </c>
       <c r="B163" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="D163" s="4"/>
       <c r="E163" s="4" t="s">
@@ -13824,7 +13747,7 @@
         <v>364</v>
       </c>
       <c r="B165" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="D165" s="10" t="s">
         <v>365</v>
@@ -13867,7 +13790,7 @@
     </row>
     <row r="168" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A168" s="28" t="s">
-        <v>459</v>
+        <v>437</v>
       </c>
       <c r="D168" s="4"/>
       <c r="E168" s="4" t="s">
@@ -13882,13 +13805,13 @@
     </row>
     <row r="169" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A169" s="28" t="s">
-        <v>532</v>
+        <v>503</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C169" t="s">
-        <v>522</v>
+        <v>495</v>
       </c>
       <c r="D169" s="4"/>
       <c r="E169" s="4" t="s">
@@ -13909,10 +13832,10 @@
         <v>391</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C170" t="s">
-        <v>517</v>
+        <v>490</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4" t="s">
@@ -13927,17 +13850,17 @@
     </row>
     <row r="171" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A171" s="28" t="s">
-        <v>515</v>
+        <v>488</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C171" t="s">
-        <v>516</v>
+        <v>489</v>
       </c>
       <c r="D171" s="4"/>
       <c r="E171" s="4" t="s">
-        <v>514</v>
+        <v>487</v>
       </c>
       <c r="F171" s="5" t="s">
         <v>9</v>
@@ -14005,7 +13928,7 @@
         <v>271</v>
       </c>
       <c r="B176" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>159</v>
@@ -14104,7 +14027,7 @@
         <v>312</v>
       </c>
       <c r="B183" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="D183" s="4"/>
       <c r="E183" s="4" t="s">
@@ -14125,7 +14048,7 @@
         <v>265</v>
       </c>
       <c r="B184" s="25" t="s">
-        <v>457</v>
+        <v>435</v>
       </c>
       <c r="C184" t="s">
         <v>340</v>
@@ -14207,7 +14130,7 @@
         <v>174</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>499</v>
+        <v>472</v>
       </c>
       <c r="G190" s="6" t="s">
         <v>7</v>
@@ -14219,7 +14142,7 @@
         <v>175</v>
       </c>
       <c r="F191" s="5" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="G191" s="6" t="s">
         <v>7</v>
@@ -14231,7 +14154,7 @@
         <v>176</v>
       </c>
       <c r="F192" s="5" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="G192" s="6" t="s">
         <v>7</v>
@@ -14251,7 +14174,7 @@
     </row>
     <row r="194" spans="1:8" s="15" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A194" s="31" t="s">
-        <v>461</v>
+        <v>439</v>
       </c>
       <c r="B194" s="27"/>
       <c r="D194" s="19" t="s">
@@ -14282,7 +14205,7 @@
         <v>180</v>
       </c>
       <c r="F196" s="5" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="G196" s="6" t="s">
         <v>7</v>
@@ -14348,7 +14271,7 @@
         <v>185</v>
       </c>
       <c r="F201" s="5" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="G201" s="6" t="s">
         <v>7</v>
@@ -14362,7 +14285,7 @@
         <v>185</v>
       </c>
       <c r="F202" s="5" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="G202" s="6" t="s">
         <v>7</v>
@@ -14374,7 +14297,7 @@
         <v>186</v>
       </c>
       <c r="F203" s="5" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="G203" s="6" t="s">
         <v>7</v>
@@ -14385,7 +14308,7 @@
         <v>331</v>
       </c>
       <c r="C204" t="s">
-        <v>542</v>
+        <v>512</v>
       </c>
       <c r="D204" s="4"/>
       <c r="E204" s="4" t="s">
@@ -14424,7 +14347,7 @@
     </row>
     <row r="207" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A207" s="28" t="s">
-        <v>549</v>
+        <v>519</v>
       </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4" t="s">
@@ -14439,13 +14362,13 @@
     </row>
     <row r="208" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A208" s="28" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="B208" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="D208" s="9" t="s">
         <v>260</v>
@@ -14462,13 +14385,13 @@
     </row>
     <row r="209" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A209" s="28" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B209" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D209" s="9"/>
       <c r="E209" s="4" t="s">
@@ -14483,17 +14406,17 @@
     </row>
     <row r="210" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A210" s="28" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="B210" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="D210" s="9"/>
       <c r="E210" s="4" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="F210" s="5" t="s">
         <v>52</v>
@@ -14507,10 +14430,10 @@
         <v>315</v>
       </c>
       <c r="B211" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="D211" s="4"/>
       <c r="E211" s="4" t="s">
@@ -14528,10 +14451,10 @@
         <v>316</v>
       </c>
       <c r="B212" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>541</v>
+        <v>511</v>
       </c>
       <c r="D212" s="4"/>
       <c r="E212" s="4" t="s">
@@ -14572,13 +14495,13 @@
     </row>
     <row r="215" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A215" s="28" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B215" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="D215" s="4"/>
       <c r="E215" s="4" t="s">
@@ -14593,7 +14516,7 @@
     </row>
     <row r="216" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A216" s="30" t="s">
-        <v>462</v>
+        <v>440</v>
       </c>
       <c r="D216" s="4"/>
       <c r="E216" s="4" t="s">
@@ -14624,7 +14547,7 @@
         <v>199</v>
       </c>
       <c r="F218" s="5" t="s">
-        <v>496</v>
+        <v>469</v>
       </c>
       <c r="G218" s="6" t="s">
         <v>7</v>
@@ -14644,13 +14567,13 @@
     </row>
     <row r="220" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A220" s="28" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="B220" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="D220" s="4"/>
       <c r="E220" s="4" t="s">
@@ -14668,7 +14591,7 @@
         <v>281</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>550</v>
+        <v>520</v>
       </c>
       <c r="D221" s="4"/>
       <c r="E221" s="4" t="s">
@@ -14686,7 +14609,7 @@
         <v>280</v>
       </c>
       <c r="B222" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C222" t="s">
         <v>342</v>
@@ -14728,17 +14651,17 @@
     </row>
     <row r="225" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A225" s="28" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="B225" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="D225" s="4"/>
       <c r="E225" s="4" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="F225" s="5" t="s">
         <v>52</v>
@@ -14749,17 +14672,17 @@
     </row>
     <row r="226" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A226" s="28" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="B226" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="D226" s="4"/>
       <c r="E226" s="4" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="F226" s="5" t="s">
         <v>52</v>
@@ -14773,10 +14696,10 @@
         <v>278</v>
       </c>
       <c r="B227" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="D227" s="10" t="s">
         <v>279</v>
@@ -14796,17 +14719,17 @@
     </row>
     <row r="228" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A228" s="28" t="s">
-        <v>501</v>
+        <v>474</v>
       </c>
       <c r="B228" s="25" t="s">
-        <v>458</v>
+        <v>436</v>
       </c>
       <c r="C228" t="s">
-        <v>502</v>
+        <v>475</v>
       </c>
       <c r="D228" s="10"/>
       <c r="E228" s="4" t="s">
-        <v>502</v>
+        <v>475</v>
       </c>
       <c r="F228" s="5" t="s">
         <v>52</v>
@@ -14862,7 +14785,7 @@
         <v>210</v>
       </c>
       <c r="F232" s="5" t="s">
-        <v>496</v>
+        <v>469</v>
       </c>
       <c r="G232" s="6" t="s">
         <v>7</v>
@@ -14902,17 +14825,17 @@
         <v>297</v>
       </c>
       <c r="B235" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C235" t="s">
-        <v>466</v>
+        <v>444</v>
       </c>
       <c r="D235" s="4"/>
       <c r="E235" s="4" t="s">
         <v>213</v>
       </c>
       <c r="F235" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G235" s="6" t="s">
         <v>7</v>
@@ -14925,7 +14848,7 @@
         <v>214</v>
       </c>
       <c r="F236" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G236" s="6" t="s">
         <v>7</v>
@@ -14938,7 +14861,7 @@
         <v>215</v>
       </c>
       <c r="F237" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G237" s="6" t="s">
         <v>7</v>
@@ -14947,14 +14870,14 @@
     </row>
     <row r="238" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A238" s="28" t="s">
-        <v>463</v>
+        <v>441</v>
       </c>
       <c r="D238" s="4"/>
       <c r="E238" s="4" t="s">
         <v>216</v>
       </c>
       <c r="F238" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G238" s="6" t="s">
         <v>7</v>
@@ -14963,14 +14886,14 @@
     </row>
     <row r="239" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A239" s="28" t="s">
-        <v>464</v>
+        <v>442</v>
       </c>
       <c r="D239" s="4"/>
       <c r="E239" s="4" t="s">
         <v>217</v>
       </c>
       <c r="F239" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G239" s="6" t="s">
         <v>7</v>
@@ -14983,7 +14906,7 @@
         <v>218</v>
       </c>
       <c r="F240" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G240" s="6" t="s">
         <v>7</v>
@@ -14996,7 +14919,7 @@
         <v>219</v>
       </c>
       <c r="F241" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G241" s="6" t="s">
         <v>7</v>
@@ -15005,20 +14928,20 @@
     </row>
     <row r="242" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A242" s="28" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="B242" s="25" t="s">
-        <v>456</v>
+        <v>434</v>
       </c>
       <c r="C242" t="s">
-        <v>504</v>
+        <v>477</v>
       </c>
       <c r="D242" s="4"/>
       <c r="E242" s="4" t="s">
         <v>220</v>
       </c>
       <c r="F242" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G242" s="6" t="s">
         <v>7</v>
@@ -15031,7 +14954,7 @@
         <v>221</v>
       </c>
       <c r="F243" s="5" t="s">
-        <v>495</v>
+        <v>468</v>
       </c>
       <c r="G243" s="6" t="s">
         <v>7</v>
@@ -15123,77 +15046,77 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D211:XFD211 D127:XFD127 A194:C194 F194:XFD194 A195:XFD208 A123:A126 C123:XFD126 A128:A137 C128:XFD137 A159:XFD160 A162:XFD162 A161 C161:XFD161 A163 C163:XFD163 A164:XFD168 A169 A185:XFD193 A183:A184 C183:XFD184 A209:A210 C209:XFD210 A236:XFD241 A235 C235:XFD235 A157:A158 C157:XFD158 A138:XFD156 A229:XFD234 A228:B228 D228:XFD228 A243:XFD1048576 A242 C242:XFD242 A170:XFD182 C169:XFD169 A1:XFD107 A212:XFD227 A109:XFD122">
-    <cfRule type="expression" dxfId="16" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C211">
-    <cfRule type="expression" dxfId="15" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B123:B137">
-    <cfRule type="expression" dxfId="14" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B157">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B161">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B163">
-    <cfRule type="expression" dxfId="11" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B169">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B184">
-    <cfRule type="expression" dxfId="9" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B183">
-    <cfRule type="expression" dxfId="8" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209:B211">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B235">
-    <cfRule type="expression" dxfId="6" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B158">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B242">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B108">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108:XFD108">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
started integration of Livestock functionality
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D07E64B9-DDBF-4BD7-A3F7-859CEF34641A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B8A451-1DB4-4831-B16A-8CE6A3158C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="540" windowWidth="27300" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="2205" windowWidth="27300" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -2496,9 +2496,6 @@
     <t>NH4-N loss adjusted</t>
   </si>
   <si>
-    <t>NH4-N total loss</t>
-  </si>
-  <si>
     <t>NH4-N or urea-N in applied manure</t>
   </si>
   <si>
@@ -2521,6 +2518,9 @@
   </si>
   <si>
     <t>Loss adjustment factor for NH4-N</t>
+  </si>
+  <si>
+    <t>Sum of all NH4-N losses</t>
   </si>
 </sst>
 </file>
@@ -10833,15 +10833,15 @@
   <dimension ref="A1:H249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C103" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21.140625" style="28" customWidth="1"/>
     <col min="2" max="2" width="15" style="25" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="120" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
@@ -11840,7 +11840,7 @@
         <v>434</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
@@ -12711,8 +12711,8 @@
       <c r="B110" s="25" t="s">
         <v>434</v>
       </c>
-      <c r="C110" t="s">
-        <v>547</v>
+      <c r="C110" s="4" t="s">
+        <v>555</v>
       </c>
       <c r="D110" s="10"/>
       <c r="E110" t="s">
@@ -12733,7 +12733,7 @@
         <v>434</v>
       </c>
       <c r="C111" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D111" s="10" t="s">
         <v>507</v>
@@ -12774,7 +12774,7 @@
         <v>434</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>292</v>
@@ -12797,7 +12797,7 @@
         <v>434</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4" t="s">
@@ -12839,7 +12839,7 @@
         <v>434</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4" t="s">
@@ -12860,7 +12860,7 @@
         <v>434</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4" t="s">
@@ -12881,7 +12881,7 @@
         <v>434</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
@@ -12905,7 +12905,7 @@
         <v>434</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4" t="s">
@@ -15046,77 +15046,77 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D211:XFD211 D127:XFD127 A194:C194 F194:XFD194 A195:XFD208 A123:A126 C123:XFD126 A128:A137 C128:XFD137 A159:XFD160 A162:XFD162 A161 C161:XFD161 A163 C163:XFD163 A164:XFD168 A169 A185:XFD193 A183:A184 C183:XFD184 A209:A210 C209:XFD210 A236:XFD241 A235 C235:XFD235 A157:A158 C157:XFD158 A138:XFD156 A229:XFD234 A228:B228 D228:XFD228 A243:XFD1048576 A242 C242:XFD242 A170:XFD182 C169:XFD169 A1:XFD107 A212:XFD227 A109:XFD122">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="0" priority="15">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C211">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B123:B137">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="13" priority="13">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B157">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="12" priority="12">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B161">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B163">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="10" priority="10">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B169">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B184">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B183">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209:B211">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B235">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B158">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B242">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B108">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108:XFD108">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
second try at adding Livestck
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B8A451-1DB4-4831-B16A-8CE6A3158C50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A232444D-CDD0-41C0-80CC-CA99A78A8621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2205" windowWidth="27300" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="31455" yWindow="75" windowWidth="27300" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -1577,9 +1577,6 @@
     <t>no3_start</t>
   </si>
   <si>
-    <t>prop_iom_in_ow</t>
-  </si>
-  <si>
     <t>nh4_immob</t>
   </si>
   <si>
@@ -2521,6 +2518,9 @@
   </si>
   <si>
     <t>Sum of all NH4-N losses</t>
+  </si>
+  <si>
+    <t>prop_iom_ow</t>
   </si>
 </sst>
 </file>
@@ -10830,11 +10830,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C110" sqref="C110"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -10855,10 +10856,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -10893,7 +10894,7 @@
         <v>277</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -10924,7 +10925,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>7</v>
@@ -10936,7 +10937,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>7</v>
@@ -10944,20 +10945,20 @@
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="28" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C7" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>7</v>
@@ -10965,17 +10966,17 @@
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>7</v>
@@ -10983,17 +10984,17 @@
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>7</v>
@@ -11001,17 +11002,17 @@
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="28" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>7</v>
@@ -11022,17 +11023,17 @@
         <v>268</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>7</v>
@@ -11040,17 +11041,17 @@
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>7</v>
@@ -11058,22 +11059,22 @@
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C13" t="s">
+        <v>373</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>371</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C13" t="s">
-        <v>374</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="E13" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>373</v>
-      </c>
       <c r="F13" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>7</v>
@@ -11081,22 +11082,22 @@
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="28" t="s">
+        <v>374</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C14" t="s">
         <v>375</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" s="7" t="s">
+        <v>377</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>376</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>378</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>377</v>
-      </c>
       <c r="F14" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>7</v>
@@ -11104,22 +11105,22 @@
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="28" t="s">
+        <v>380</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C15" t="s">
+        <v>378</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>381</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="E15" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>380</v>
-      </c>
       <c r="F15" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>7</v>
@@ -11127,22 +11128,22 @@
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="28" t="s">
+        <v>382</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C16" t="s">
         <v>383</v>
       </c>
-      <c r="B16" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="D16" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>372</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>385</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>7</v>
@@ -11153,7 +11154,7 @@
         <v>267</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
@@ -11163,7 +11164,7 @@
         <v>19</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>7</v>
@@ -11175,7 +11176,7 @@
         <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>7</v>
@@ -11183,17 +11184,17 @@
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>7</v>
@@ -11201,17 +11202,17 @@
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="28" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>7</v>
@@ -11224,7 +11225,7 @@
         <v>21</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G21" s="34" t="s">
         <v>7</v>
@@ -11237,7 +11238,7 @@
         <v>22</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>7</v>
@@ -11249,7 +11250,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>7</v>
@@ -11261,7 +11262,7 @@
         <v>24</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>7</v>
@@ -11272,17 +11273,17 @@
         <v>25</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>7</v>
@@ -11293,17 +11294,17 @@
         <v>27</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4" t="s">
         <v>28</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>7</v>
@@ -11314,17 +11315,17 @@
         <v>29</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>7</v>
@@ -11332,20 +11333,20 @@
     </row>
     <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="28" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>7</v>
@@ -11357,7 +11358,7 @@
         <v>32</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>7</v>
@@ -11371,7 +11372,7 @@
         <v>34</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>7</v>
@@ -11385,7 +11386,7 @@
         <v>35</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>7</v>
@@ -11397,7 +11398,7 @@
         <v>36</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>7</v>
@@ -11409,7 +11410,7 @@
         <v>37</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>7</v>
@@ -11417,20 +11418,20 @@
     </row>
     <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="28" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C34" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>7</v>
@@ -11438,20 +11439,20 @@
     </row>
     <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="28" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C35" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4" t="s">
         <v>39</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>7</v>
@@ -11462,17 +11463,17 @@
         <v>266</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>7</v>
@@ -11486,7 +11487,7 @@
         <v>41</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>7</v>
@@ -11500,7 +11501,7 @@
         <v>42</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>7</v>
@@ -11512,7 +11513,7 @@
         <v>43</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>7</v>
@@ -11520,20 +11521,20 @@
     </row>
     <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="28" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>7</v>
@@ -11541,20 +11542,20 @@
     </row>
     <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="28" t="s">
+        <v>455</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C41" t="s">
         <v>456</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C41" t="s">
-        <v>457</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>7</v>
@@ -11562,20 +11563,20 @@
     </row>
     <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="28" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C42" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>7</v>
@@ -11583,14 +11584,14 @@
     </row>
     <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B43" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>7</v>
@@ -11598,20 +11599,20 @@
     </row>
     <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>7</v>
@@ -11619,20 +11620,20 @@
     </row>
     <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="28" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>7</v>
@@ -11640,20 +11641,20 @@
     </row>
     <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="28" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>7</v>
@@ -11661,20 +11662,20 @@
     </row>
     <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="28" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>7</v>
@@ -11682,20 +11683,20 @@
     </row>
     <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="28" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>7</v>
@@ -11703,10 +11704,10 @@
     </row>
     <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="28" t="s">
+        <v>523</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>524</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>525</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -11718,7 +11719,7 @@
         <v>46</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>7</v>
@@ -11726,7 +11727,7 @@
     </row>
     <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="28" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>47</v>
@@ -11736,7 +11737,7 @@
         <v>47</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>7</v>
@@ -11756,7 +11757,7 @@
     </row>
     <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="28" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>50</v>
@@ -11834,13 +11835,13 @@
     </row>
     <row r="59" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
@@ -11855,13 +11856,13 @@
     </row>
     <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A60" s="28" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
@@ -11876,10 +11877,10 @@
     </row>
     <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D61" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>362</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>363</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>9</v>
@@ -11904,10 +11905,10 @@
     </row>
     <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="28" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>61</v>
@@ -11925,7 +11926,7 @@
     </row>
     <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
@@ -11976,13 +11977,13 @@
     </row>
     <row r="68" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A68" s="28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
@@ -11995,18 +11996,18 @@
         <v>7</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A69" s="32" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
@@ -12019,18 +12020,18 @@
         <v>7</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
@@ -12043,7 +12044,7 @@
         <v>7</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -12052,7 +12053,7 @@
         <v>71</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G71" s="6" t="s">
         <v>7</v>
@@ -12064,7 +12065,7 @@
         <v>72</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>7</v>
@@ -12078,7 +12079,7 @@
         <v>73</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G73" s="6" t="s">
         <v>7</v>
@@ -12092,7 +12093,7 @@
         <v>74</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G74" s="6" t="s">
         <v>7</v>
@@ -12106,7 +12107,7 @@
         <v>75</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>7</v>
@@ -12120,7 +12121,7 @@
         <v>76</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G76" s="6" t="s">
         <v>7</v>
@@ -12134,7 +12135,7 @@
         <v>77</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>7</v>
@@ -12148,7 +12149,7 @@
         <v>78</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>7</v>
@@ -12160,7 +12161,7 @@
         <v>79</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>7</v>
@@ -12174,7 +12175,7 @@
         <v>80</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>7</v>
@@ -12188,7 +12189,7 @@
         <v>81</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>7</v>
@@ -12287,14 +12288,14 @@
         <v>282</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
         <v>89</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>7</v>
@@ -12302,20 +12303,20 @@
     </row>
     <row r="90" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A90" s="28" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="35" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>7</v>
@@ -12323,20 +12324,20 @@
     </row>
     <row r="91" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A91" s="28" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>7</v>
@@ -12344,17 +12345,17 @@
     </row>
     <row r="92" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A92" s="28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
         <v>90</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G92" s="6" t="s">
         <v>7</v>
@@ -12362,98 +12363,98 @@
     </row>
     <row r="93" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A93" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
         <v>91</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G93" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="28" t="s">
+        <v>495</v>
+      </c>
+      <c r="B94" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>496</v>
-      </c>
-      <c r="B94" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>497</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G94" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="28" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C95" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G95" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A96" s="28" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C96" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G96" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -12464,7 +12465,7 @@
         <v>94</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>7</v>
@@ -12478,7 +12479,7 @@
         <v>95</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G98" s="6" t="s">
         <v>7</v>
@@ -12492,7 +12493,7 @@
         <v>96</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G99" s="6" t="s">
         <v>7</v>
@@ -12504,7 +12505,7 @@
         <v>97</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>7</v>
@@ -12512,20 +12513,20 @@
     </row>
     <row r="101" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A101" s="28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C101" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>7</v>
@@ -12533,20 +12534,20 @@
     </row>
     <row r="102" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A102" s="28" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C102" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G102" s="6" t="s">
         <v>7</v>
@@ -12554,20 +12555,20 @@
     </row>
     <row r="103" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A103" s="28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
         <v>98</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G103" s="6" t="s">
         <v>7</v>
@@ -12578,17 +12579,17 @@
         <v>284</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G104" s="6" t="s">
         <v>7</v>
@@ -12596,20 +12597,20 @@
     </row>
     <row r="105" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A105" s="28" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C105" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
         <v>100</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G105" s="6" t="s">
         <v>7</v>
@@ -12617,20 +12618,20 @@
     </row>
     <row r="106" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A106" s="28" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4" t="s">
         <v>101</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G106" s="6" t="s">
         <v>7</v>
@@ -12638,22 +12639,22 @@
     </row>
     <row r="107" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A107" s="28" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D107" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>102</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G107" s="6" t="s">
         <v>7</v>
@@ -12661,44 +12662,44 @@
     </row>
     <row r="108" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A108" s="28" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C108" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G108" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H108" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A109" s="28" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C109" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D109" s="10"/>
       <c r="E109" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G109" s="6" t="s">
         <v>7</v>
@@ -12706,20 +12707,20 @@
     </row>
     <row r="110" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A110" s="28" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B110" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D110" s="10"/>
       <c r="E110" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G110" s="6" t="s">
         <v>7</v>
@@ -12727,22 +12728,22 @@
     </row>
     <row r="111" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A111" s="28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C111" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E111" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G111" s="6" t="s">
         <v>7</v>
@@ -12750,17 +12751,17 @@
     </row>
     <row r="112" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A112" s="28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
         <v>103</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G112" s="6" t="s">
         <v>7</v>
@@ -12768,22 +12769,22 @@
     </row>
     <row r="113" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A113" s="28" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B113" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D113" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>104</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G113" s="6" t="s">
         <v>7</v>
@@ -12791,20 +12792,20 @@
     </row>
     <row r="114" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A114" s="28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4" t="s">
         <v>105</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G114" s="6" t="s">
         <v>7</v>
@@ -12812,20 +12813,20 @@
     </row>
     <row r="115" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A115" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="B115" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="C115" s="4" t="s">
         <v>521</v>
-      </c>
-      <c r="B115" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>522</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G115" s="6" t="s">
         <v>7</v>
@@ -12833,20 +12834,20 @@
     </row>
     <row r="116" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A116" s="28" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B116" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G116" s="6" t="s">
         <v>7</v>
@@ -12854,20 +12855,20 @@
     </row>
     <row r="117" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A117" s="28" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B117" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G117" s="6" t="s">
         <v>7</v>
@@ -12875,68 +12876,68 @@
     </row>
     <row r="118" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A118" s="28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B118" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
         <v>106</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G118" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H118" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A119" s="28" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B119" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G119" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H119" s="13" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A120" s="28" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B120" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C120" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G120" s="6" t="s">
         <v>7</v>
@@ -12944,20 +12945,20 @@
     </row>
     <row r="121" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A121" s="28" t="s">
+        <v>504</v>
+      </c>
+      <c r="B121" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="C121" s="4" t="s">
         <v>505</v>
-      </c>
-      <c r="B121" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>506</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G121" s="6" t="s">
         <v>7</v>
@@ -12965,20 +12966,20 @@
     </row>
     <row r="122" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A122" s="28" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B122" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4" t="s">
         <v>108</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G122" s="6" t="s">
         <v>7</v>
@@ -12989,17 +12990,17 @@
         <v>283</v>
       </c>
       <c r="B123" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4" t="s">
         <v>109</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G123" s="6" t="s">
         <v>7</v>
@@ -13007,20 +13008,20 @@
     </row>
     <row r="124" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A124" s="28" t="s">
+        <v>393</v>
+      </c>
+      <c r="B124" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="C124" t="s">
         <v>394</v>
-      </c>
-      <c r="B124" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C124" t="s">
-        <v>395</v>
       </c>
       <c r="D124" s="4"/>
       <c r="E124" s="4" t="s">
         <v>110</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G124" s="6" t="s">
         <v>7</v>
@@ -13028,20 +13029,20 @@
     </row>
     <row r="125" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A125" s="28" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B125" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G125" s="6" t="s">
         <v>7</v>
@@ -13052,10 +13053,10 @@
         <v>275</v>
       </c>
       <c r="B126" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>248</v>
@@ -13064,7 +13065,7 @@
         <v>112</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G126" s="6" t="s">
         <v>7</v>
@@ -13072,26 +13073,26 @@
     </row>
     <row r="127" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A127" s="28" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B127" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C127" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4" t="s">
         <v>113</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G127" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H127" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -13099,10 +13100,10 @@
         <v>276</v>
       </c>
       <c r="B128" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>249</v>
@@ -13111,7 +13112,7 @@
         <v>250</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G128" s="6" t="s">
         <v>7</v>
@@ -13119,20 +13120,20 @@
     </row>
     <row r="129" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A129" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="B129" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="C129" s="4" t="s">
         <v>392</v>
-      </c>
-      <c r="B129" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C129" s="4" t="s">
-        <v>393</v>
       </c>
       <c r="D129" s="9"/>
       <c r="E129" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G129" s="6" t="s">
         <v>7</v>
@@ -13140,20 +13141,20 @@
     </row>
     <row r="130" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A130" s="28" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B130" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4" t="s">
         <v>114</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G130" s="6" t="s">
         <v>7</v>
@@ -13161,20 +13162,20 @@
     </row>
     <row r="131" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A131" s="28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B131" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D131" s="4"/>
       <c r="E131" s="4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G131" s="6" t="s">
         <v>7</v>
@@ -13182,17 +13183,17 @@
     </row>
     <row r="132" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A132" s="28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B132" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4" t="s">
         <v>115</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G132" s="6" t="s">
         <v>7</v>
@@ -13203,17 +13204,17 @@
         <v>274</v>
       </c>
       <c r="B133" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4" t="s">
         <v>116</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G133" s="6" t="s">
         <v>7</v>
@@ -13224,17 +13225,17 @@
         <v>286</v>
       </c>
       <c r="B134" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G134" s="6" t="s">
         <v>7</v>
@@ -13242,20 +13243,20 @@
     </row>
     <row r="135" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A135" s="28" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B135" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G135" s="6" t="s">
         <v>7</v>
@@ -13266,17 +13267,17 @@
         <v>285</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D136" s="4"/>
       <c r="E136" s="4" t="s">
         <v>118</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G136" s="6" t="s">
         <v>7</v>
@@ -13284,10 +13285,10 @@
     </row>
     <row r="137" spans="1:8" s="8" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A137" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B137" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>119</v>
@@ -13297,7 +13298,7 @@
         <v>119</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G137" s="6" t="s">
         <v>7</v>
@@ -13306,10 +13307,10 @@
     </row>
     <row r="138" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A138" s="28" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B138" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4" t="s">
@@ -13324,10 +13325,10 @@
     </row>
     <row r="139" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A139" s="28" t="s">
+        <v>459</v>
+      </c>
+      <c r="C139" s="4" t="s">
         <v>460</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>461</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4" t="s">
@@ -13356,10 +13357,10 @@
     </row>
     <row r="141" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A141" s="28" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4" t="s">
@@ -13388,10 +13389,10 @@
     </row>
     <row r="143" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A143" s="28" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D143" s="4"/>
       <c r="E143" s="4" t="s">
@@ -13459,10 +13460,10 @@
     </row>
     <row r="148" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A148" s="28" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B148" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4" t="s">
@@ -13478,10 +13479,10 @@
     </row>
     <row r="149" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A149" s="28" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B149" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
@@ -13497,10 +13498,10 @@
     </row>
     <row r="150" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A150" s="28" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B150" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4" t="s">
@@ -13542,10 +13543,10 @@
     </row>
     <row r="153" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A153" s="28" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B153" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4" t="s">
@@ -13561,10 +13562,10 @@
     </row>
     <row r="154" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A154" s="28" t="s">
-        <v>287</v>
+        <v>555</v>
       </c>
       <c r="B154" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4" t="s">
@@ -13595,7 +13596,7 @@
     </row>
     <row r="156" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A156" s="8" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4" t="s">
@@ -13614,10 +13615,10 @@
         <v>273</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4" t="s">
@@ -13633,10 +13634,10 @@
     </row>
     <row r="158" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A158" s="8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B158" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4" t="s">
@@ -13678,13 +13679,13 @@
     </row>
     <row r="161" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A161" s="28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B161" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C161" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D161" s="4"/>
       <c r="E161" s="4" t="s">
@@ -13697,7 +13698,7 @@
         <v>7</v>
       </c>
       <c r="H161" s="13" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="162" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -13714,10 +13715,10 @@
     </row>
     <row r="163" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A163" s="28" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B163" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D163" s="4"/>
       <c r="E163" s="4" t="s">
@@ -13744,16 +13745,16 @@
     </row>
     <row r="165" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A165" s="28" t="s">
+        <v>363</v>
+      </c>
+      <c r="B165" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="D165" s="10" t="s">
         <v>364</v>
       </c>
-      <c r="B165" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="D165" s="10" t="s">
+      <c r="E165" s="4" t="s">
         <v>365</v>
-      </c>
-      <c r="E165" s="4" t="s">
-        <v>366</v>
       </c>
       <c r="F165" s="5" t="s">
         <v>9</v>
@@ -13790,7 +13791,7 @@
     </row>
     <row r="168" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A168" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D168" s="4"/>
       <c r="E168" s="4" t="s">
@@ -13805,13 +13806,13 @@
     </row>
     <row r="169" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A169" s="28" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C169" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D169" s="4"/>
       <c r="E169" s="4" t="s">
@@ -13824,18 +13825,18 @@
         <v>7</v>
       </c>
       <c r="H169" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="170" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A170" s="28" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C170" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4" t="s">
@@ -13850,17 +13851,17 @@
     </row>
     <row r="171" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A171" s="28" t="s">
+        <v>487</v>
+      </c>
+      <c r="B171" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C171" t="s">
         <v>488</v>
-      </c>
-      <c r="B171" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C171" t="s">
-        <v>489</v>
       </c>
       <c r="D171" s="4"/>
       <c r="E171" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F171" s="5" t="s">
         <v>9</v>
@@ -13928,7 +13929,7 @@
         <v>271</v>
       </c>
       <c r="B176" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>159</v>
@@ -14024,10 +14025,10 @@
     </row>
     <row r="183" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A183" s="28" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B183" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D183" s="4"/>
       <c r="E183" s="4" t="s">
@@ -14040,7 +14041,7 @@
         <v>7</v>
       </c>
       <c r="H183" s="13" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="184" spans="1:8" ht="20.100000000000001" customHeight="1">
@@ -14048,10 +14049,10 @@
         <v>265</v>
       </c>
       <c r="B184" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C184" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D184" s="4"/>
       <c r="E184" s="4" t="s">
@@ -14130,7 +14131,7 @@
         <v>174</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G190" s="6" t="s">
         <v>7</v>
@@ -14142,7 +14143,7 @@
         <v>175</v>
       </c>
       <c r="F191" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G191" s="6" t="s">
         <v>7</v>
@@ -14154,7 +14155,7 @@
         <v>176</v>
       </c>
       <c r="F192" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G192" s="6" t="s">
         <v>7</v>
@@ -14174,14 +14175,14 @@
     </row>
     <row r="194" spans="1:8" s="15" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A194" s="31" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B194" s="27"/>
       <c r="D194" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E194" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F194" s="16"/>
       <c r="G194" s="17"/>
@@ -14205,7 +14206,7 @@
         <v>180</v>
       </c>
       <c r="F196" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G196" s="6" t="s">
         <v>7</v>
@@ -14271,7 +14272,7 @@
         <v>185</v>
       </c>
       <c r="F201" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G201" s="6" t="s">
         <v>7</v>
@@ -14285,7 +14286,7 @@
         <v>185</v>
       </c>
       <c r="F202" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G202" s="6" t="s">
         <v>7</v>
@@ -14297,7 +14298,7 @@
         <v>186</v>
       </c>
       <c r="F203" s="5" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G203" s="6" t="s">
         <v>7</v>
@@ -14305,10 +14306,10 @@
     </row>
     <row r="204" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A204" s="28" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C204" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D204" s="4"/>
       <c r="E204" s="4" t="s">
@@ -14347,7 +14348,7 @@
     </row>
     <row r="207" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A207" s="28" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4" t="s">
@@ -14362,13 +14363,13 @@
     </row>
     <row r="208" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A208" s="28" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B208" s="25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D208" s="9" t="s">
         <v>260</v>
@@ -14385,13 +14386,13 @@
     </row>
     <row r="209" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A209" s="28" t="s">
+        <v>426</v>
+      </c>
+      <c r="B209" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="C209" s="4" t="s">
         <v>427</v>
-      </c>
-      <c r="B209" s="25" t="s">
-        <v>436</v>
-      </c>
-      <c r="C209" s="4" t="s">
-        <v>428</v>
       </c>
       <c r="D209" s="9"/>
       <c r="E209" s="4" t="s">
@@ -14406,17 +14407,17 @@
     </row>
     <row r="210" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A210" s="28" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B210" s="25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D210" s="9"/>
       <c r="E210" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F210" s="5" t="s">
         <v>52</v>
@@ -14427,13 +14428,13 @@
     </row>
     <row r="211" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A211" s="29" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B211" s="25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D211" s="4"/>
       <c r="E211" s="4" t="s">
@@ -14448,13 +14449,13 @@
     </row>
     <row r="212" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A212" s="28" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B212" s="25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D212" s="4"/>
       <c r="E212" s="4" t="s">
@@ -14495,13 +14496,13 @@
     </row>
     <row r="215" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A215" s="28" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B215" s="25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C215" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D215" s="4"/>
       <c r="E215" s="4" t="s">
@@ -14516,7 +14517,7 @@
     </row>
     <row r="216" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A216" s="30" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D216" s="4"/>
       <c r="E216" s="4" t="s">
@@ -14547,7 +14548,7 @@
         <v>199</v>
       </c>
       <c r="F218" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G218" s="6" t="s">
         <v>7</v>
@@ -14567,13 +14568,13 @@
     </row>
     <row r="220" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A220" s="28" t="s">
+        <v>418</v>
+      </c>
+      <c r="B220" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="C220" s="4" t="s">
         <v>419</v>
-      </c>
-      <c r="B220" s="25" t="s">
-        <v>436</v>
-      </c>
-      <c r="C220" s="4" t="s">
-        <v>420</v>
       </c>
       <c r="D220" s="4"/>
       <c r="E220" s="4" t="s">
@@ -14591,7 +14592,7 @@
         <v>281</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D221" s="4"/>
       <c r="E221" s="4" t="s">
@@ -14609,14 +14610,14 @@
         <v>280</v>
       </c>
       <c r="B222" s="25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C222" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D222" s="4"/>
       <c r="E222" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F222" s="5" t="s">
         <v>52</v>
@@ -14651,17 +14652,17 @@
     </row>
     <row r="225" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A225" s="28" t="s">
+        <v>421</v>
+      </c>
+      <c r="B225" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="C225" s="4" t="s">
         <v>422</v>
-      </c>
-      <c r="B225" s="25" t="s">
-        <v>436</v>
-      </c>
-      <c r="C225" s="4" t="s">
-        <v>423</v>
       </c>
       <c r="D225" s="4"/>
       <c r="E225" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F225" s="5" t="s">
         <v>52</v>
@@ -14672,17 +14673,17 @@
     </row>
     <row r="226" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A226" s="28" t="s">
+        <v>423</v>
+      </c>
+      <c r="B226" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="C226" s="4" t="s">
         <v>424</v>
-      </c>
-      <c r="B226" s="25" t="s">
-        <v>436</v>
-      </c>
-      <c r="C226" s="4" t="s">
-        <v>425</v>
       </c>
       <c r="D226" s="4"/>
       <c r="E226" s="4" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F226" s="5" t="s">
         <v>52</v>
@@ -14696,10 +14697,10 @@
         <v>278</v>
       </c>
       <c r="B227" s="25" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C227" s="4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D227" s="10" t="s">
         <v>279</v>
@@ -14714,22 +14715,22 @@
         <v>7</v>
       </c>
       <c r="H227" s="13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="228" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A228" s="28" t="s">
+        <v>473</v>
+      </c>
+      <c r="B228" s="25" t="s">
+        <v>435</v>
+      </c>
+      <c r="C228" t="s">
         <v>474</v>
-      </c>
-      <c r="B228" s="25" t="s">
-        <v>436</v>
-      </c>
-      <c r="C228" t="s">
-        <v>475</v>
       </c>
       <c r="D228" s="10"/>
       <c r="E228" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F228" s="5" t="s">
         <v>52</v>
@@ -14785,7 +14786,7 @@
         <v>210</v>
       </c>
       <c r="F232" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G232" s="6" t="s">
         <v>7</v>
@@ -14822,20 +14823,20 @@
     </row>
     <row r="235" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A235" s="28" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B235" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C235" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D235" s="4"/>
       <c r="E235" s="4" t="s">
         <v>213</v>
       </c>
       <c r="F235" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G235" s="6" t="s">
         <v>7</v>
@@ -14848,7 +14849,7 @@
         <v>214</v>
       </c>
       <c r="F236" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G236" s="6" t="s">
         <v>7</v>
@@ -14861,7 +14862,7 @@
         <v>215</v>
       </c>
       <c r="F237" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G237" s="6" t="s">
         <v>7</v>
@@ -14870,14 +14871,14 @@
     </row>
     <row r="238" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A238" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D238" s="4"/>
       <c r="E238" s="4" t="s">
         <v>216</v>
       </c>
       <c r="F238" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G238" s="6" t="s">
         <v>7</v>
@@ -14886,14 +14887,14 @@
     </row>
     <row r="239" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A239" s="28" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D239" s="4"/>
       <c r="E239" s="4" t="s">
         <v>217</v>
       </c>
       <c r="F239" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G239" s="6" t="s">
         <v>7</v>
@@ -14906,7 +14907,7 @@
         <v>218</v>
       </c>
       <c r="F240" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G240" s="6" t="s">
         <v>7</v>
@@ -14919,7 +14920,7 @@
         <v>219</v>
       </c>
       <c r="F241" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G241" s="6" t="s">
         <v>7</v>
@@ -14928,20 +14929,20 @@
     </row>
     <row r="242" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A242" s="28" t="s">
+        <v>475</v>
+      </c>
+      <c r="B242" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="C242" t="s">
         <v>476</v>
-      </c>
-      <c r="B242" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C242" t="s">
-        <v>477</v>
       </c>
       <c r="D242" s="4"/>
       <c r="E242" s="4" t="s">
         <v>220</v>
       </c>
       <c r="F242" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G242" s="6" t="s">
         <v>7</v>
@@ -14954,7 +14955,7 @@
         <v>221</v>
       </c>
       <c r="F243" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G243" s="6" t="s">
         <v>7</v>
@@ -15046,77 +15047,77 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D211:XFD211 D127:XFD127 A194:C194 F194:XFD194 A195:XFD208 A123:A126 C123:XFD126 A128:A137 C128:XFD137 A159:XFD160 A162:XFD162 A161 C161:XFD161 A163 C163:XFD163 A164:XFD168 A169 A185:XFD193 A183:A184 C183:XFD184 A209:A210 C209:XFD210 A236:XFD241 A235 C235:XFD235 A157:A158 C157:XFD158 A138:XFD156 A229:XFD234 A228:B228 D228:XFD228 A243:XFD1048576 A242 C242:XFD242 A170:XFD182 C169:XFD169 A1:XFD107 A212:XFD227 A109:XFD122">
-    <cfRule type="expression" dxfId="0" priority="15">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C211">
-    <cfRule type="expression" dxfId="14" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B123:B137">
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B157">
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B161">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B163">
-    <cfRule type="expression" dxfId="10" priority="10">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B169">
-    <cfRule type="expression" dxfId="9" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B184">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B183">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209:B211">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B235">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B158">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B242">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B108">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108:XFD108">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
improvements to nitrogen initialisation
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A232444D-CDD0-41C0-80CC-CA99A78A8621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD81F5C-79E9-42BE-A467-36F9674A5453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="31455" yWindow="75" windowWidth="27300" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30135" yWindow="690" windowWidth="27300" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -2093,9 +2093,6 @@
     <t>nh4_total_loss</t>
   </si>
   <si>
-    <t>NH4 total loss ???</t>
-  </si>
-  <si>
     <t>irrig</t>
   </si>
   <si>
@@ -2521,6 +2518,9 @@
   </si>
   <si>
     <t>prop_iom_ow</t>
+  </si>
+  <si>
+    <t>Ammonium total losses</t>
   </si>
 </sst>
 </file>
@@ -10834,8 +10834,8 @@
   <dimension ref="A1:H249"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C155" sqref="C155"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E123" sqref="E123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -10856,7 +10856,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>337</v>
@@ -10894,7 +10894,7 @@
         <v>277</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -10925,7 +10925,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>7</v>
@@ -10937,7 +10937,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>7</v>
@@ -10945,20 +10945,20 @@
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="28" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C7" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>7</v>
@@ -10969,14 +10969,14 @@
         <v>335</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>7</v>
@@ -10987,14 +10987,14 @@
         <v>334</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>7</v>
@@ -11005,14 +11005,14 @@
         <v>336</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>7</v>
@@ -11023,7 +11023,7 @@
         <v>268</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>357</v>
@@ -11033,7 +11033,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>7</v>
@@ -11044,14 +11044,14 @@
         <v>331</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>7</v>
@@ -11062,7 +11062,7 @@
         <v>370</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C13" t="s">
         <v>373</v>
@@ -11074,7 +11074,7 @@
         <v>372</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>7</v>
@@ -11085,7 +11085,7 @@
         <v>374</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C14" t="s">
         <v>375</v>
@@ -11097,7 +11097,7 @@
         <v>376</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>7</v>
@@ -11108,7 +11108,7 @@
         <v>380</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C15" t="s">
         <v>378</v>
@@ -11120,7 +11120,7 @@
         <v>379</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>7</v>
@@ -11131,7 +11131,7 @@
         <v>382</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C16" t="s">
         <v>383</v>
@@ -11143,7 +11143,7 @@
         <v>384</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>7</v>
@@ -11154,7 +11154,7 @@
         <v>267</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
@@ -11164,7 +11164,7 @@
         <v>19</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>7</v>
@@ -11176,7 +11176,7 @@
         <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>7</v>
@@ -11184,17 +11184,17 @@
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="28" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>7</v>
@@ -11202,17 +11202,17 @@
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="28" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>7</v>
@@ -11225,7 +11225,7 @@
         <v>21</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G21" s="34" t="s">
         <v>7</v>
@@ -11238,7 +11238,7 @@
         <v>22</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>7</v>
@@ -11250,7 +11250,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>7</v>
@@ -11262,7 +11262,7 @@
         <v>24</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>7</v>
@@ -11273,7 +11273,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>366</v>
@@ -11283,7 +11283,7 @@
         <v>26</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>7</v>
@@ -11294,7 +11294,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>367</v>
@@ -11304,7 +11304,7 @@
         <v>28</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>7</v>
@@ -11315,7 +11315,7 @@
         <v>29</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>368</v>
@@ -11325,7 +11325,7 @@
         <v>30</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>7</v>
@@ -11336,7 +11336,7 @@
         <v>318</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>369</v>
@@ -11346,7 +11346,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>7</v>
@@ -11358,7 +11358,7 @@
         <v>32</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>7</v>
@@ -11372,7 +11372,7 @@
         <v>34</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>7</v>
@@ -11386,7 +11386,7 @@
         <v>35</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>7</v>
@@ -11398,7 +11398,7 @@
         <v>36</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>7</v>
@@ -11410,7 +11410,7 @@
         <v>37</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>7</v>
@@ -11421,7 +11421,7 @@
         <v>319</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C34" t="s">
         <v>359</v>
@@ -11431,7 +11431,7 @@
         <v>38</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>7</v>
@@ -11442,7 +11442,7 @@
         <v>320</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C35" t="s">
         <v>360</v>
@@ -11452,7 +11452,7 @@
         <v>39</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>7</v>
@@ -11463,7 +11463,7 @@
         <v>266</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C36" t="s">
         <v>358</v>
@@ -11473,7 +11473,7 @@
         <v>40</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>7</v>
@@ -11487,7 +11487,7 @@
         <v>41</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>7</v>
@@ -11501,7 +11501,7 @@
         <v>42</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>7</v>
@@ -11513,7 +11513,7 @@
         <v>43</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>7</v>
@@ -11524,17 +11524,17 @@
         <v>385</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
         <v>387</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>7</v>
@@ -11542,20 +11542,20 @@
     </row>
     <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="28" t="s">
+        <v>454</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="C41" t="s">
         <v>455</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C41" t="s">
-        <v>456</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>7</v>
@@ -11566,17 +11566,17 @@
         <v>386</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C42" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
         <v>388</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>7</v>
@@ -11584,14 +11584,14 @@
     </row>
     <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B43" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>7</v>
@@ -11602,7 +11602,7 @@
         <v>345</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>353</v>
@@ -11612,7 +11612,7 @@
         <v>348</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>7</v>
@@ -11623,7 +11623,7 @@
         <v>346</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>354</v>
@@ -11633,7 +11633,7 @@
         <v>349</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>7</v>
@@ -11644,7 +11644,7 @@
         <v>347</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>355</v>
@@ -11654,7 +11654,7 @@
         <v>350</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>7</v>
@@ -11665,7 +11665,7 @@
         <v>352</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>356</v>
@@ -11675,7 +11675,7 @@
         <v>351</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>7</v>
@@ -11686,7 +11686,7 @@
         <v>324</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>338</v>
@@ -11696,7 +11696,7 @@
         <v>45</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>7</v>
@@ -11704,10 +11704,10 @@
     </row>
     <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="C49" s="4" t="s">
         <v>523</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>524</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -11719,7 +11719,7 @@
         <v>46</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>7</v>
@@ -11737,7 +11737,7 @@
         <v>47</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>7</v>
@@ -11757,7 +11757,7 @@
     </row>
     <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="28" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>50</v>
@@ -11838,10 +11838,10 @@
         <v>322</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
@@ -11859,10 +11859,10 @@
         <v>321</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
@@ -11905,10 +11905,10 @@
     </row>
     <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="28" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>61</v>
@@ -11926,7 +11926,7 @@
     </row>
     <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="28" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
@@ -11980,10 +11980,10 @@
         <v>301</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
@@ -12004,10 +12004,10 @@
         <v>298</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
@@ -12028,10 +12028,10 @@
         <v>297</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
@@ -12053,7 +12053,7 @@
         <v>71</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G71" s="6" t="s">
         <v>7</v>
@@ -12065,7 +12065,7 @@
         <v>72</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>7</v>
@@ -12079,7 +12079,7 @@
         <v>73</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G73" s="6" t="s">
         <v>7</v>
@@ -12093,7 +12093,7 @@
         <v>74</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G74" s="6" t="s">
         <v>7</v>
@@ -12107,7 +12107,7 @@
         <v>75</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>7</v>
@@ -12121,7 +12121,7 @@
         <v>76</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G76" s="6" t="s">
         <v>7</v>
@@ -12135,7 +12135,7 @@
         <v>77</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>7</v>
@@ -12149,7 +12149,7 @@
         <v>78</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>7</v>
@@ -12161,7 +12161,7 @@
         <v>79</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>7</v>
@@ -12175,7 +12175,7 @@
         <v>80</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>7</v>
@@ -12189,7 +12189,7 @@
         <v>81</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>7</v>
@@ -12288,14 +12288,14 @@
         <v>282</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
         <v>89</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>7</v>
@@ -12303,20 +12303,20 @@
     </row>
     <row r="90" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A90" s="28" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="35" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>7</v>
@@ -12324,20 +12324,20 @@
     </row>
     <row r="91" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A91" s="28" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>7</v>
@@ -12348,14 +12348,14 @@
         <v>303</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
         <v>90</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G92" s="6" t="s">
         <v>7</v>
@@ -12363,20 +12363,20 @@
     </row>
     <row r="93" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A93" s="28" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
         <v>91</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G93" s="6" t="s">
         <v>7</v>
@@ -12387,20 +12387,20 @@
     </row>
     <row r="94" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="28" t="s">
+        <v>494</v>
+      </c>
+      <c r="B94" s="25" t="s">
+        <v>432</v>
+      </c>
+      <c r="C94" s="4" t="s">
         <v>495</v>
-      </c>
-      <c r="B94" s="25" t="s">
-        <v>433</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>496</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G94" s="6" t="s">
         <v>7</v>
@@ -12411,20 +12411,20 @@
     </row>
     <row r="95" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="28" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C95" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G95" s="6" t="s">
         <v>7</v>
@@ -12435,20 +12435,20 @@
     </row>
     <row r="96" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A96" s="28" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C96" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G96" s="6" t="s">
         <v>7</v>
@@ -12465,7 +12465,7 @@
         <v>94</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>7</v>
@@ -12479,7 +12479,7 @@
         <v>95</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G98" s="6" t="s">
         <v>7</v>
@@ -12493,7 +12493,7 @@
         <v>96</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="G99" s="6" t="s">
         <v>7</v>
@@ -12505,7 +12505,7 @@
         <v>97</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>7</v>
@@ -12513,20 +12513,20 @@
     </row>
     <row r="101" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A101" s="28" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C101" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>7</v>
@@ -12534,20 +12534,20 @@
     </row>
     <row r="102" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A102" s="28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C102" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G102" s="6" t="s">
         <v>7</v>
@@ -12555,20 +12555,20 @@
     </row>
     <row r="103" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A103" s="28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
         <v>98</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G103" s="6" t="s">
         <v>7</v>
@@ -12579,17 +12579,17 @@
         <v>284</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G104" s="6" t="s">
         <v>7</v>
@@ -12600,17 +12600,17 @@
         <v>325</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C105" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
         <v>100</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G105" s="6" t="s">
         <v>7</v>
@@ -12618,20 +12618,20 @@
     </row>
     <row r="106" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A106" s="28" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4" t="s">
         <v>101</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G106" s="6" t="s">
         <v>7</v>
@@ -12642,10 +12642,10 @@
         <v>287</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D107" s="10" t="s">
         <v>292</v>
@@ -12654,7 +12654,7 @@
         <v>102</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G107" s="6" t="s">
         <v>7</v>
@@ -12665,17 +12665,17 @@
         <v>326</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C108" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G108" s="6" t="s">
         <v>7</v>
@@ -12689,17 +12689,17 @@
         <v>409</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C109" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D109" s="10"/>
       <c r="E109" t="s">
         <v>410</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G109" s="6" t="s">
         <v>7</v>
@@ -12710,17 +12710,17 @@
         <v>416</v>
       </c>
       <c r="B110" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D110" s="10"/>
       <c r="E110" t="s">
-        <v>417</v>
+        <v>555</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G110" s="6" t="s">
         <v>7</v>
@@ -12728,22 +12728,22 @@
     </row>
     <row r="111" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A111" s="28" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C111" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D111" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E111" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G111" s="6" t="s">
         <v>7</v>
@@ -12754,14 +12754,14 @@
         <v>327</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
         <v>103</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G112" s="6" t="s">
         <v>7</v>
@@ -12772,10 +12772,10 @@
         <v>288</v>
       </c>
       <c r="B113" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>291</v>
@@ -12784,7 +12784,7 @@
         <v>104</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G113" s="6" t="s">
         <v>7</v>
@@ -12795,17 +12795,17 @@
         <v>290</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4" t="s">
         <v>105</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G114" s="6" t="s">
         <v>7</v>
@@ -12813,20 +12813,20 @@
     </row>
     <row r="115" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A115" s="28" t="s">
+        <v>519</v>
+      </c>
+      <c r="B115" s="25" t="s">
+        <v>432</v>
+      </c>
+      <c r="C115" s="4" t="s">
         <v>520</v>
-      </c>
-      <c r="B115" s="25" t="s">
-        <v>433</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>521</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G115" s="6" t="s">
         <v>7</v>
@@ -12837,17 +12837,17 @@
         <v>401</v>
       </c>
       <c r="B116" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4" t="s">
         <v>403</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G116" s="6" t="s">
         <v>7</v>
@@ -12858,17 +12858,17 @@
         <v>402</v>
       </c>
       <c r="B117" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4" t="s">
         <v>404</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G117" s="6" t="s">
         <v>7</v>
@@ -12879,17 +12879,17 @@
         <v>289</v>
       </c>
       <c r="B118" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
         <v>106</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G118" s="6" t="s">
         <v>7</v>
@@ -12903,17 +12903,17 @@
         <v>408</v>
       </c>
       <c r="B119" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G119" s="6" t="s">
         <v>7</v>
@@ -12924,20 +12924,20 @@
     </row>
     <row r="120" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A120" s="28" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B120" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C120" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G120" s="6" t="s">
         <v>7</v>
@@ -12945,20 +12945,20 @@
     </row>
     <row r="121" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A121" s="28" t="s">
+        <v>503</v>
+      </c>
+      <c r="B121" s="25" t="s">
+        <v>432</v>
+      </c>
+      <c r="C121" s="4" t="s">
         <v>504</v>
-      </c>
-      <c r="B121" s="25" t="s">
-        <v>433</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>505</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G121" s="6" t="s">
         <v>7</v>
@@ -12966,20 +12966,20 @@
     </row>
     <row r="122" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A122" s="28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B122" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4" t="s">
         <v>108</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G122" s="6" t="s">
         <v>7</v>
@@ -12990,17 +12990,17 @@
         <v>283</v>
       </c>
       <c r="B123" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4" t="s">
         <v>109</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G123" s="6" t="s">
         <v>7</v>
@@ -13011,7 +13011,7 @@
         <v>393</v>
       </c>
       <c r="B124" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C124" t="s">
         <v>394</v>
@@ -13021,7 +13021,7 @@
         <v>110</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G124" s="6" t="s">
         <v>7</v>
@@ -13029,20 +13029,20 @@
     </row>
     <row r="125" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A125" s="28" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B125" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G125" s="6" t="s">
         <v>7</v>
@@ -13053,10 +13053,10 @@
         <v>275</v>
       </c>
       <c r="B126" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>248</v>
@@ -13065,7 +13065,7 @@
         <v>112</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G126" s="6" t="s">
         <v>7</v>
@@ -13076,17 +13076,17 @@
         <v>329</v>
       </c>
       <c r="B127" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C127" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4" t="s">
         <v>113</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G127" s="6" t="s">
         <v>7</v>
@@ -13100,10 +13100,10 @@
         <v>276</v>
       </c>
       <c r="B128" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>249</v>
@@ -13112,7 +13112,7 @@
         <v>250</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G128" s="6" t="s">
         <v>7</v>
@@ -13123,7 +13123,7 @@
         <v>391</v>
       </c>
       <c r="B129" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>392</v>
@@ -13133,7 +13133,7 @@
         <v>395</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G129" s="6" t="s">
         <v>7</v>
@@ -13144,17 +13144,17 @@
         <v>328</v>
       </c>
       <c r="B130" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4" t="s">
         <v>114</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G130" s="6" t="s">
         <v>7</v>
@@ -13165,7 +13165,7 @@
         <v>396</v>
       </c>
       <c r="B131" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>398</v>
@@ -13175,7 +13175,7 @@
         <v>397</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G131" s="6" t="s">
         <v>7</v>
@@ -13186,14 +13186,14 @@
         <v>327</v>
       </c>
       <c r="B132" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4" t="s">
         <v>115</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G132" s="6" t="s">
         <v>7</v>
@@ -13204,17 +13204,17 @@
         <v>274</v>
       </c>
       <c r="B133" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4" t="s">
         <v>116</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G133" s="6" t="s">
         <v>7</v>
@@ -13225,17 +13225,17 @@
         <v>286</v>
       </c>
       <c r="B134" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G134" s="6" t="s">
         <v>7</v>
@@ -13246,17 +13246,17 @@
         <v>399</v>
       </c>
       <c r="B135" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4" t="s">
         <v>400</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G135" s="6" t="s">
         <v>7</v>
@@ -13267,7 +13267,7 @@
         <v>285</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>340</v>
@@ -13277,7 +13277,7 @@
         <v>118</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G136" s="6" t="s">
         <v>7</v>
@@ -13288,7 +13288,7 @@
         <v>389</v>
       </c>
       <c r="B137" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>119</v>
@@ -13298,7 +13298,7 @@
         <v>119</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G137" s="6" t="s">
         <v>7</v>
@@ -13310,7 +13310,7 @@
         <v>295</v>
       </c>
       <c r="B138" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4" t="s">
@@ -13325,10 +13325,10 @@
     </row>
     <row r="139" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A139" s="28" t="s">
+        <v>458</v>
+      </c>
+      <c r="C139" s="4" t="s">
         <v>459</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>460</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4" t="s">
@@ -13357,10 +13357,10 @@
     </row>
     <row r="141" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A141" s="28" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4" t="s">
@@ -13389,10 +13389,10 @@
     </row>
     <row r="143" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A143" s="28" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D143" s="4"/>
       <c r="E143" s="4" t="s">
@@ -13463,7 +13463,7 @@
         <v>293</v>
       </c>
       <c r="B148" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4" t="s">
@@ -13482,7 +13482,7 @@
         <v>333</v>
       </c>
       <c r="B149" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
@@ -13501,7 +13501,7 @@
         <v>332</v>
       </c>
       <c r="B150" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4" t="s">
@@ -13546,7 +13546,7 @@
         <v>294</v>
       </c>
       <c r="B153" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4" t="s">
@@ -13562,10 +13562,10 @@
     </row>
     <row r="154" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A154" s="28" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B154" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4" t="s">
@@ -13596,7 +13596,7 @@
     </row>
     <row r="156" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A156" s="8" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4" t="s">
@@ -13615,10 +13615,10 @@
         <v>273</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4" t="s">
@@ -13634,10 +13634,10 @@
     </row>
     <row r="158" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A158" s="8" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B158" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4" t="s">
@@ -13682,10 +13682,10 @@
         <v>308</v>
       </c>
       <c r="B161" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C161" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D161" s="4"/>
       <c r="E161" s="4" t="s">
@@ -13718,7 +13718,7 @@
         <v>317</v>
       </c>
       <c r="B163" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D163" s="4"/>
       <c r="E163" s="4" t="s">
@@ -13748,7 +13748,7 @@
         <v>363</v>
       </c>
       <c r="B165" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D165" s="10" t="s">
         <v>364</v>
@@ -13791,7 +13791,7 @@
     </row>
     <row r="168" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A168" s="28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D168" s="4"/>
       <c r="E168" s="4" t="s">
@@ -13806,13 +13806,13 @@
     </row>
     <row r="169" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A169" s="28" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C169" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D169" s="4"/>
       <c r="E169" s="4" t="s">
@@ -13833,10 +13833,10 @@
         <v>390</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C170" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4" t="s">
@@ -13851,17 +13851,17 @@
     </row>
     <row r="171" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A171" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="B171" s="25" t="s">
+        <v>433</v>
+      </c>
+      <c r="C171" t="s">
         <v>487</v>
-      </c>
-      <c r="B171" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C171" t="s">
-        <v>488</v>
       </c>
       <c r="D171" s="4"/>
       <c r="E171" s="4" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F171" s="5" t="s">
         <v>9</v>
@@ -13929,7 +13929,7 @@
         <v>271</v>
       </c>
       <c r="B176" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>159</v>
@@ -14028,7 +14028,7 @@
         <v>311</v>
       </c>
       <c r="B183" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D183" s="4"/>
       <c r="E183" s="4" t="s">
@@ -14049,7 +14049,7 @@
         <v>265</v>
       </c>
       <c r="B184" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C184" t="s">
         <v>339</v>
@@ -14131,7 +14131,7 @@
         <v>174</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="G190" s="6" t="s">
         <v>7</v>
@@ -14143,7 +14143,7 @@
         <v>175</v>
       </c>
       <c r="F191" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G191" s="6" t="s">
         <v>7</v>
@@ -14155,7 +14155,7 @@
         <v>176</v>
       </c>
       <c r="F192" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G192" s="6" t="s">
         <v>7</v>
@@ -14175,7 +14175,7 @@
     </row>
     <row r="194" spans="1:8" s="15" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A194" s="31" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B194" s="27"/>
       <c r="D194" s="19" t="s">
@@ -14206,7 +14206,7 @@
         <v>180</v>
       </c>
       <c r="F196" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G196" s="6" t="s">
         <v>7</v>
@@ -14272,7 +14272,7 @@
         <v>185</v>
       </c>
       <c r="F201" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G201" s="6" t="s">
         <v>7</v>
@@ -14286,7 +14286,7 @@
         <v>185</v>
       </c>
       <c r="F202" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G202" s="6" t="s">
         <v>7</v>
@@ -14298,7 +14298,7 @@
         <v>186</v>
       </c>
       <c r="F203" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G203" s="6" t="s">
         <v>7</v>
@@ -14309,7 +14309,7 @@
         <v>330</v>
       </c>
       <c r="C204" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D204" s="4"/>
       <c r="E204" s="4" t="s">
@@ -14348,7 +14348,7 @@
     </row>
     <row r="207" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A207" s="28" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4" t="s">
@@ -14366,7 +14366,7 @@
         <v>411</v>
       </c>
       <c r="B208" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C208" s="4" t="s">
         <v>413</v>
@@ -14386,13 +14386,13 @@
     </row>
     <row r="209" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A209" s="28" t="s">
+        <v>425</v>
+      </c>
+      <c r="B209" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C209" s="4" t="s">
         <v>426</v>
-      </c>
-      <c r="B209" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C209" s="4" t="s">
-        <v>427</v>
       </c>
       <c r="D209" s="9"/>
       <c r="E209" s="4" t="s">
@@ -14410,7 +14410,7 @@
         <v>412</v>
       </c>
       <c r="B210" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C210" s="4" t="s">
         <v>414</v>
@@ -14431,10 +14431,10 @@
         <v>314</v>
       </c>
       <c r="B211" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D211" s="4"/>
       <c r="E211" s="4" t="s">
@@ -14452,10 +14452,10 @@
         <v>315</v>
       </c>
       <c r="B212" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C212" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D212" s="4"/>
       <c r="E212" s="4" t="s">
@@ -14499,7 +14499,7 @@
         <v>407</v>
       </c>
       <c r="B215" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>406</v>
@@ -14517,7 +14517,7 @@
     </row>
     <row r="216" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A216" s="30" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D216" s="4"/>
       <c r="E216" s="4" t="s">
@@ -14548,7 +14548,7 @@
         <v>199</v>
       </c>
       <c r="F218" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G218" s="6" t="s">
         <v>7</v>
@@ -14568,13 +14568,13 @@
     </row>
     <row r="220" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A220" s="28" t="s">
+        <v>417</v>
+      </c>
+      <c r="B220" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C220" s="4" t="s">
         <v>418</v>
-      </c>
-      <c r="B220" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C220" s="4" t="s">
-        <v>419</v>
       </c>
       <c r="D220" s="4"/>
       <c r="E220" s="4" t="s">
@@ -14592,7 +14592,7 @@
         <v>281</v>
       </c>
       <c r="C221" s="4" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D221" s="4"/>
       <c r="E221" s="4" t="s">
@@ -14610,7 +14610,7 @@
         <v>280</v>
       </c>
       <c r="B222" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C222" t="s">
         <v>341</v>
@@ -14652,17 +14652,17 @@
     </row>
     <row r="225" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A225" s="28" t="s">
+        <v>420</v>
+      </c>
+      <c r="B225" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C225" s="4" t="s">
         <v>421</v>
-      </c>
-      <c r="B225" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C225" s="4" t="s">
-        <v>422</v>
       </c>
       <c r="D225" s="4"/>
       <c r="E225" s="4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F225" s="5" t="s">
         <v>52</v>
@@ -14673,17 +14673,17 @@
     </row>
     <row r="226" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A226" s="28" t="s">
+        <v>422</v>
+      </c>
+      <c r="B226" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C226" s="4" t="s">
         <v>423</v>
-      </c>
-      <c r="B226" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C226" s="4" t="s">
-        <v>424</v>
       </c>
       <c r="D226" s="4"/>
       <c r="E226" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F226" s="5" t="s">
         <v>52</v>
@@ -14697,7 +14697,7 @@
         <v>278</v>
       </c>
       <c r="B227" s="25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C227" s="4" t="s">
         <v>405</v>
@@ -14720,17 +14720,17 @@
     </row>
     <row r="228" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A228" s="28" t="s">
+        <v>472</v>
+      </c>
+      <c r="B228" s="25" t="s">
+        <v>434</v>
+      </c>
+      <c r="C228" t="s">
         <v>473</v>
-      </c>
-      <c r="B228" s="25" t="s">
-        <v>435</v>
-      </c>
-      <c r="C228" t="s">
-        <v>474</v>
       </c>
       <c r="D228" s="10"/>
       <c r="E228" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F228" s="5" t="s">
         <v>52</v>
@@ -14786,7 +14786,7 @@
         <v>210</v>
       </c>
       <c r="F232" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G232" s="6" t="s">
         <v>7</v>
@@ -14826,17 +14826,17 @@
         <v>296</v>
       </c>
       <c r="B235" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C235" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D235" s="4"/>
       <c r="E235" s="4" t="s">
         <v>213</v>
       </c>
       <c r="F235" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G235" s="6" t="s">
         <v>7</v>
@@ -14849,7 +14849,7 @@
         <v>214</v>
       </c>
       <c r="F236" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G236" s="6" t="s">
         <v>7</v>
@@ -14862,7 +14862,7 @@
         <v>215</v>
       </c>
       <c r="F237" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G237" s="6" t="s">
         <v>7</v>
@@ -14871,14 +14871,14 @@
     </row>
     <row r="238" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A238" s="28" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D238" s="4"/>
       <c r="E238" s="4" t="s">
         <v>216</v>
       </c>
       <c r="F238" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G238" s="6" t="s">
         <v>7</v>
@@ -14887,14 +14887,14 @@
     </row>
     <row r="239" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A239" s="28" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D239" s="4"/>
       <c r="E239" s="4" t="s">
         <v>217</v>
       </c>
       <c r="F239" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G239" s="6" t="s">
         <v>7</v>
@@ -14907,7 +14907,7 @@
         <v>218</v>
       </c>
       <c r="F240" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G240" s="6" t="s">
         <v>7</v>
@@ -14920,7 +14920,7 @@
         <v>219</v>
       </c>
       <c r="F241" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G241" s="6" t="s">
         <v>7</v>
@@ -14929,20 +14929,20 @@
     </row>
     <row r="242" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A242" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="B242" s="25" t="s">
+        <v>432</v>
+      </c>
+      <c r="C242" t="s">
         <v>475</v>
-      </c>
-      <c r="B242" s="25" t="s">
-        <v>433</v>
-      </c>
-      <c r="C242" t="s">
-        <v>476</v>
       </c>
       <c r="D242" s="4"/>
       <c r="E242" s="4" t="s">
         <v>220</v>
       </c>
       <c r="F242" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G242" s="6" t="s">
         <v>7</v>
@@ -14955,7 +14955,7 @@
         <v>221</v>
       </c>
       <c r="F243" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="G243" s="6" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
detailed by mainly cosmetic improvements to Nitrogen model
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD81F5C-79E9-42BE-A467-36F9674A5453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0510392-9452-4CC8-9E1A-ACA2E2CD807E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30135" yWindow="690" windowWidth="27300" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30375" yWindow="570" windowWidth="27300" windowHeight="13995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="556">
   <si>
     <t>PyOrator variable</t>
   </si>
@@ -2078,16 +2078,7 @@
     <t>aet</t>
   </si>
   <si>
-    <t>aet_prentice</t>
-  </si>
-  <si>
     <t>AET</t>
-  </si>
-  <si>
-    <t>AET Prentice</t>
-  </si>
-  <si>
-    <t>Actual evapotranspiration last month from Prentice</t>
   </si>
   <si>
     <t>nh4_total_loss</t>
@@ -2521,6 +2512,27 @@
   </si>
   <si>
     <t>Ammonium total losses</t>
+  </si>
+  <si>
+    <t>(eq.2.4.7) Effective rainfall (or precipitation) is equal to the difference between total rainfall and actual evapotranspiration.</t>
+  </si>
+  <si>
+    <t>Actual evapotranspiration last month after irrigation</t>
+  </si>
+  <si>
+    <r>
+      <t>Prop. of aerobically produced CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2797,14 +2809,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -9126,7 +9131,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>210</xdr:row>
+      <xdr:row>209</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="200025" cy="190496"/>
@@ -9170,7 +9175,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>211</xdr:row>
+      <xdr:row>210</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="266703" cy="190496"/>
@@ -9214,7 +9219,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>212</xdr:row>
+      <xdr:row>211</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="476246" cy="200025"/>
@@ -9258,7 +9263,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>214</xdr:row>
+      <xdr:row>213</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="304796" cy="190496"/>
@@ -9302,7 +9307,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>215</xdr:row>
+      <xdr:row>214</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="466728" cy="200025"/>
@@ -9346,7 +9351,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>216</xdr:row>
+      <xdr:row>215</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="552453" cy="209553"/>
@@ -9390,7 +9395,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>217</xdr:row>
+      <xdr:row>216</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="295278" cy="209553"/>
@@ -9434,7 +9439,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>218</xdr:row>
+      <xdr:row>217</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="533396" cy="209553"/>
@@ -9478,7 +9483,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>219</xdr:row>
+      <xdr:row>218</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="476246" cy="209553"/>
@@ -9522,7 +9527,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>220</xdr:row>
+      <xdr:row>219</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="390521" cy="200025"/>
@@ -9566,7 +9571,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>221</xdr:row>
+      <xdr:row>220</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257175" cy="190496"/>
@@ -9610,7 +9615,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>222</xdr:row>
+      <xdr:row>221</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="495303" cy="209553"/>
@@ -9654,7 +9659,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>223</xdr:row>
+      <xdr:row>222</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="438153" cy="209553"/>
@@ -9698,7 +9703,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>228</xdr:row>
+      <xdr:row>227</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="514350" cy="200025"/>
@@ -9742,7 +9747,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>229</xdr:row>
+      <xdr:row>228</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="381003" cy="200025"/>
@@ -9786,7 +9791,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>232</xdr:row>
+      <xdr:row>231</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="571500" cy="209553"/>
@@ -9830,7 +9835,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>234</xdr:row>
+      <xdr:row>233</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="390521" cy="209553"/>
@@ -9874,7 +9879,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>235</xdr:row>
+      <xdr:row>234</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="266703" cy="190496"/>
@@ -9918,7 +9923,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>236</xdr:row>
+      <xdr:row>235</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="390521" cy="200025"/>
@@ -9962,7 +9967,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>237</xdr:row>
+      <xdr:row>236</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="276221" cy="190496"/>
@@ -10006,7 +10011,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>238</xdr:row>
+      <xdr:row>237</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="257175" cy="209553"/>
@@ -10050,7 +10055,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>239</xdr:row>
+      <xdr:row>238</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="523878" cy="200025"/>
@@ -10094,7 +10099,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>240</xdr:row>
+      <xdr:row>239</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="533396" cy="200025"/>
@@ -10138,7 +10143,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>241</xdr:row>
+      <xdr:row>240</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="447671" cy="190496"/>
@@ -10182,7 +10187,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>242</xdr:row>
+      <xdr:row>241</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="266703" cy="190496"/>
@@ -10226,7 +10231,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>243</xdr:row>
+      <xdr:row>242</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="76196" cy="190496"/>
@@ -10270,7 +10275,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>244</xdr:row>
+      <xdr:row>243</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="66678" cy="190496"/>
@@ -10314,7 +10319,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>245</xdr:row>
+      <xdr:row>244</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="142875" cy="190496"/>
@@ -10358,7 +10363,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>246</xdr:row>
+      <xdr:row>245</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="200025" cy="190496"/>
@@ -10402,7 +10407,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>247</xdr:row>
+      <xdr:row>246</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="314325" cy="190496"/>
@@ -10446,7 +10451,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>248</xdr:row>
+      <xdr:row>247</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="95253" cy="190496"/>
@@ -10831,11 +10836,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H249"/>
+  <dimension ref="A1:H248"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E123" sqref="E123"/>
+      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -10847,7 +10852,7 @@
     <col min="5" max="5" width="120" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="19.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="44.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="64.5703125" style="13" customWidth="1"/>
     <col min="9" max="9" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10856,7 +10861,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>337</v>
@@ -10894,7 +10899,7 @@
         <v>277</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
@@ -10925,7 +10930,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>7</v>
@@ -10937,7 +10942,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>7</v>
@@ -10945,20 +10950,20 @@
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="28" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C7" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>7</v>
@@ -10969,14 +10974,14 @@
         <v>335</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>7</v>
@@ -10987,14 +10992,14 @@
         <v>334</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>7</v>
@@ -11005,14 +11010,14 @@
         <v>336</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>7</v>
@@ -11023,7 +11028,7 @@
         <v>268</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>357</v>
@@ -11033,7 +11038,7 @@
         <v>17</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>7</v>
@@ -11044,14 +11049,14 @@
         <v>331</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>7</v>
@@ -11062,7 +11067,7 @@
         <v>370</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C13" t="s">
         <v>373</v>
@@ -11074,7 +11079,7 @@
         <v>372</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>7</v>
@@ -11085,7 +11090,7 @@
         <v>374</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C14" t="s">
         <v>375</v>
@@ -11097,7 +11102,7 @@
         <v>376</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>7</v>
@@ -11108,7 +11113,7 @@
         <v>380</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C15" t="s">
         <v>378</v>
@@ -11120,7 +11125,7 @@
         <v>379</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>7</v>
@@ -11131,7 +11136,7 @@
         <v>382</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C16" t="s">
         <v>383</v>
@@ -11143,7 +11148,7 @@
         <v>384</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>7</v>
@@ -11154,7 +11159,7 @@
         <v>267</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>19</v>
@@ -11164,7 +11169,7 @@
         <v>19</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>7</v>
@@ -11176,7 +11181,7 @@
         <v>20</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>7</v>
@@ -11184,17 +11189,17 @@
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="28" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>7</v>
@@ -11202,17 +11207,17 @@
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="28" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>7</v>
@@ -11225,7 +11230,7 @@
         <v>21</v>
       </c>
       <c r="F21" s="33" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G21" s="34" t="s">
         <v>7</v>
@@ -11238,7 +11243,7 @@
         <v>22</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>7</v>
@@ -11250,7 +11255,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>7</v>
@@ -11262,7 +11267,7 @@
         <v>24</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>7</v>
@@ -11273,7 +11278,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>366</v>
@@ -11283,7 +11288,7 @@
         <v>26</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G25" s="6" t="s">
         <v>7</v>
@@ -11294,7 +11299,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>367</v>
@@ -11304,7 +11309,7 @@
         <v>28</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>7</v>
@@ -11315,7 +11320,7 @@
         <v>29</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>368</v>
@@ -11325,7 +11330,7 @@
         <v>30</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G27" s="6" t="s">
         <v>7</v>
@@ -11336,7 +11341,7 @@
         <v>318</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>369</v>
@@ -11346,7 +11351,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G28" s="6" t="s">
         <v>7</v>
@@ -11358,7 +11363,7 @@
         <v>32</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G29" s="6" t="s">
         <v>7</v>
@@ -11372,7 +11377,7 @@
         <v>34</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>7</v>
@@ -11386,7 +11391,7 @@
         <v>35</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>7</v>
@@ -11398,7 +11403,7 @@
         <v>36</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>7</v>
@@ -11410,7 +11415,7 @@
         <v>37</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>7</v>
@@ -11421,7 +11426,7 @@
         <v>319</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C34" t="s">
         <v>359</v>
@@ -11431,7 +11436,7 @@
         <v>38</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>7</v>
@@ -11442,7 +11447,7 @@
         <v>320</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C35" t="s">
         <v>360</v>
@@ -11452,7 +11457,7 @@
         <v>39</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>7</v>
@@ -11463,7 +11468,7 @@
         <v>266</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C36" t="s">
         <v>358</v>
@@ -11473,7 +11478,7 @@
         <v>40</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>7</v>
@@ -11487,7 +11492,7 @@
         <v>41</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>7</v>
@@ -11501,7 +11506,7 @@
         <v>42</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>7</v>
@@ -11513,7 +11518,7 @@
         <v>43</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>7</v>
@@ -11524,17 +11529,17 @@
         <v>385</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4" t="s">
         <v>387</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>7</v>
@@ -11542,20 +11547,20 @@
     </row>
     <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="28" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C41" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>7</v>
@@ -11566,17 +11571,17 @@
         <v>386</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C42" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="4" t="s">
         <v>388</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>7</v>
@@ -11584,14 +11589,14 @@
     </row>
     <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B43" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>7</v>
@@ -11602,7 +11607,7 @@
         <v>345</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>353</v>
@@ -11612,7 +11617,7 @@
         <v>348</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>7</v>
@@ -11623,7 +11628,7 @@
         <v>346</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>354</v>
@@ -11633,7 +11638,7 @@
         <v>349</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>7</v>
@@ -11644,7 +11649,7 @@
         <v>347</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>355</v>
@@ -11654,7 +11659,7 @@
         <v>350</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>7</v>
@@ -11665,7 +11670,7 @@
         <v>352</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>356</v>
@@ -11675,7 +11680,7 @@
         <v>351</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>7</v>
@@ -11686,7 +11691,7 @@
         <v>324</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>338</v>
@@ -11696,7 +11701,7 @@
         <v>45</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>7</v>
@@ -11704,10 +11709,10 @@
     </row>
     <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="28" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
@@ -11719,7 +11724,7 @@
         <v>46</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>7</v>
@@ -11737,7 +11742,7 @@
         <v>47</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>7</v>
@@ -11757,7 +11762,7 @@
     </row>
     <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="28" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>50</v>
@@ -11838,10 +11843,10 @@
         <v>322</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
@@ -11859,10 +11864,10 @@
         <v>321</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
@@ -11905,10 +11910,10 @@
     </row>
     <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A63" s="28" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>61</v>
@@ -11926,7 +11931,7 @@
     </row>
     <row r="64" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A64" s="28" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4" t="s">
@@ -11980,10 +11985,10 @@
         <v>301</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
@@ -12004,10 +12009,10 @@
         <v>298</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
@@ -12028,10 +12033,10 @@
         <v>297</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
@@ -12053,7 +12058,7 @@
         <v>71</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G71" s="6" t="s">
         <v>7</v>
@@ -12065,7 +12070,7 @@
         <v>72</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G72" s="6" t="s">
         <v>7</v>
@@ -12079,7 +12084,7 @@
         <v>73</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G73" s="6" t="s">
         <v>7</v>
@@ -12093,7 +12098,7 @@
         <v>74</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G74" s="6" t="s">
         <v>7</v>
@@ -12107,7 +12112,7 @@
         <v>75</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G75" s="6" t="s">
         <v>7</v>
@@ -12121,7 +12126,7 @@
         <v>76</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G76" s="6" t="s">
         <v>7</v>
@@ -12135,7 +12140,7 @@
         <v>77</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G77" s="6" t="s">
         <v>7</v>
@@ -12149,7 +12154,7 @@
         <v>78</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G78" s="6" t="s">
         <v>7</v>
@@ -12161,7 +12166,7 @@
         <v>79</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G79" s="6" t="s">
         <v>7</v>
@@ -12175,7 +12180,7 @@
         <v>80</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G80" s="6" t="s">
         <v>7</v>
@@ -12189,7 +12194,7 @@
         <v>81</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G81" s="6" t="s">
         <v>7</v>
@@ -12288,14 +12293,14 @@
         <v>282</v>
       </c>
       <c r="B89" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
         <v>89</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>7</v>
@@ -12303,20 +12308,20 @@
     </row>
     <row r="90" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A90" s="28" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="35" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G90" s="6" t="s">
         <v>7</v>
@@ -12324,20 +12329,20 @@
     </row>
     <row r="91" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A91" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="B91" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="C91" s="4" t="s">
         <v>489</v>
-      </c>
-      <c r="B91" s="25" t="s">
-        <v>432</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>492</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>7</v>
@@ -12348,14 +12353,14 @@
         <v>303</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
         <v>90</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G92" s="6" t="s">
         <v>7</v>
@@ -12363,20 +12368,20 @@
     </row>
     <row r="93" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A93" s="28" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B93" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D93" s="4"/>
       <c r="E93" s="4" t="s">
         <v>91</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G93" s="6" t="s">
         <v>7</v>
@@ -12387,20 +12392,20 @@
     </row>
     <row r="94" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="28" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G94" s="6" t="s">
         <v>7</v>
@@ -12411,20 +12416,20 @@
     </row>
     <row r="95" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="28" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B95" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C95" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
         <v>92</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G95" s="6" t="s">
         <v>7</v>
@@ -12435,20 +12440,20 @@
     </row>
     <row r="96" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A96" s="28" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C96" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G96" s="6" t="s">
         <v>7</v>
@@ -12465,7 +12470,7 @@
         <v>94</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>7</v>
@@ -12479,7 +12484,7 @@
         <v>95</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G98" s="6" t="s">
         <v>7</v>
@@ -12493,7 +12498,7 @@
         <v>96</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G99" s="6" t="s">
         <v>7</v>
@@ -12505,7 +12510,7 @@
         <v>97</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G100" s="6" t="s">
         <v>7</v>
@@ -12513,20 +12518,20 @@
     </row>
     <row r="101" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A101" s="28" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C101" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G101" s="6" t="s">
         <v>7</v>
@@ -12534,20 +12539,20 @@
     </row>
     <row r="102" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A102" s="28" t="s">
+        <v>477</v>
+      </c>
+      <c r="B102" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="C102" t="s">
         <v>480</v>
-      </c>
-      <c r="B102" s="25" t="s">
-        <v>432</v>
-      </c>
-      <c r="C102" t="s">
-        <v>483</v>
       </c>
       <c r="D102" s="4"/>
       <c r="E102" s="4" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G102" s="6" t="s">
         <v>7</v>
@@ -12555,20 +12560,20 @@
     </row>
     <row r="103" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A103" s="28" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="D103" s="4"/>
       <c r="E103" s="4" t="s">
         <v>98</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G103" s="6" t="s">
         <v>7</v>
@@ -12579,17 +12584,17 @@
         <v>284</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
         <v>99</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G104" s="6" t="s">
         <v>7</v>
@@ -12600,17 +12605,17 @@
         <v>325</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C105" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
         <v>100</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G105" s="6" t="s">
         <v>7</v>
@@ -12618,20 +12623,20 @@
     </row>
     <row r="106" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A106" s="28" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4" t="s">
         <v>101</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G106" s="6" t="s">
         <v>7</v>
@@ -12642,10 +12647,10 @@
         <v>287</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D107" s="10" t="s">
         <v>292</v>
@@ -12654,7 +12659,7 @@
         <v>102</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G107" s="6" t="s">
         <v>7</v>
@@ -12665,17 +12670,17 @@
         <v>326</v>
       </c>
       <c r="B108" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C108" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G108" s="6" t="s">
         <v>7</v>
@@ -12689,17 +12694,17 @@
         <v>409</v>
       </c>
       <c r="B109" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C109" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="D109" s="10"/>
       <c r="E109" t="s">
         <v>410</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G109" s="6" t="s">
         <v>7</v>
@@ -12707,20 +12712,20 @@
     </row>
     <row r="110" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A110" s="28" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B110" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="D110" s="10"/>
       <c r="E110" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G110" s="6" t="s">
         <v>7</v>
@@ -12728,22 +12733,22 @@
     </row>
     <row r="111" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A111" s="28" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B111" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C111" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="D111" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="E111" t="s">
         <v>505</v>
       </c>
-      <c r="E111" t="s">
-        <v>508</v>
-      </c>
       <c r="F111" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G111" s="6" t="s">
         <v>7</v>
@@ -12754,14 +12759,14 @@
         <v>327</v>
       </c>
       <c r="B112" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4" t="s">
         <v>103</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G112" s="6" t="s">
         <v>7</v>
@@ -12772,10 +12777,10 @@
         <v>288</v>
       </c>
       <c r="B113" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>291</v>
@@ -12784,7 +12789,7 @@
         <v>104</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G113" s="6" t="s">
         <v>7</v>
@@ -12795,17 +12800,17 @@
         <v>290</v>
       </c>
       <c r="B114" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4" t="s">
         <v>105</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G114" s="6" t="s">
         <v>7</v>
@@ -12813,20 +12818,20 @@
     </row>
     <row r="115" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A115" s="28" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B115" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="D115" s="4"/>
       <c r="E115" s="4" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G115" s="6" t="s">
         <v>7</v>
@@ -12837,17 +12842,17 @@
         <v>401</v>
       </c>
       <c r="B116" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="4" t="s">
         <v>403</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G116" s="6" t="s">
         <v>7</v>
@@ -12858,17 +12863,17 @@
         <v>402</v>
       </c>
       <c r="B117" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="4" t="s">
         <v>404</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G117" s="6" t="s">
         <v>7</v>
@@ -12879,17 +12884,17 @@
         <v>289</v>
       </c>
       <c r="B118" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D118" s="4"/>
       <c r="E118" s="4" t="s">
         <v>106</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G118" s="6" t="s">
         <v>7</v>
@@ -12903,17 +12908,17 @@
         <v>408</v>
       </c>
       <c r="B119" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="D119" s="4"/>
       <c r="E119" s="4" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G119" s="6" t="s">
         <v>7</v>
@@ -12924,20 +12929,20 @@
     </row>
     <row r="120" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A120" s="28" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B120" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C120" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D120" s="4"/>
       <c r="E120" s="4" t="s">
         <v>107</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G120" s="6" t="s">
         <v>7</v>
@@ -12945,20 +12950,20 @@
     </row>
     <row r="121" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A121" s="28" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B121" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="4" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G121" s="6" t="s">
         <v>7</v>
@@ -12966,20 +12971,20 @@
     </row>
     <row r="122" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A122" s="28" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B122" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D122" s="4"/>
       <c r="E122" s="4" t="s">
         <v>108</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G122" s="6" t="s">
         <v>7</v>
@@ -12990,17 +12995,17 @@
         <v>283</v>
       </c>
       <c r="B123" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D123" s="4"/>
       <c r="E123" s="4" t="s">
         <v>109</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G123" s="6" t="s">
         <v>7</v>
@@ -13011,7 +13016,7 @@
         <v>393</v>
       </c>
       <c r="B124" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C124" t="s">
         <v>394</v>
@@ -13021,7 +13026,7 @@
         <v>110</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G124" s="6" t="s">
         <v>7</v>
@@ -13029,20 +13034,20 @@
     </row>
     <row r="125" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A125" s="28" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B125" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D125" s="4"/>
       <c r="E125" s="4" t="s">
         <v>111</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G125" s="6" t="s">
         <v>7</v>
@@ -13053,10 +13058,10 @@
         <v>275</v>
       </c>
       <c r="B126" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>248</v>
@@ -13065,7 +13070,7 @@
         <v>112</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G126" s="6" t="s">
         <v>7</v>
@@ -13076,17 +13081,17 @@
         <v>329</v>
       </c>
       <c r="B127" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C127" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D127" s="4"/>
       <c r="E127" s="4" t="s">
         <v>113</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G127" s="6" t="s">
         <v>7</v>
@@ -13100,10 +13105,10 @@
         <v>276</v>
       </c>
       <c r="B128" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>249</v>
@@ -13112,7 +13117,7 @@
         <v>250</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G128" s="6" t="s">
         <v>7</v>
@@ -13123,7 +13128,7 @@
         <v>391</v>
       </c>
       <c r="B129" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>392</v>
@@ -13133,7 +13138,7 @@
         <v>395</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G129" s="6" t="s">
         <v>7</v>
@@ -13144,17 +13149,17 @@
         <v>328</v>
       </c>
       <c r="B130" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="D130" s="4"/>
       <c r="E130" s="4" t="s">
         <v>114</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G130" s="6" t="s">
         <v>7</v>
@@ -13165,7 +13170,7 @@
         <v>396</v>
       </c>
       <c r="B131" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>398</v>
@@ -13175,7 +13180,7 @@
         <v>397</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G131" s="6" t="s">
         <v>7</v>
@@ -13186,14 +13191,14 @@
         <v>327</v>
       </c>
       <c r="B132" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D132" s="4"/>
       <c r="E132" s="4" t="s">
         <v>115</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G132" s="6" t="s">
         <v>7</v>
@@ -13204,17 +13209,17 @@
         <v>274</v>
       </c>
       <c r="B133" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="4" t="s">
         <v>116</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G133" s="6" t="s">
         <v>7</v>
@@ -13225,17 +13230,17 @@
         <v>286</v>
       </c>
       <c r="B134" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="D134" s="4"/>
       <c r="E134" s="4" t="s">
         <v>117</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G134" s="6" t="s">
         <v>7</v>
@@ -13246,17 +13251,17 @@
         <v>399</v>
       </c>
       <c r="B135" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D135" s="4"/>
       <c r="E135" s="4" t="s">
         <v>400</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G135" s="6" t="s">
         <v>7</v>
@@ -13267,7 +13272,7 @@
         <v>285</v>
       </c>
       <c r="B136" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C136" s="4" t="s">
         <v>340</v>
@@ -13277,7 +13282,7 @@
         <v>118</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G136" s="6" t="s">
         <v>7</v>
@@ -13288,7 +13293,7 @@
         <v>389</v>
       </c>
       <c r="B137" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>119</v>
@@ -13298,7 +13303,7 @@
         <v>119</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G137" s="6" t="s">
         <v>7</v>
@@ -13310,7 +13315,7 @@
         <v>295</v>
       </c>
       <c r="B138" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D138" s="4"/>
       <c r="E138" s="4" t="s">
@@ -13325,10 +13330,10 @@
     </row>
     <row r="139" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A139" s="28" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D139" s="4"/>
       <c r="E139" s="4" t="s">
@@ -13357,10 +13362,10 @@
     </row>
     <row r="141" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A141" s="28" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D141" s="4"/>
       <c r="E141" s="4" t="s">
@@ -13389,10 +13394,10 @@
     </row>
     <row r="143" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A143" s="28" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D143" s="4"/>
       <c r="E143" s="4" t="s">
@@ -13463,7 +13468,10 @@
         <v>293</v>
       </c>
       <c r="B148" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>555</v>
       </c>
       <c r="D148" s="4"/>
       <c r="E148" s="4" t="s">
@@ -13482,7 +13490,7 @@
         <v>333</v>
       </c>
       <c r="B149" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
@@ -13501,7 +13509,7 @@
         <v>332</v>
       </c>
       <c r="B150" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D150" s="4"/>
       <c r="E150" s="4" t="s">
@@ -13546,7 +13554,7 @@
         <v>294</v>
       </c>
       <c r="B153" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D153" s="4"/>
       <c r="E153" s="4" t="s">
@@ -13562,10 +13570,10 @@
     </row>
     <row r="154" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A154" s="28" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B154" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D154" s="4"/>
       <c r="E154" s="4" t="s">
@@ -13596,7 +13604,7 @@
     </row>
     <row r="156" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A156" s="8" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D156" s="4"/>
       <c r="E156" s="4" t="s">
@@ -13615,10 +13623,10 @@
         <v>273</v>
       </c>
       <c r="B157" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D157" s="4"/>
       <c r="E157" s="4" t="s">
@@ -13634,10 +13642,10 @@
     </row>
     <row r="158" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A158" s="8" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B158" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D158" s="4"/>
       <c r="E158" s="4" t="s">
@@ -13682,10 +13690,10 @@
         <v>308</v>
       </c>
       <c r="B161" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C161" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D161" s="4"/>
       <c r="E161" s="4" t="s">
@@ -13718,7 +13726,7 @@
         <v>317</v>
       </c>
       <c r="B163" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D163" s="4"/>
       <c r="E163" s="4" t="s">
@@ -13748,7 +13756,7 @@
         <v>363</v>
       </c>
       <c r="B165" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D165" s="10" t="s">
         <v>364</v>
@@ -13791,7 +13799,7 @@
     </row>
     <row r="168" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A168" s="28" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D168" s="4"/>
       <c r="E168" s="4" t="s">
@@ -13806,13 +13814,13 @@
     </row>
     <row r="169" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A169" s="28" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B169" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C169" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D169" s="4"/>
       <c r="E169" s="4" t="s">
@@ -13833,10 +13841,10 @@
         <v>390</v>
       </c>
       <c r="B170" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C170" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D170" s="4"/>
       <c r="E170" s="4" t="s">
@@ -13851,17 +13859,17 @@
     </row>
     <row r="171" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A171" s="28" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C171" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D171" s="4"/>
       <c r="E171" s="4" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F171" s="5" t="s">
         <v>9</v>
@@ -13929,7 +13937,7 @@
         <v>271</v>
       </c>
       <c r="B176" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>159</v>
@@ -14028,7 +14036,7 @@
         <v>311</v>
       </c>
       <c r="B183" s="25" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D183" s="4"/>
       <c r="E183" s="4" t="s">
@@ -14049,7 +14057,7 @@
         <v>265</v>
       </c>
       <c r="B184" s="25" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C184" t="s">
         <v>339</v>
@@ -14131,7 +14139,7 @@
         <v>174</v>
       </c>
       <c r="F190" s="5" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="G190" s="6" t="s">
         <v>7</v>
@@ -14143,7 +14151,7 @@
         <v>175</v>
       </c>
       <c r="F191" s="5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G191" s="6" t="s">
         <v>7</v>
@@ -14155,7 +14163,7 @@
         <v>176</v>
       </c>
       <c r="F192" s="5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G192" s="6" t="s">
         <v>7</v>
@@ -14175,7 +14183,7 @@
     </row>
     <row r="194" spans="1:8" s="15" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A194" s="31" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B194" s="27"/>
       <c r="D194" s="19" t="s">
@@ -14206,7 +14214,7 @@
         <v>180</v>
       </c>
       <c r="F196" s="5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G196" s="6" t="s">
         <v>7</v>
@@ -14272,7 +14280,7 @@
         <v>185</v>
       </c>
       <c r="F201" s="5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G201" s="6" t="s">
         <v>7</v>
@@ -14286,7 +14294,7 @@
         <v>185</v>
       </c>
       <c r="F202" s="5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G202" s="6" t="s">
         <v>7</v>
@@ -14298,7 +14306,7 @@
         <v>186</v>
       </c>
       <c r="F203" s="5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G203" s="6" t="s">
         <v>7</v>
@@ -14309,7 +14317,7 @@
         <v>330</v>
       </c>
       <c r="C204" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D204" s="4"/>
       <c r="E204" s="4" t="s">
@@ -14348,7 +14356,7 @@
     </row>
     <row r="207" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A207" s="28" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="D207" s="4"/>
       <c r="E207" s="4" t="s">
@@ -14366,10 +14374,10 @@
         <v>411</v>
       </c>
       <c r="B208" s="25" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C208" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D208" s="9" t="s">
         <v>260</v>
@@ -14386,17 +14394,17 @@
     </row>
     <row r="209" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A209" s="28" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B209" s="25" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C209" s="4" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D209" s="9"/>
       <c r="E209" s="4" t="s">
-        <v>191</v>
+        <v>554</v>
       </c>
       <c r="F209" s="5" t="s">
         <v>52</v>
@@ -14406,18 +14414,18 @@
       </c>
     </row>
     <row r="210" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A210" s="28" t="s">
-        <v>412</v>
+      <c r="A210" s="29" t="s">
+        <v>314</v>
       </c>
       <c r="B210" s="25" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C210" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="D210" s="9"/>
+        <v>424</v>
+      </c>
+      <c r="D210" s="4"/>
       <c r="E210" s="4" t="s">
-        <v>415</v>
+        <v>192</v>
       </c>
       <c r="F210" s="5" t="s">
         <v>52</v>
@@ -14427,18 +14435,18 @@
       </c>
     </row>
     <row r="211" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A211" s="29" t="s">
-        <v>314</v>
+      <c r="A211" s="28" t="s">
+        <v>315</v>
       </c>
       <c r="B211" s="25" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>427</v>
+        <v>506</v>
       </c>
       <c r="D211" s="4"/>
       <c r="E211" s="4" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F211" s="5" t="s">
         <v>52</v>
@@ -14448,18 +14456,9 @@
       </c>
     </row>
     <row r="212" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A212" s="28" t="s">
-        <v>315</v>
-      </c>
-      <c r="B212" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C212" s="4" t="s">
-        <v>509</v>
-      </c>
       <c r="D212" s="4"/>
       <c r="E212" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F212" s="5" t="s">
         <v>52</v>
@@ -14469,9 +14468,11 @@
       </c>
     </row>
     <row r="213" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="D213" s="4"/>
+      <c r="D213" s="9" t="s">
+        <v>261</v>
+      </c>
       <c r="E213" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F213" s="5" t="s">
         <v>52</v>
@@ -14481,11 +14482,18 @@
       </c>
     </row>
     <row r="214" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="D214" s="9" t="s">
-        <v>261</v>
-      </c>
+      <c r="A214" s="28" t="s">
+        <v>407</v>
+      </c>
+      <c r="B214" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="C214" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="D214" s="4"/>
       <c r="E214" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F214" s="5" t="s">
         <v>52</v>
@@ -14495,18 +14503,12 @@
       </c>
     </row>
     <row r="215" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A215" s="28" t="s">
-        <v>407</v>
-      </c>
-      <c r="B215" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C215" s="4" t="s">
-        <v>406</v>
+      <c r="A215" s="30" t="s">
+        <v>435</v>
       </c>
       <c r="D215" s="4"/>
       <c r="E215" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F215" s="5" t="s">
         <v>52</v>
@@ -14516,12 +14518,9 @@
       </c>
     </row>
     <row r="216" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A216" s="30" t="s">
-        <v>438</v>
-      </c>
       <c r="D216" s="4"/>
       <c r="E216" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F216" s="5" t="s">
         <v>52</v>
@@ -14533,10 +14532,10 @@
     <row r="217" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D217" s="4"/>
       <c r="E217" s="4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F217" s="5" t="s">
-        <v>52</v>
+        <v>464</v>
       </c>
       <c r="G217" s="6" t="s">
         <v>7</v>
@@ -14545,19 +14544,28 @@
     <row r="218" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D218" s="4"/>
       <c r="E218" s="4" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F218" s="5" t="s">
-        <v>467</v>
+        <v>52</v>
       </c>
       <c r="G218" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="219" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A219" s="28" t="s">
+        <v>414</v>
+      </c>
+      <c r="B219" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="C219" s="4" t="s">
+        <v>415</v>
+      </c>
       <c r="D219" s="4"/>
       <c r="E219" s="4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F219" s="5" t="s">
         <v>52</v>
@@ -14568,17 +14576,14 @@
     </row>
     <row r="220" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A220" s="28" t="s">
-        <v>417</v>
-      </c>
-      <c r="B220" s="25" t="s">
-        <v>434</v>
+        <v>281</v>
       </c>
       <c r="C220" s="4" t="s">
-        <v>418</v>
+        <v>515</v>
       </c>
       <c r="D220" s="4"/>
       <c r="E220" s="4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F220" s="5" t="s">
         <v>52</v>
@@ -14589,14 +14594,17 @@
     </row>
     <row r="221" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A221" s="28" t="s">
-        <v>281</v>
-      </c>
-      <c r="C221" s="4" t="s">
-        <v>518</v>
+        <v>280</v>
+      </c>
+      <c r="B221" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="C221" t="s">
+        <v>341</v>
       </c>
       <c r="D221" s="4"/>
       <c r="E221" s="4" t="s">
-        <v>202</v>
+        <v>342</v>
       </c>
       <c r="F221" s="5" t="s">
         <v>52</v>
@@ -14606,18 +14614,9 @@
       </c>
     </row>
     <row r="222" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A222" s="28" t="s">
-        <v>280</v>
-      </c>
-      <c r="B222" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C222" t="s">
-        <v>341</v>
-      </c>
       <c r="D222" s="4"/>
       <c r="E222" s="4" t="s">
-        <v>342</v>
+        <v>203</v>
       </c>
       <c r="F222" s="5" t="s">
         <v>52</v>
@@ -14629,7 +14628,7 @@
     <row r="223" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D223" s="4"/>
       <c r="E223" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F223" s="5" t="s">
         <v>52</v>
@@ -14639,9 +14638,18 @@
       </c>
     </row>
     <row r="224" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A224" s="28" t="s">
+        <v>417</v>
+      </c>
+      <c r="B224" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="C224" s="4" t="s">
+        <v>418</v>
+      </c>
       <c r="D224" s="4"/>
       <c r="E224" s="4" t="s">
-        <v>204</v>
+        <v>416</v>
       </c>
       <c r="F224" s="5" t="s">
         <v>52</v>
@@ -14652,17 +14660,17 @@
     </row>
     <row r="225" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A225" s="28" t="s">
+        <v>419</v>
+      </c>
+      <c r="B225" s="25" t="s">
+        <v>431</v>
+      </c>
+      <c r="C225" s="4" t="s">
         <v>420</v>
-      </c>
-      <c r="B225" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C225" s="4" t="s">
-        <v>421</v>
       </c>
       <c r="D225" s="4"/>
       <c r="E225" s="4" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="F225" s="5" t="s">
         <v>52</v>
@@ -14673,17 +14681,19 @@
     </row>
     <row r="226" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A226" s="28" t="s">
-        <v>422</v>
+        <v>278</v>
       </c>
       <c r="B226" s="25" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>423</v>
-      </c>
-      <c r="D226" s="4"/>
+        <v>405</v>
+      </c>
+      <c r="D226" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="E226" s="4" t="s">
-        <v>424</v>
+        <v>205</v>
       </c>
       <c r="F226" s="5" t="s">
         <v>52</v>
@@ -14691,22 +14701,23 @@
       <c r="G226" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="H226" s="13" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="227" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A227" s="28" t="s">
-        <v>278</v>
+        <v>469</v>
       </c>
       <c r="B227" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C227" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="D227" s="10" t="s">
-        <v>279</v>
-      </c>
+        <v>431</v>
+      </c>
+      <c r="C227" t="s">
+        <v>470</v>
+      </c>
+      <c r="D227" s="10"/>
       <c r="E227" s="4" t="s">
-        <v>205</v>
+        <v>470</v>
       </c>
       <c r="F227" s="5" t="s">
         <v>52</v>
@@ -14715,22 +14726,13 @@
         <v>7</v>
       </c>
       <c r="H227" s="13" t="s">
-        <v>313</v>
+        <v>553</v>
       </c>
     </row>
     <row r="228" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A228" s="28" t="s">
-        <v>472</v>
-      </c>
-      <c r="B228" s="25" t="s">
-        <v>434</v>
-      </c>
-      <c r="C228" t="s">
-        <v>473</v>
-      </c>
-      <c r="D228" s="10"/>
+      <c r="D228" s="4"/>
       <c r="E228" s="4" t="s">
-        <v>473</v>
+        <v>206</v>
       </c>
       <c r="F228" s="5" t="s">
         <v>52</v>
@@ -14742,7 +14744,7 @@
     <row r="229" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D229" s="4"/>
       <c r="E229" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F229" s="5" t="s">
         <v>52</v>
@@ -14752,51 +14754,54 @@
       </c>
     </row>
     <row r="230" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="D230" s="4"/>
+      <c r="D230" s="9" t="s">
+        <v>262</v>
+      </c>
       <c r="E230" s="4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F230" s="5" t="s">
-        <v>52</v>
+        <v>209</v>
       </c>
       <c r="G230" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="H230"/>
     </row>
     <row r="231" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D231" s="9" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E231" s="4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F231" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="G231" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H231"/>
+    </row>
+    <row r="232" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="D232" s="4"/>
+      <c r="E232" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F232" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="G231" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H231"/>
-    </row>
-    <row r="232" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="D232" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="E232" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="F232" s="5" t="s">
-        <v>467</v>
-      </c>
       <c r="G232" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H232"/>
     </row>
     <row r="233" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="D233" s="4"/>
+      <c r="D233" s="9" t="s">
+        <v>264</v>
+      </c>
       <c r="E233" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F233" s="5" t="s">
         <v>209</v>
@@ -14807,14 +14812,21 @@
       <c r="H233"/>
     </row>
     <row r="234" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="D234" s="9" t="s">
-        <v>264</v>
-      </c>
+      <c r="A234" s="28" t="s">
+        <v>296</v>
+      </c>
+      <c r="B234" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="C234" t="s">
+        <v>439</v>
+      </c>
+      <c r="D234" s="4"/>
       <c r="E234" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F234" s="5" t="s">
-        <v>209</v>
+        <v>463</v>
       </c>
       <c r="G234" s="6" t="s">
         <v>7</v>
@@ -14822,21 +14834,12 @@
       <c r="H234"/>
     </row>
     <row r="235" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A235" s="28" t="s">
-        <v>296</v>
-      </c>
-      <c r="B235" s="25" t="s">
-        <v>432</v>
-      </c>
-      <c r="C235" t="s">
-        <v>442</v>
-      </c>
       <c r="D235" s="4"/>
       <c r="E235" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F235" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G235" s="6" t="s">
         <v>7</v>
@@ -14846,10 +14849,10 @@
     <row r="236" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D236" s="4"/>
       <c r="E236" s="4" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F236" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G236" s="6" t="s">
         <v>7</v>
@@ -14857,12 +14860,15 @@
       <c r="H236"/>
     </row>
     <row r="237" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A237" s="28" t="s">
+        <v>436</v>
+      </c>
       <c r="D237" s="4"/>
       <c r="E237" s="4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F237" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G237" s="6" t="s">
         <v>7</v>
@@ -14871,14 +14877,14 @@
     </row>
     <row r="238" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A238" s="28" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D238" s="4"/>
       <c r="E238" s="4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F238" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G238" s="6" t="s">
         <v>7</v>
@@ -14886,15 +14892,12 @@
       <c r="H238"/>
     </row>
     <row r="239" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A239" s="28" t="s">
-        <v>440</v>
-      </c>
       <c r="D239" s="4"/>
       <c r="E239" s="4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F239" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G239" s="6" t="s">
         <v>7</v>
@@ -14904,10 +14907,10 @@
     <row r="240" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D240" s="4"/>
       <c r="E240" s="4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F240" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G240" s="6" t="s">
         <v>7</v>
@@ -14915,12 +14918,21 @@
       <c r="H240"/>
     </row>
     <row r="241" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A241" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="B241" s="25" t="s">
+        <v>429</v>
+      </c>
+      <c r="C241" t="s">
+        <v>472</v>
+      </c>
       <c r="D241" s="4"/>
       <c r="E241" s="4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F241" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G241" s="6" t="s">
         <v>7</v>
@@ -14928,21 +14940,12 @@
       <c r="H241"/>
     </row>
     <row r="242" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A242" s="28" t="s">
-        <v>474</v>
-      </c>
-      <c r="B242" s="25" t="s">
-        <v>432</v>
-      </c>
-      <c r="C242" t="s">
-        <v>475</v>
-      </c>
       <c r="D242" s="4"/>
       <c r="E242" s="4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F242" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G242" s="6" t="s">
         <v>7</v>
@@ -14952,10 +14955,10 @@
     <row r="243" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D243" s="4"/>
       <c r="E243" s="4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F243" s="5" t="s">
-        <v>466</v>
+        <v>223</v>
       </c>
       <c r="G243" s="6" t="s">
         <v>7</v>
@@ -14965,10 +14968,10 @@
     <row r="244" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D244" s="4"/>
       <c r="E244" s="4" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F244" s="5" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G244" s="6" t="s">
         <v>7</v>
@@ -14978,10 +14981,10 @@
     <row r="245" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D245" s="4"/>
       <c r="E245" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F245" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G245" s="6" t="s">
         <v>7</v>
@@ -14991,10 +14994,10 @@
     <row r="246" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D246" s="4"/>
       <c r="E246" s="4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F246" s="5" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="G246" s="6" t="s">
         <v>7</v>
@@ -15004,7 +15007,7 @@
     <row r="247" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D247" s="4"/>
       <c r="E247" s="4" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F247" s="5" t="s">
         <v>228</v>
@@ -15017,28 +15020,15 @@
     <row r="248" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D248" s="4"/>
       <c r="E248" s="4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F248" s="5" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="G248" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H248"/>
-    </row>
-    <row r="249" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="D249" s="4"/>
-      <c r="E249" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="F249" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="G249" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H249"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J162">
@@ -15046,12 +15036,12 @@
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D211:XFD211 D127:XFD127 A194:C194 F194:XFD194 A195:XFD208 A123:A126 C123:XFD126 A128:A137 C128:XFD137 A159:XFD160 A162:XFD162 A161 C161:XFD161 A163 C163:XFD163 A164:XFD168 A169 A185:XFD193 A183:A184 C183:XFD184 A209:A210 C209:XFD210 A236:XFD241 A235 C235:XFD235 A157:A158 C157:XFD158 A138:XFD156 A229:XFD234 A228:B228 D228:XFD228 A243:XFD1048576 A242 C242:XFD242 A170:XFD182 C169:XFD169 A1:XFD107 A212:XFD227 A109:XFD122">
-    <cfRule type="expression" dxfId="14" priority="15">
+  <conditionalFormatting sqref="D210:XFD210 D127:XFD127 A194:C194 F194:XFD194 A195:XFD208 A123:A126 C123:XFD126 A128:A137 C128:XFD137 A159:XFD160 A162:XFD162 A161 C161:XFD161 A163 C163:XFD163 A164:XFD168 A169 A185:XFD193 A183:A184 C183:XFD184 A209 C209:XFD209 A235:XFD240 A234 C234:XFD234 A157:A158 C157:XFD158 A228:XFD233 A227:B227 D227:XFD227 A242:XFD1048576 A241 C241:XFD241 A170:XFD182 C169:XFD169 A1:XFD107 A211:XFD226 A109:XFD122 B209:B210 A138:XFD156">
+    <cfRule type="expression" dxfId="0" priority="15">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C211">
+  <conditionalFormatting sqref="C210">
     <cfRule type="expression" dxfId="13" priority="14">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
@@ -15091,33 +15081,28 @@
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B209:B211">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B235">
-    <cfRule type="expression" dxfId="4" priority="5">
+  <conditionalFormatting sqref="B234">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B158">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B242">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="B241">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B108">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D108:XFD108">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated GUI to include impact of applying extra organic waste - not finished!
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25EABE3-64CF-4BB4-9C31-D877D710E094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F298A2CF-BF0D-4EF2-9B96-6B885ECBFD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1965" yWindow="1860" windowWidth="25155" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="4680" windowWidth="25155" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -10918,8 +10918,8 @@
   <dimension ref="A1:H251"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E76" sqref="E76"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>

</xml_diff>

<commit_message>
Changed formatting of econ data so it can be read by GUI graph constructor
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F298A2CF-BF0D-4EF2-9B96-6B885ECBFD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369ABC0F-B389-46F1-8B2F-A712DB5BBE8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="4680" windowWidth="25155" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43215" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="587">
   <si>
     <t>PyOrator variable</t>
   </si>
@@ -2611,6 +2611,21 @@
   </si>
   <si>
     <t>Total milk for typical year</t>
+  </si>
+  <si>
+    <t>full_hh_income_n_lim</t>
+  </si>
+  <si>
+    <t>economics</t>
+  </si>
+  <si>
+    <t>ETB</t>
+  </si>
+  <si>
+    <t>Ful household income of farm, crop growth limited by N availability</t>
+  </si>
+  <si>
+    <t>Full household income N Limited</t>
   </si>
 </sst>
 </file>
@@ -10915,11 +10930,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H251"/>
+  <dimension ref="A1:H252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C252" sqref="C252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -15278,79 +15293,99 @@
       </c>
       <c r="H251"/>
     </row>
+    <row r="252" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A252" s="28" t="s">
+        <v>582</v>
+      </c>
+      <c r="B252" s="25" t="s">
+        <v>583</v>
+      </c>
+      <c r="C252" t="s">
+        <v>586</v>
+      </c>
+      <c r="E252" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="F252" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="G252" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="J165">
     <cfRule type="expression" priority="16">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D213:XFD213 D130:XFD130 A197:C197 F197:XFD197 A198:XFD211 A126:A129 C126:XFD129 A131:A140 C131:XFD140 A162:XFD163 A165:XFD165 A164 C164:XFD164 A166 C166:XFD166 A167:XFD171 A172 A188:XFD196 A186:A187 C186:XFD187 A212 C212:XFD212 A238:XFD243 A237 C237:XFD237 A160:A161 C160:XFD161 A231:XFD236 A230:B230 D230:XFD230 A244 C244:XFD244 A173:XFD185 C172:XFD172 A214:XFD229 A112:XFD125 B212:B213 A141:XFD159 A245:XFD251 A253:XFD1048576 B252:XFD252 A1:XFD110">
-    <cfRule type="expression" dxfId="0" priority="15">
+  <conditionalFormatting sqref="D213:XFD213 D130:XFD130 A197:C197 F197:XFD197 A198:XFD211 A126:A129 C126:XFD129 A131:A140 C131:XFD140 A162:XFD163 A165:XFD165 A164 C164:XFD164 A166 C166:XFD166 A167:XFD171 A172 A188:XFD196 A186:A187 C186:XFD187 A212 C212:XFD212 A238:XFD243 A237 C237:XFD237 A160:A161 C160:XFD161 A231:XFD236 A230:B230 D230:XFD230 A244 C244:XFD244 A173:XFD185 C172:XFD172 A214:XFD229 A112:XFD125 B212:B213 A141:XFD159 A245:XFD251 A253:XFD1048576 A1:XFD110 B252:XFD252">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C213">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B126:B140">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B160">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B164">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B166">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B172">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B187">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B186">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B237">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B161">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B244">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B111">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D111:XFD111">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Collapse livestock data to whole farm rather than by subarea
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369ABC0F-B389-46F1-8B2F-A712DB5BBE8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5FA76A-8E19-4628-B4B6-8E05AFB15979}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43215" yWindow="1245" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="593">
   <si>
     <t>PyOrator variable</t>
   </si>
@@ -2622,10 +2622,28 @@
     <t>ETB</t>
   </si>
   <si>
-    <t>Ful household income of farm, crop growth limited by N availability</t>
-  </si>
-  <si>
-    <t>Full household income N Limited</t>
+    <t>full_hh_income_zaks</t>
+  </si>
+  <si>
+    <t>full_hh_income_miami</t>
+  </si>
+  <si>
+    <t>Full household income (N Limited)</t>
+  </si>
+  <si>
+    <t>Full household income (Zaks)</t>
+  </si>
+  <si>
+    <t>Full household income (Miami)</t>
+  </si>
+  <si>
+    <t>Full household income of farm, crop growth limited by N availability</t>
+  </si>
+  <si>
+    <t>Full household income of farm, crop growth calcualted using Zaks</t>
+  </si>
+  <si>
+    <t>Full household income of farm, crop growth calculated using Miami</t>
   </si>
 </sst>
 </file>
@@ -10930,27 +10948,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H252"/>
+  <dimension ref="A1:H254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C252" sqref="C252"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G252" sqref="G252:G254"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="20.149999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="28" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" style="28" customWidth="1"/>
     <col min="2" max="2" width="15" style="25" customWidth="1"/>
-    <col min="3" max="3" width="35.140625" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.1796875" customWidth="1"/>
+    <col min="4" max="4" width="30.26953125" customWidth="1"/>
     <col min="5" max="5" width="120" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="64.5703125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="19.1796875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="64.54296875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10976,7 +10994,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
         <v>5</v>
@@ -10988,7 +11006,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A3" s="28" t="s">
         <v>277</v>
       </c>
@@ -11006,7 +11024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
         <v>10</v>
@@ -11018,7 +11036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
         <v>11</v>
@@ -11030,7 +11048,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
         <v>12</v>
@@ -11042,7 +11060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A7" s="28" t="s">
         <v>470</v>
       </c>
@@ -11063,7 +11081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A8" s="28" t="s">
         <v>333</v>
       </c>
@@ -11081,7 +11099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A9" s="28" t="s">
         <v>332</v>
       </c>
@@ -11099,7 +11117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A10" s="28" t="s">
         <v>334</v>
       </c>
@@ -11117,7 +11135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A11" s="28" t="s">
         <v>268</v>
       </c>
@@ -11138,7 +11156,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A12" s="28" t="s">
         <v>329</v>
       </c>
@@ -11156,7 +11174,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A13" s="28" t="s">
         <v>368</v>
       </c>
@@ -11179,7 +11197,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A14" s="28" t="s">
         <v>372</v>
       </c>
@@ -11202,7 +11220,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A15" s="28" t="s">
         <v>378</v>
       </c>
@@ -11225,7 +11243,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A16" s="28" t="s">
         <v>380</v>
       </c>
@@ -11248,7 +11266,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A17" s="28" t="s">
         <v>267</v>
       </c>
@@ -11269,7 +11287,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
         <v>20</v>
@@ -11281,7 +11299,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A19" s="28" t="s">
         <v>505</v>
       </c>
@@ -11299,7 +11317,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A20" s="28" t="s">
         <v>506</v>
       </c>
@@ -11317,7 +11335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="20" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:8" s="20" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="B21" s="26"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9" t="s">
@@ -11331,7 +11349,7 @@
       </c>
       <c r="H21" s="21"/>
     </row>
-    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
         <v>22</v>
@@ -11343,7 +11361,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="23" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
         <v>23</v>
@@ -11355,7 +11373,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
         <v>24</v>
@@ -11367,7 +11385,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="25" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A25" s="28" t="s">
         <v>25</v>
       </c>
@@ -11388,7 +11406,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="26" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A26" s="28" t="s">
         <v>27</v>
       </c>
@@ -11409,7 +11427,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="27" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A27" s="28" t="s">
         <v>29</v>
       </c>
@@ -11430,7 +11448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="28" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A28" s="28" t="s">
         <v>318</v>
       </c>
@@ -11451,7 +11469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="29" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
         <v>32</v>
@@ -11463,7 +11481,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="30" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D30" s="7" t="s">
         <v>33</v>
       </c>
@@ -11477,7 +11495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="31" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D31" s="7" t="s">
         <v>232</v>
       </c>
@@ -11491,7 +11509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="32" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
         <v>36</v>
@@ -11503,7 +11521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="33" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
         <v>37</v>
@@ -11515,7 +11533,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="34" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A34" s="28" t="s">
         <v>319</v>
       </c>
@@ -11536,7 +11554,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="35" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A35" s="28" t="s">
         <v>320</v>
       </c>
@@ -11557,7 +11575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="36" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A36" s="28" t="s">
         <v>266</v>
       </c>
@@ -11578,7 +11596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="37" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="D37" s="7" t="s">
         <v>233</v>
       </c>
@@ -11592,7 +11610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="38" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="D38" s="7" t="s">
         <v>234</v>
       </c>
@@ -11606,7 +11624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="39" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
         <v>43</v>
@@ -11618,7 +11636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="40" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A40" s="28" t="s">
         <v>383</v>
       </c>
@@ -11639,7 +11657,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A41" s="28" t="s">
         <v>448</v>
       </c>
@@ -11660,7 +11678,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="42" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A42" s="28" t="s">
         <v>384</v>
       </c>
@@ -11681,7 +11699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="B43" s="25" t="s">
         <v>427</v>
       </c>
@@ -11696,7 +11714,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="44" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A44" s="28" t="s">
         <v>343</v>
       </c>
@@ -11717,7 +11735,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="45" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A45" s="28" t="s">
         <v>344</v>
       </c>
@@ -11738,7 +11756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="46" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A46" s="28" t="s">
         <v>345</v>
       </c>
@@ -11759,7 +11777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="47" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A47" s="28" t="s">
         <v>350</v>
       </c>
@@ -11780,7 +11798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="48" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A48" s="28" t="s">
         <v>323</v>
       </c>
@@ -11801,7 +11819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="49" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A49" s="28" t="s">
         <v>514</v>
       </c>
@@ -11815,7 +11833,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="50" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="B50" s="25" t="s">
         <v>562</v>
       </c>
@@ -11830,7 +11848,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="51" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A51" s="36" t="s">
         <v>561</v>
       </c>
@@ -11851,7 +11869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="52" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A52" s="28" t="s">
         <v>563</v>
       </c>
@@ -11872,13 +11890,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="53" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="54" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
         <v>48</v>
@@ -11890,7 +11908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="55" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A55" s="28" t="s">
         <v>451</v>
       </c>
@@ -11908,7 +11926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="56" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
         <v>51</v>
@@ -11920,7 +11938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="57" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
         <v>53</v>
@@ -11932,7 +11950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="58" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
         <v>55</v>
@@ -11944,7 +11962,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="59" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
         <v>56</v>
@@ -11956,7 +11974,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="60" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
         <v>57</v>
@@ -11968,7 +11986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="61" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A61" s="28" t="s">
         <v>322</v>
       </c>
@@ -11989,7 +12007,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="62" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A62" s="28" t="s">
         <v>321</v>
       </c>
@@ -12010,7 +12028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="63" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D63" s="10" t="s">
         <v>359</v>
       </c>
@@ -12024,7 +12042,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="20" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="64" spans="1:8" s="20" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="B64" s="26"/>
       <c r="D64" s="9"/>
       <c r="E64" s="22" t="s">
@@ -12038,7 +12056,7 @@
       </c>
       <c r="H64" s="21"/>
     </row>
-    <row r="65" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="65" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A65" s="28" t="s">
         <v>445</v>
       </c>
@@ -12059,7 +12077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="66" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A66" s="28" t="s">
         <v>444</v>
       </c>
@@ -12074,7 +12092,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="67" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
         <v>64</v>
@@ -12086,7 +12104,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="68" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
         <v>65</v>
@@ -12098,7 +12116,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="69" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
         <v>66</v>
@@ -12110,7 +12128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="70" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A70" s="28" t="s">
         <v>301</v>
       </c>
@@ -12134,7 +12152,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="71" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A71" s="32" t="s">
         <v>298</v>
       </c>
@@ -12158,7 +12176,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="72" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A72" s="28" t="s">
         <v>297</v>
       </c>
@@ -12182,7 +12200,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="73" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="B73" s="25" t="s">
         <v>562</v>
       </c>
@@ -12197,7 +12215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="74" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="B74" s="25" t="s">
         <v>562</v>
       </c>
@@ -12212,7 +12230,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="75" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="B75" s="25" t="s">
         <v>575</v>
       </c>
@@ -12229,7 +12247,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="76" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A76" t="s">
         <v>569</v>
       </c>
@@ -12252,7 +12270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="77" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A77" t="s">
         <v>570</v>
       </c>
@@ -12275,7 +12293,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="78" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A78"/>
       <c r="B78" s="25" t="s">
         <v>575</v>
@@ -12294,7 +12312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="79" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A79" t="s">
         <v>567</v>
       </c>
@@ -12317,7 +12335,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="80" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A80" t="s">
         <v>568</v>
       </c>
@@ -12340,7 +12358,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="81" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A81"/>
       <c r="B81" s="25" t="s">
         <v>575</v>
@@ -12357,7 +12375,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="82" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A82" t="s">
         <v>565</v>
       </c>
@@ -12380,7 +12398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="83" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A83" t="s">
         <v>566</v>
       </c>
@@ -12403,7 +12421,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="84" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
         <v>82</v>
@@ -12415,7 +12433,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="85" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D85" s="9" t="s">
         <v>243</v>
       </c>
@@ -12429,7 +12447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="86" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
         <v>84</v>
@@ -12441,7 +12459,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="87" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
         <v>85</v>
@@ -12453,7 +12471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="88" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
         <v>86</v>
@@ -12465,7 +12483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="89" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D89" s="9" t="s">
         <v>244</v>
       </c>
@@ -12479,7 +12497,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="90" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
         <v>88</v>
@@ -12491,7 +12509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="91" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A91" s="28" t="s">
         <v>282</v>
       </c>
@@ -12512,7 +12530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="92" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A92" s="28" t="s">
         <v>554</v>
       </c>
@@ -12536,7 +12554,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="93" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A93" s="28" t="s">
         <v>430</v>
       </c>
@@ -12557,7 +12575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="94" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A94" s="28" t="s">
         <v>481</v>
       </c>
@@ -12578,7 +12596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="95" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A95" s="28" t="s">
         <v>303</v>
       </c>
@@ -12596,7 +12614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="96" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A96" s="28" t="s">
         <v>440</v>
       </c>
@@ -12620,7 +12638,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="97" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A97" s="28" t="s">
         <v>486</v>
       </c>
@@ -12644,7 +12662,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="98" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A98" s="28" t="s">
         <v>441</v>
       </c>
@@ -12668,7 +12686,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="99" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A99" s="28" t="s">
         <v>471</v>
       </c>
@@ -12692,7 +12710,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="100" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D100" s="9" t="s">
         <v>245</v>
       </c>
@@ -12706,7 +12724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="101" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A101" t="s">
         <v>571</v>
       </c>
@@ -12729,7 +12747,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="102" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A102" t="s">
         <v>572</v>
       </c>
@@ -12752,7 +12770,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="103" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A103" s="28" t="s">
         <v>551</v>
       </c>
@@ -12773,7 +12791,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="104" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A104" s="28" t="s">
         <v>559</v>
       </c>
@@ -12794,7 +12812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="105" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A105" s="28" t="s">
         <v>560</v>
       </c>
@@ -12815,7 +12833,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="106" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A106" s="28" t="s">
         <v>490</v>
       </c>
@@ -12836,7 +12854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="107" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A107" s="28" t="s">
         <v>284</v>
       </c>
@@ -12857,7 +12875,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="108" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A108" s="28" t="s">
         <v>557</v>
       </c>
@@ -12878,7 +12896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="109" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A109" s="28" t="s">
         <v>457</v>
       </c>
@@ -12899,7 +12917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="110" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A110" s="28" t="s">
         <v>287</v>
       </c>
@@ -12922,7 +12940,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="111" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A111" s="28" t="s">
         <v>324</v>
       </c>
@@ -12946,7 +12964,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="112" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A112" s="28" t="s">
         <v>406</v>
       </c>
@@ -12967,7 +12985,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="113" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A113" s="28" t="s">
         <v>410</v>
       </c>
@@ -12988,7 +13006,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="114" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A114" s="28" t="s">
         <v>498</v>
       </c>
@@ -13011,7 +13029,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="115" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A115" s="28" t="s">
         <v>325</v>
       </c>
@@ -13029,7 +13047,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="116" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A116" s="28" t="s">
         <v>288</v>
       </c>
@@ -13052,7 +13070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="117" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A117" s="28" t="s">
         <v>290</v>
       </c>
@@ -13073,7 +13091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="118" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A118" s="28" t="s">
         <v>511</v>
       </c>
@@ -13094,7 +13112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="119" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A119" s="28" t="s">
         <v>398</v>
       </c>
@@ -13115,7 +13133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="120" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A120" s="28" t="s">
         <v>399</v>
       </c>
@@ -13136,7 +13154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="121" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A121" s="28" t="s">
         <v>289</v>
       </c>
@@ -13160,7 +13178,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="122" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A122" s="28" t="s">
         <v>405</v>
       </c>
@@ -13184,7 +13202,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="123" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A123" s="28" t="s">
         <v>472</v>
       </c>
@@ -13205,7 +13223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="124" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A124" s="28" t="s">
         <v>495</v>
       </c>
@@ -13226,7 +13244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="125" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A125" s="28" t="s">
         <v>491</v>
       </c>
@@ -13247,7 +13265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="126" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A126" s="28" t="s">
         <v>283</v>
       </c>
@@ -13268,7 +13286,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="127" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A127" s="28" t="s">
         <v>558</v>
       </c>
@@ -13289,7 +13307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="128" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A128" s="28" t="s">
         <v>456</v>
       </c>
@@ -13310,7 +13328,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="129" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A129" s="28" t="s">
         <v>275</v>
       </c>
@@ -13333,7 +13351,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="130" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A130" s="28" t="s">
         <v>327</v>
       </c>
@@ -13357,7 +13375,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="131" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A131" s="28" t="s">
         <v>276</v>
       </c>
@@ -13380,7 +13398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="132" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A132" s="28" t="s">
         <v>389</v>
       </c>
@@ -13401,7 +13419,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="133" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A133" s="28" t="s">
         <v>326</v>
       </c>
@@ -13422,7 +13440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="134" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A134" s="28" t="s">
         <v>393</v>
       </c>
@@ -13443,7 +13461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="135" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A135" s="28" t="s">
         <v>325</v>
       </c>
@@ -13461,7 +13479,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="136" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A136" s="28" t="s">
         <v>274</v>
       </c>
@@ -13482,7 +13500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="137" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A137" s="28" t="s">
         <v>286</v>
       </c>
@@ -13503,7 +13521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="138" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A138" s="28" t="s">
         <v>396</v>
       </c>
@@ -13524,7 +13542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="139" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A139" s="28" t="s">
         <v>285</v>
       </c>
@@ -13545,7 +13563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:8" s="8" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="140" spans="1:8" s="8" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A140" s="30" t="s">
         <v>387</v>
       </c>
@@ -13567,7 +13585,7 @@
       </c>
       <c r="H140" s="14"/>
     </row>
-    <row r="141" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="141" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A141" s="28" t="s">
         <v>295</v>
       </c>
@@ -13585,7 +13603,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="142" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A142" s="28" t="s">
         <v>452</v>
       </c>
@@ -13603,7 +13621,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="143" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D143" s="9" t="s">
         <v>251</v>
       </c>
@@ -13617,7 +13635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="144" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A144" s="28" t="s">
         <v>458</v>
       </c>
@@ -13635,7 +13653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="145" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D145" s="9" t="s">
         <v>252</v>
       </c>
@@ -13649,7 +13667,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="146" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A146" s="28" t="s">
         <v>459</v>
       </c>
@@ -13667,7 +13685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="147" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D147" s="9" t="s">
         <v>253</v>
       </c>
@@ -13681,7 +13699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="148" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D148" s="4"/>
       <c r="E148" s="4" t="s">
         <v>127</v>
@@ -13694,7 +13712,7 @@
       </c>
       <c r="H148"/>
     </row>
-    <row r="149" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="149" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
         <v>128</v>
@@ -13707,7 +13725,7 @@
       </c>
       <c r="H149"/>
     </row>
-    <row r="150" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="150" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D150" s="4"/>
       <c r="E150" s="4" t="s">
         <v>129</v>
@@ -13720,7 +13738,7 @@
       </c>
       <c r="H150"/>
     </row>
-    <row r="151" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="151" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A151" s="28" t="s">
         <v>293</v>
       </c>
@@ -13742,7 +13760,7 @@
       </c>
       <c r="H151"/>
     </row>
-    <row r="152" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="152" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A152" s="28" t="s">
         <v>331</v>
       </c>
@@ -13761,7 +13779,7 @@
       </c>
       <c r="H152"/>
     </row>
-    <row r="153" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="153" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A153" s="28" t="s">
         <v>330</v>
       </c>
@@ -13780,7 +13798,7 @@
       </c>
       <c r="H153"/>
     </row>
-    <row r="154" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="154" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D154" s="4"/>
       <c r="E154" s="4" t="s">
         <v>133</v>
@@ -13793,7 +13811,7 @@
       </c>
       <c r="H154"/>
     </row>
-    <row r="155" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="155" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D155" s="4"/>
       <c r="E155" s="4" t="s">
         <v>134</v>
@@ -13806,7 +13824,7 @@
       </c>
       <c r="H155"/>
     </row>
-    <row r="156" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="156" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A156" s="28" t="s">
         <v>294</v>
       </c>
@@ -13825,7 +13843,7 @@
       </c>
       <c r="H156"/>
     </row>
-    <row r="157" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="157" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A157" s="28" t="s">
         <v>546</v>
       </c>
@@ -13844,7 +13862,7 @@
       </c>
       <c r="H157"/>
     </row>
-    <row r="158" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="158" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D158" s="9" t="s">
         <v>254</v>
       </c>
@@ -13859,7 +13877,7 @@
       </c>
       <c r="H158"/>
     </row>
-    <row r="159" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="159" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A159" s="8" t="s">
         <v>443</v>
       </c>
@@ -13875,7 +13893,7 @@
       </c>
       <c r="H159"/>
     </row>
-    <row r="160" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="160" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A160" s="28" t="s">
         <v>273</v>
       </c>
@@ -13897,7 +13915,7 @@
       </c>
       <c r="H160"/>
     </row>
-    <row r="161" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="161" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A161" s="8" t="s">
         <v>442</v>
       </c>
@@ -13916,7 +13934,7 @@
       </c>
       <c r="H161"/>
     </row>
-    <row r="162" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="162" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D162" s="4"/>
       <c r="E162" s="4" t="s">
         <v>141</v>
@@ -13929,7 +13947,7 @@
       </c>
       <c r="H162"/>
     </row>
-    <row r="163" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="163" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D163" s="4"/>
       <c r="E163" s="4" t="s">
         <v>142</v>
@@ -13942,7 +13960,7 @@
       </c>
       <c r="H163"/>
     </row>
-    <row r="164" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="164" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A164" s="28" t="s">
         <v>308</v>
       </c>
@@ -13966,7 +13984,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="165" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D165" s="4"/>
       <c r="E165" s="4" t="s">
         <v>144</v>
@@ -13978,7 +13996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="166" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A166" s="28" t="s">
         <v>317</v>
       </c>
@@ -13996,7 +14014,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="167" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D167" s="4"/>
       <c r="E167" s="4" t="s">
         <v>146</v>
@@ -14008,7 +14026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="168" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A168" s="28" t="s">
         <v>361</v>
       </c>
@@ -14028,7 +14046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="169" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D169" s="4"/>
       <c r="E169" s="4" t="s">
         <v>147</v>
@@ -14040,7 +14058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="170" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D170" s="9" t="s">
         <v>255</v>
       </c>
@@ -14054,7 +14072,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="171" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A171" s="28" t="s">
         <v>429</v>
       </c>
@@ -14069,7 +14087,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="172" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A172" s="28" t="s">
         <v>493</v>
       </c>
@@ -14093,7 +14111,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="173" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A173" s="28" t="s">
         <v>388</v>
       </c>
@@ -14114,7 +14132,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="174" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A174" s="28" t="s">
         <v>478</v>
       </c>
@@ -14135,7 +14153,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="175" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D175" s="4"/>
       <c r="E175" s="4" t="s">
         <v>152</v>
@@ -14150,7 +14168,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="176" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D176" s="4"/>
       <c r="E176" s="4" t="s">
         <v>153</v>
@@ -14162,7 +14180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="177" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A177" s="28" t="s">
         <v>272</v>
       </c>
@@ -14177,7 +14195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="178" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D178" s="4"/>
       <c r="E178" s="4" t="s">
         <v>157</v>
@@ -14189,7 +14207,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="179" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A179" s="28" t="s">
         <v>271</v>
       </c>
@@ -14210,7 +14228,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="180" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D180" s="4"/>
       <c r="E180" s="4" t="s">
         <v>160</v>
@@ -14222,7 +14240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="181" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D181" s="4"/>
       <c r="E181" s="4" t="s">
         <v>161</v>
@@ -14234,7 +14252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="182" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D182" s="4"/>
       <c r="E182" s="4" t="s">
         <v>162</v>
@@ -14246,7 +14264,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="183" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A183" s="28" t="s">
         <v>270</v>
       </c>
@@ -14261,7 +14279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="184" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A184" s="28" t="s">
         <v>269</v>
       </c>
@@ -14276,7 +14294,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="185" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D185" s="4"/>
       <c r="E185" s="4" t="s">
         <v>165</v>
@@ -14288,7 +14306,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="186" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A186" s="28" t="s">
         <v>311</v>
       </c>
@@ -14309,7 +14327,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="187" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A187" s="28" t="s">
         <v>265</v>
       </c>
@@ -14330,7 +14348,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="188" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D188" s="4"/>
       <c r="E188" s="4" t="s">
         <v>169</v>
@@ -14342,7 +14360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="189" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D189" s="4"/>
       <c r="E189" s="4" t="s">
         <v>170</v>
@@ -14354,7 +14372,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="190" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D190" s="4"/>
       <c r="E190" s="4" t="s">
         <v>171</v>
@@ -14366,7 +14384,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="191" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D191" s="4"/>
       <c r="E191" s="4" t="s">
         <v>172</v>
@@ -14378,7 +14396,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="192" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D192" s="4"/>
       <c r="E192" s="4" t="s">
         <v>173</v>
@@ -14390,7 +14408,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="193" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D193" s="4"/>
       <c r="E193" s="4" t="s">
         <v>174</v>
@@ -14402,7 +14420,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="194" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D194" s="4"/>
       <c r="E194" s="4" t="s">
         <v>175</v>
@@ -14414,7 +14432,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="195" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D195" s="4"/>
       <c r="E195" s="4" t="s">
         <v>176</v>
@@ -14426,7 +14444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="196" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D196" s="4"/>
       <c r="E196" s="4" t="s">
         <v>177</v>
@@ -14438,7 +14456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="197" spans="1:8" s="15" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="197" spans="1:8" s="15" customFormat="1" ht="20.149999999999999" customHeight="1">
       <c r="A197" s="31" t="s">
         <v>431</v>
       </c>
@@ -14453,7 +14471,7 @@
       <c r="G197" s="17"/>
       <c r="H197" s="18"/>
     </row>
-    <row r="198" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="198" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D198" s="4"/>
       <c r="E198" s="4" t="s">
         <v>179</v>
@@ -14465,7 +14483,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="199" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D199" s="4"/>
       <c r="E199" s="4" t="s">
         <v>180</v>
@@ -14477,7 +14495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="200" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D200" s="4"/>
       <c r="E200" s="4" t="s">
         <v>181</v>
@@ -14489,7 +14507,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="201" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D201" s="9" t="s">
         <v>256</v>
       </c>
@@ -14503,7 +14521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="202" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D202" s="9" t="s">
         <v>257</v>
       </c>
@@ -14517,7 +14535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="203" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D203" s="9" t="s">
         <v>258</v>
       </c>
@@ -14531,7 +14549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="204" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="204" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D204" s="4"/>
       <c r="E204" s="4" t="s">
         <v>185</v>
@@ -14543,7 +14561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="205" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D205" s="9" t="s">
         <v>259</v>
       </c>
@@ -14557,7 +14575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="206" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D206" s="4"/>
       <c r="E206" s="4" t="s">
         <v>186</v>
@@ -14569,7 +14587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="207" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A207" s="28" t="s">
         <v>328</v>
       </c>
@@ -14587,7 +14605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="208" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D208" s="4"/>
       <c r="E208" s="4" t="s">
         <v>189</v>
@@ -14599,7 +14617,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="209" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="D209" s="4"/>
       <c r="E209" s="4" t="s">
         <v>187</v>
@@ -14611,7 +14629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="210" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A210" s="28" t="s">
         <v>509</v>
       </c>
@@ -14632,7 +14650,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="211" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A211" s="28" t="s">
         <v>408</v>
       </c>
@@ -14655,7 +14673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="212" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A212" s="28" t="s">
         <v>419</v>
       </c>
@@ -14676,7 +14694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="213" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A213" s="29" t="s">
         <v>314</v>
       </c>
@@ -14697,7 +14715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="214" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A214" s="28" t="s">
         <v>315</v>
       </c>
@@ -14718,7 +14736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="215" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="D215" s="4"/>
       <c r="E215" s="4" t="s">
         <v>194</v>
@@ -14730,7 +14748,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="216" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="D216" s="9" t="s">
         <v>261</v>
       </c>
@@ -14744,7 +14762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="217" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A217" s="28" t="s">
         <v>404</v>
       </c>
@@ -14765,7 +14783,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="218" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A218" s="30" t="s">
         <v>432</v>
       </c>
@@ -14780,7 +14798,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="219" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="D219" s="4"/>
       <c r="E219" s="4" t="s">
         <v>198</v>
@@ -14792,7 +14810,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="220" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="D220" s="4"/>
       <c r="E220" s="4" t="s">
         <v>199</v>
@@ -14804,7 +14822,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="221" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="D221" s="4"/>
       <c r="E221" s="4" t="s">
         <v>200</v>
@@ -14816,7 +14834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="222" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A222" s="28" t="s">
         <v>411</v>
       </c>
@@ -14837,7 +14855,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="223" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A223" s="28" t="s">
         <v>281</v>
       </c>
@@ -14855,7 +14873,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="224" spans="1:7" ht="20.149999999999999" customHeight="1">
       <c r="A224" s="28" t="s">
         <v>280</v>
       </c>
@@ -14876,7 +14894,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="225" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D225" s="4"/>
       <c r="E225" s="4" t="s">
         <v>203</v>
@@ -14888,7 +14906,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="226" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D226" s="4"/>
       <c r="E226" s="4" t="s">
         <v>204</v>
@@ -14900,7 +14918,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="227" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A227" s="28" t="s">
         <v>414</v>
       </c>
@@ -14921,7 +14939,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="228" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A228" s="28" t="s">
         <v>416</v>
       </c>
@@ -14942,7 +14960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="229" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A229" s="28" t="s">
         <v>278</v>
       </c>
@@ -14968,7 +14986,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="230" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A230" s="28" t="s">
         <v>466</v>
       </c>
@@ -14992,7 +15010,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="231" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D231" s="4"/>
       <c r="E231" s="4" t="s">
         <v>206</v>
@@ -15004,7 +15022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="232" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D232" s="4"/>
       <c r="E232" s="4" t="s">
         <v>207</v>
@@ -15016,7 +15034,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="233" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D233" s="9" t="s">
         <v>262</v>
       </c>
@@ -15031,7 +15049,7 @@
       </c>
       <c r="H233"/>
     </row>
-    <row r="234" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="234" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D234" s="9" t="s">
         <v>263</v>
       </c>
@@ -15046,7 +15064,7 @@
       </c>
       <c r="H234"/>
     </row>
-    <row r="235" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="235" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D235" s="4"/>
       <c r="E235" s="4" t="s">
         <v>211</v>
@@ -15059,7 +15077,7 @@
       </c>
       <c r="H235"/>
     </row>
-    <row r="236" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="236" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D236" s="9" t="s">
         <v>264</v>
       </c>
@@ -15074,7 +15092,7 @@
       </c>
       <c r="H236"/>
     </row>
-    <row r="237" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="237" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A237" s="28" t="s">
         <v>296</v>
       </c>
@@ -15096,7 +15114,7 @@
       </c>
       <c r="H237"/>
     </row>
-    <row r="238" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="238" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D238" s="4"/>
       <c r="E238" s="4" t="s">
         <v>214</v>
@@ -15109,7 +15127,7 @@
       </c>
       <c r="H238"/>
     </row>
-    <row r="239" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="239" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D239" s="4"/>
       <c r="E239" s="4" t="s">
         <v>215</v>
@@ -15122,7 +15140,7 @@
       </c>
       <c r="H239"/>
     </row>
-    <row r="240" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="240" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A240" s="28" t="s">
         <v>433</v>
       </c>
@@ -15138,7 +15156,7 @@
       </c>
       <c r="H240"/>
     </row>
-    <row r="241" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="241" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A241" s="28" t="s">
         <v>434</v>
       </c>
@@ -15154,7 +15172,7 @@
       </c>
       <c r="H241"/>
     </row>
-    <row r="242" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="242" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D242" s="4"/>
       <c r="E242" s="4" t="s">
         <v>218</v>
@@ -15167,7 +15185,7 @@
       </c>
       <c r="H242"/>
     </row>
-    <row r="243" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="243" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D243" s="4"/>
       <c r="E243" s="4" t="s">
         <v>219</v>
@@ -15180,7 +15198,7 @@
       </c>
       <c r="H243"/>
     </row>
-    <row r="244" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="244" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A244" s="28" t="s">
         <v>468</v>
       </c>
@@ -15202,7 +15220,7 @@
       </c>
       <c r="H244"/>
     </row>
-    <row r="245" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="245" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D245" s="4"/>
       <c r="E245" s="4" t="s">
         <v>221</v>
@@ -15215,7 +15233,7 @@
       </c>
       <c r="H245"/>
     </row>
-    <row r="246" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="246" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D246" s="4"/>
       <c r="E246" s="4" t="s">
         <v>222</v>
@@ -15228,7 +15246,7 @@
       </c>
       <c r="H246"/>
     </row>
-    <row r="247" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="247" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D247" s="4"/>
       <c r="E247" s="4" t="s">
         <v>224</v>
@@ -15241,7 +15259,7 @@
       </c>
       <c r="H247"/>
     </row>
-    <row r="248" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="248" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D248" s="4"/>
       <c r="E248" s="4" t="s">
         <v>226</v>
@@ -15254,7 +15272,7 @@
       </c>
       <c r="H248"/>
     </row>
-    <row r="249" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="249" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D249" s="4"/>
       <c r="E249" s="4" t="s">
         <v>227</v>
@@ -15267,7 +15285,7 @@
       </c>
       <c r="H249"/>
     </row>
-    <row r="250" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="250" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D250" s="4"/>
       <c r="E250" s="4" t="s">
         <v>229</v>
@@ -15280,7 +15298,7 @@
       </c>
       <c r="H250"/>
     </row>
-    <row r="251" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="251" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="D251" s="4"/>
       <c r="E251" s="4" t="s">
         <v>230</v>
@@ -15293,7 +15311,7 @@
       </c>
       <c r="H251"/>
     </row>
-    <row r="252" spans="1:8" ht="20.100000000000001" customHeight="1">
+    <row r="252" spans="1:8" ht="20.149999999999999" customHeight="1">
       <c r="A252" s="28" t="s">
         <v>582</v>
       </c>
@@ -15301,15 +15319,55 @@
         <v>583</v>
       </c>
       <c r="C252" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="E252" s="4" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="F252" s="5" t="s">
         <v>584</v>
       </c>
       <c r="G252" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" ht="20.149999999999999" customHeight="1">
+      <c r="A253" s="28" t="s">
+        <v>585</v>
+      </c>
+      <c r="B253" s="25" t="s">
+        <v>583</v>
+      </c>
+      <c r="C253" t="s">
+        <v>588</v>
+      </c>
+      <c r="E253" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="F253" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="G253" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" ht="20.149999999999999" customHeight="1">
+      <c r="A254" s="28" t="s">
+        <v>586</v>
+      </c>
+      <c r="B254" s="25" t="s">
+        <v>583</v>
+      </c>
+      <c r="C254" t="s">
+        <v>589</v>
+      </c>
+      <c r="E254" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="F254" s="5" t="s">
+        <v>584</v>
+      </c>
+      <c r="G254" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -15319,7 +15377,7 @@
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D213:XFD213 D130:XFD130 A197:C197 F197:XFD197 A198:XFD211 A126:A129 C126:XFD129 A131:A140 C131:XFD140 A162:XFD163 A165:XFD165 A164 C164:XFD164 A166 C166:XFD166 A167:XFD171 A172 A188:XFD196 A186:A187 C186:XFD187 A212 C212:XFD212 A238:XFD243 A237 C237:XFD237 A160:A161 C160:XFD161 A231:XFD236 A230:B230 D230:XFD230 A244 C244:XFD244 A173:XFD185 C172:XFD172 A214:XFD229 A112:XFD125 B212:B213 A141:XFD159 A245:XFD251 A253:XFD1048576 A1:XFD110 B252:XFD252">
+  <conditionalFormatting sqref="D213:XFD213 D130:XFD130 A197:C197 F197:XFD197 A198:XFD211 A126:A129 C126:XFD129 A131:A140 C131:XFD140 A162:XFD163 A165:XFD165 A164 C164:XFD164 A166 C166:XFD166 A167:XFD171 A172 A188:XFD196 A186:A187 C186:XFD187 A212 C212:XFD212 A238:XFD243 A237 C237:XFD237 A160:A161 C160:XFD161 A231:XFD236 A230:B230 D230:XFD230 A244 C244:XFD244 A173:XFD185 C172:XFD172 A214:XFD229 A112:XFD125 B212:B213 A141:XFD159 A245:XFD251 A255:XFD1048576 A1:XFD110 B252:XFD254">
     <cfRule type="expression" dxfId="13" priority="15">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Tidy up livestock and economics GUI outputs
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D5FA76A-8E19-4628-B4B6-8E05AFB15979}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{615E24A2-3431-4F14-84D2-846227AC7AE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="596">
   <si>
     <t>PyOrator variable</t>
   </si>
@@ -2644,6 +2644,15 @@
   </si>
   <si>
     <t>Full household income of farm, crop growth calculated using Miami</t>
+  </si>
+  <si>
+    <t>dairy_cat_n_excrete_nlim</t>
+  </si>
+  <si>
+    <t>N excreted by Dairy Cattle (N Limited)</t>
+  </si>
+  <si>
+    <t>Nitrogen excreted by dairy cattle, crop growth limited by N availability</t>
   </si>
 </sst>
 </file>
@@ -10948,27 +10957,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H254"/>
+  <dimension ref="A1:H255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G252" sqref="G252:G254"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E255" sqref="E255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.149999999999999" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" style="28" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="25" customWidth="1"/>
-    <col min="3" max="3" width="35.1796875" customWidth="1"/>
-    <col min="4" max="4" width="30.26953125" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="120" customWidth="1"/>
-    <col min="6" max="6" width="18.81640625" customWidth="1"/>
-    <col min="7" max="7" width="19.1796875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="64.54296875" style="13" customWidth="1"/>
-    <col min="9" max="9" width="23.26953125" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="64.5703125" style="13" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="20.149999999999999" customHeight="1">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10994,7 +11003,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
         <v>5</v>
@@ -11006,7 +11015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A3" s="28" t="s">
         <v>277</v>
       </c>
@@ -11024,7 +11033,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
         <v>10</v>
@@ -11036,7 +11045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
         <v>11</v>
@@ -11048,7 +11057,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
         <v>12</v>
@@ -11060,7 +11069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="28" t="s">
         <v>470</v>
       </c>
@@ -11081,7 +11090,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="28" t="s">
         <v>333</v>
       </c>
@@ -11099,7 +11108,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="28" t="s">
         <v>332</v>
       </c>
@@ -11117,7 +11126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="28" t="s">
         <v>334</v>
       </c>
@@ -11135,7 +11144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="28" t="s">
         <v>268</v>
       </c>
@@ -11156,7 +11165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A12" s="28" t="s">
         <v>329</v>
       </c>
@@ -11174,7 +11183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A13" s="28" t="s">
         <v>368</v>
       </c>
@@ -11197,7 +11206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A14" s="28" t="s">
         <v>372</v>
       </c>
@@ -11220,7 +11229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A15" s="28" t="s">
         <v>378</v>
       </c>
@@ -11243,7 +11252,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A16" s="28" t="s">
         <v>380</v>
       </c>
@@ -11266,7 +11275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A17" s="28" t="s">
         <v>267</v>
       </c>
@@ -11287,7 +11296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D18" s="4"/>
       <c r="E18" s="4" t="s">
         <v>20</v>
@@ -11299,7 +11308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A19" s="28" t="s">
         <v>505</v>
       </c>
@@ -11317,7 +11326,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A20" s="28" t="s">
         <v>506</v>
       </c>
@@ -11335,7 +11344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="20" customFormat="1" ht="20.149999999999999" customHeight="1">
+    <row r="21" spans="1:8" s="20" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B21" s="26"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9" t="s">
@@ -11349,7 +11358,7 @@
       </c>
       <c r="H21" s="21"/>
     </row>
-    <row r="22" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
         <v>22</v>
@@ -11361,7 +11370,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D23" s="4"/>
       <c r="E23" s="4" t="s">
         <v>23</v>
@@ -11373,7 +11382,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D24" s="4"/>
       <c r="E24" s="4" t="s">
         <v>24</v>
@@ -11385,7 +11394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A25" s="28" t="s">
         <v>25</v>
       </c>
@@ -11406,7 +11415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A26" s="28" t="s">
         <v>27</v>
       </c>
@@ -11427,7 +11436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A27" s="28" t="s">
         <v>29</v>
       </c>
@@ -11448,7 +11457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A28" s="28" t="s">
         <v>318</v>
       </c>
@@ -11469,7 +11478,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D29" s="4"/>
       <c r="E29" s="4" t="s">
         <v>32</v>
@@ -11481,7 +11490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D30" s="7" t="s">
         <v>33</v>
       </c>
@@ -11495,7 +11504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D31" s="7" t="s">
         <v>232</v>
       </c>
@@ -11509,7 +11518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D32" s="4"/>
       <c r="E32" s="4" t="s">
         <v>36</v>
@@ -11521,7 +11530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D33" s="4"/>
       <c r="E33" s="4" t="s">
         <v>37</v>
@@ -11533,7 +11542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="28" t="s">
         <v>319</v>
       </c>
@@ -11554,7 +11563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="28" t="s">
         <v>320</v>
       </c>
@@ -11575,7 +11584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="28" t="s">
         <v>266</v>
       </c>
@@ -11596,7 +11605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D37" s="7" t="s">
         <v>233</v>
       </c>
@@ -11610,7 +11619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D38" s="7" t="s">
         <v>234</v>
       </c>
@@ -11624,7 +11633,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D39" s="4"/>
       <c r="E39" s="4" t="s">
         <v>43</v>
@@ -11636,7 +11645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="28" t="s">
         <v>383</v>
       </c>
@@ -11657,7 +11666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="28" t="s">
         <v>448</v>
       </c>
@@ -11678,7 +11687,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="28" t="s">
         <v>384</v>
       </c>
@@ -11699,7 +11708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="B43" s="25" t="s">
         <v>427</v>
       </c>
@@ -11714,7 +11723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="28" t="s">
         <v>343</v>
       </c>
@@ -11735,7 +11744,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="28" t="s">
         <v>344</v>
       </c>
@@ -11756,7 +11765,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="28" t="s">
         <v>345</v>
       </c>
@@ -11777,7 +11786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="28" t="s">
         <v>350</v>
       </c>
@@ -11798,7 +11807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="28" t="s">
         <v>323</v>
       </c>
@@ -11819,7 +11828,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="28" t="s">
         <v>514</v>
       </c>
@@ -11833,7 +11842,7 @@
       <c r="E49" s="4"/>
       <c r="F49" s="5"/>
     </row>
-    <row r="50" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="B50" s="25" t="s">
         <v>562</v>
       </c>
@@ -11848,7 +11857,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="36" t="s">
         <v>561</v>
       </c>
@@ -11869,7 +11878,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="52" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="28" t="s">
         <v>563</v>
       </c>
@@ -11890,13 +11899,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="53" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="5"/>
     </row>
-    <row r="54" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="54" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D54" s="4"/>
       <c r="E54" s="4" t="s">
         <v>48</v>
@@ -11908,7 +11917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A55" s="28" t="s">
         <v>451</v>
       </c>
@@ -11926,7 +11935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="56" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
         <v>51</v>
@@ -11938,7 +11947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="57" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
         <v>53</v>
@@ -11950,7 +11959,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="58" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
         <v>55</v>
@@ -11962,7 +11971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="59" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
         <v>56</v>
@@ -11974,7 +11983,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="60" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
         <v>57</v>
@@ -11986,7 +11995,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A61" s="28" t="s">
         <v>322</v>
       </c>
@@ -12007,7 +12016,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="62" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A62" s="28" t="s">
         <v>321</v>
       </c>
@@ -12028,7 +12037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D63" s="10" t="s">
         <v>359</v>
       </c>
@@ -12042,7 +12051,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="20" customFormat="1" ht="20.149999999999999" customHeight="1">
+    <row r="64" spans="1:8" s="20" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B64" s="26"/>
       <c r="D64" s="9"/>
       <c r="E64" s="22" t="s">
@@ -12056,7 +12065,7 @@
       </c>
       <c r="H64" s="21"/>
     </row>
-    <row r="65" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="65" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A65" s="28" t="s">
         <v>445</v>
       </c>
@@ -12077,7 +12086,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="66" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A66" s="28" t="s">
         <v>444</v>
       </c>
@@ -12092,7 +12101,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="67" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D67" s="4"/>
       <c r="E67" s="4" t="s">
         <v>64</v>
@@ -12104,7 +12113,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="68" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
         <v>65</v>
@@ -12116,7 +12125,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="69" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
         <v>66</v>
@@ -12128,7 +12137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="70" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A70" s="28" t="s">
         <v>301</v>
       </c>
@@ -12152,7 +12161,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="71" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A71" s="32" t="s">
         <v>298</v>
       </c>
@@ -12176,7 +12185,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="72" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A72" s="28" t="s">
         <v>297</v>
       </c>
@@ -12200,7 +12209,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="73" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="B73" s="25" t="s">
         <v>562</v>
       </c>
@@ -12215,7 +12224,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="74" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="B74" s="25" t="s">
         <v>562</v>
       </c>
@@ -12230,7 +12239,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="75" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="B75" s="25" t="s">
         <v>575</v>
       </c>
@@ -12247,7 +12256,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="76" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A76" t="s">
         <v>569</v>
       </c>
@@ -12270,7 +12279,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="77" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A77" t="s">
         <v>570</v>
       </c>
@@ -12293,7 +12302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="78" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A78"/>
       <c r="B78" s="25" t="s">
         <v>575</v>
@@ -12312,7 +12321,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="79" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A79" t="s">
         <v>567</v>
       </c>
@@ -12335,7 +12344,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="80" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A80" t="s">
         <v>568</v>
       </c>
@@ -12358,7 +12367,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="81" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A81"/>
       <c r="B81" s="25" t="s">
         <v>575</v>
@@ -12375,7 +12384,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="82" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A82" t="s">
         <v>565</v>
       </c>
@@ -12398,7 +12407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="83" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A83" t="s">
         <v>566</v>
       </c>
@@ -12421,7 +12430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="84" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D84" s="4"/>
       <c r="E84" s="4" t="s">
         <v>82</v>
@@ -12433,7 +12442,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="85" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D85" s="9" t="s">
         <v>243</v>
       </c>
@@ -12447,7 +12456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="86" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D86" s="4"/>
       <c r="E86" s="4" t="s">
         <v>84</v>
@@ -12459,7 +12468,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="87" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D87" s="4"/>
       <c r="E87" s="4" t="s">
         <v>85</v>
@@ -12471,7 +12480,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="88" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
         <v>86</v>
@@ -12483,7 +12492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="89" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D89" s="9" t="s">
         <v>244</v>
       </c>
@@ -12497,7 +12506,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="90" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
         <v>88</v>
@@ -12509,7 +12518,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="91" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A91" s="28" t="s">
         <v>282</v>
       </c>
@@ -12530,7 +12539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="92" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A92" s="28" t="s">
         <v>554</v>
       </c>
@@ -12554,7 +12563,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="93" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A93" s="28" t="s">
         <v>430</v>
       </c>
@@ -12575,7 +12584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="94" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A94" s="28" t="s">
         <v>481</v>
       </c>
@@ -12596,7 +12605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="95" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A95" s="28" t="s">
         <v>303</v>
       </c>
@@ -12614,7 +12623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="96" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A96" s="28" t="s">
         <v>440</v>
       </c>
@@ -12638,7 +12647,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="97" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A97" s="28" t="s">
         <v>486</v>
       </c>
@@ -12662,7 +12671,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="98" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A98" s="28" t="s">
         <v>441</v>
       </c>
@@ -12686,7 +12695,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="99" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A99" s="28" t="s">
         <v>471</v>
       </c>
@@ -12710,7 +12719,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="100" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D100" s="9" t="s">
         <v>245</v>
       </c>
@@ -12724,7 +12733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="101" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A101" t="s">
         <v>571</v>
       </c>
@@ -12747,7 +12756,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="102" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A102" t="s">
         <v>572</v>
       </c>
@@ -12770,7 +12779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="103" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A103" s="28" t="s">
         <v>551</v>
       </c>
@@ -12791,7 +12800,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="104" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A104" s="28" t="s">
         <v>559</v>
       </c>
@@ -12812,7 +12821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="105" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A105" s="28" t="s">
         <v>560</v>
       </c>
@@ -12833,7 +12842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="106" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A106" s="28" t="s">
         <v>490</v>
       </c>
@@ -12854,7 +12863,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="107" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A107" s="28" t="s">
         <v>284</v>
       </c>
@@ -12875,7 +12884,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="108" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A108" s="28" t="s">
         <v>557</v>
       </c>
@@ -12896,7 +12905,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="109" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A109" s="28" t="s">
         <v>457</v>
       </c>
@@ -12917,7 +12926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="110" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A110" s="28" t="s">
         <v>287</v>
       </c>
@@ -12940,7 +12949,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="111" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A111" s="28" t="s">
         <v>324</v>
       </c>
@@ -12964,7 +12973,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="112" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A112" s="28" t="s">
         <v>406</v>
       </c>
@@ -12985,7 +12994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="113" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A113" s="28" t="s">
         <v>410</v>
       </c>
@@ -13006,7 +13015,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="114" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A114" s="28" t="s">
         <v>498</v>
       </c>
@@ -13029,7 +13038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="115" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A115" s="28" t="s">
         <v>325</v>
       </c>
@@ -13047,7 +13056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="116" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A116" s="28" t="s">
         <v>288</v>
       </c>
@@ -13070,7 +13079,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="117" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A117" s="28" t="s">
         <v>290</v>
       </c>
@@ -13091,7 +13100,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="118" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A118" s="28" t="s">
         <v>511</v>
       </c>
@@ -13112,7 +13121,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="119" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A119" s="28" t="s">
         <v>398</v>
       </c>
@@ -13133,7 +13142,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="120" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A120" s="28" t="s">
         <v>399</v>
       </c>
@@ -13154,7 +13163,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="121" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A121" s="28" t="s">
         <v>289</v>
       </c>
@@ -13178,7 +13187,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="122" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A122" s="28" t="s">
         <v>405</v>
       </c>
@@ -13202,7 +13211,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="123" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A123" s="28" t="s">
         <v>472</v>
       </c>
@@ -13223,7 +13232,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="124" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A124" s="28" t="s">
         <v>495</v>
       </c>
@@ -13244,7 +13253,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="125" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A125" s="28" t="s">
         <v>491</v>
       </c>
@@ -13265,7 +13274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="126" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A126" s="28" t="s">
         <v>283</v>
       </c>
@@ -13286,7 +13295,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="127" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A127" s="28" t="s">
         <v>558</v>
       </c>
@@ -13307,7 +13316,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="128" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A128" s="28" t="s">
         <v>456</v>
       </c>
@@ -13328,7 +13337,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="129" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A129" s="28" t="s">
         <v>275</v>
       </c>
@@ -13351,7 +13360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="130" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A130" s="28" t="s">
         <v>327</v>
       </c>
@@ -13375,7 +13384,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="131" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A131" s="28" t="s">
         <v>276</v>
       </c>
@@ -13398,7 +13407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="132" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A132" s="28" t="s">
         <v>389</v>
       </c>
@@ -13419,7 +13428,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="133" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A133" s="28" t="s">
         <v>326</v>
       </c>
@@ -13440,7 +13449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="134" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A134" s="28" t="s">
         <v>393</v>
       </c>
@@ -13461,7 +13470,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="135" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A135" s="28" t="s">
         <v>325</v>
       </c>
@@ -13479,7 +13488,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="136" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A136" s="28" t="s">
         <v>274</v>
       </c>
@@ -13500,7 +13509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="137" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A137" s="28" t="s">
         <v>286</v>
       </c>
@@ -13521,7 +13530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="138" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A138" s="28" t="s">
         <v>396</v>
       </c>
@@ -13542,7 +13551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="139" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A139" s="28" t="s">
         <v>285</v>
       </c>
@@ -13563,7 +13572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="140" spans="1:8" s="8" customFormat="1" ht="20.149999999999999" customHeight="1">
+    <row r="140" spans="1:8" s="8" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A140" s="30" t="s">
         <v>387</v>
       </c>
@@ -13585,7 +13594,7 @@
       </c>
       <c r="H140" s="14"/>
     </row>
-    <row r="141" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="141" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A141" s="28" t="s">
         <v>295</v>
       </c>
@@ -13603,7 +13612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="142" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A142" s="28" t="s">
         <v>452</v>
       </c>
@@ -13621,7 +13630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="143" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D143" s="9" t="s">
         <v>251</v>
       </c>
@@ -13635,7 +13644,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="144" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A144" s="28" t="s">
         <v>458</v>
       </c>
@@ -13653,7 +13662,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="145" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D145" s="9" t="s">
         <v>252</v>
       </c>
@@ -13667,7 +13676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="146" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A146" s="28" t="s">
         <v>459</v>
       </c>
@@ -13685,7 +13694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="147" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D147" s="9" t="s">
         <v>253</v>
       </c>
@@ -13699,7 +13708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="148" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D148" s="4"/>
       <c r="E148" s="4" t="s">
         <v>127</v>
@@ -13712,7 +13721,7 @@
       </c>
       <c r="H148"/>
     </row>
-    <row r="149" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="149" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D149" s="4"/>
       <c r="E149" s="4" t="s">
         <v>128</v>
@@ -13725,7 +13734,7 @@
       </c>
       <c r="H149"/>
     </row>
-    <row r="150" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="150" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D150" s="4"/>
       <c r="E150" s="4" t="s">
         <v>129</v>
@@ -13738,7 +13747,7 @@
       </c>
       <c r="H150"/>
     </row>
-    <row r="151" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="151" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A151" s="28" t="s">
         <v>293</v>
       </c>
@@ -13760,7 +13769,7 @@
       </c>
       <c r="H151"/>
     </row>
-    <row r="152" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="152" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A152" s="28" t="s">
         <v>331</v>
       </c>
@@ -13779,7 +13788,7 @@
       </c>
       <c r="H152"/>
     </row>
-    <row r="153" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="153" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A153" s="28" t="s">
         <v>330</v>
       </c>
@@ -13798,7 +13807,7 @@
       </c>
       <c r="H153"/>
     </row>
-    <row r="154" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="154" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D154" s="4"/>
       <c r="E154" s="4" t="s">
         <v>133</v>
@@ -13811,7 +13820,7 @@
       </c>
       <c r="H154"/>
     </row>
-    <row r="155" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="155" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D155" s="4"/>
       <c r="E155" s="4" t="s">
         <v>134</v>
@@ -13824,7 +13833,7 @@
       </c>
       <c r="H155"/>
     </row>
-    <row r="156" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="156" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A156" s="28" t="s">
         <v>294</v>
       </c>
@@ -13843,7 +13852,7 @@
       </c>
       <c r="H156"/>
     </row>
-    <row r="157" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="157" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A157" s="28" t="s">
         <v>546</v>
       </c>
@@ -13862,7 +13871,7 @@
       </c>
       <c r="H157"/>
     </row>
-    <row r="158" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="158" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D158" s="9" t="s">
         <v>254</v>
       </c>
@@ -13877,7 +13886,7 @@
       </c>
       <c r="H158"/>
     </row>
-    <row r="159" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="159" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A159" s="8" t="s">
         <v>443</v>
       </c>
@@ -13893,7 +13902,7 @@
       </c>
       <c r="H159"/>
     </row>
-    <row r="160" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="160" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A160" s="28" t="s">
         <v>273</v>
       </c>
@@ -13915,7 +13924,7 @@
       </c>
       <c r="H160"/>
     </row>
-    <row r="161" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="161" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A161" s="8" t="s">
         <v>442</v>
       </c>
@@ -13934,7 +13943,7 @@
       </c>
       <c r="H161"/>
     </row>
-    <row r="162" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="162" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D162" s="4"/>
       <c r="E162" s="4" t="s">
         <v>141</v>
@@ -13947,7 +13956,7 @@
       </c>
       <c r="H162"/>
     </row>
-    <row r="163" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="163" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D163" s="4"/>
       <c r="E163" s="4" t="s">
         <v>142</v>
@@ -13960,7 +13969,7 @@
       </c>
       <c r="H163"/>
     </row>
-    <row r="164" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="164" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A164" s="28" t="s">
         <v>308</v>
       </c>
@@ -13984,7 +13993,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="165" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D165" s="4"/>
       <c r="E165" s="4" t="s">
         <v>144</v>
@@ -13996,7 +14005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="166" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A166" s="28" t="s">
         <v>317</v>
       </c>
@@ -14014,7 +14023,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="167" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D167" s="4"/>
       <c r="E167" s="4" t="s">
         <v>146</v>
@@ -14026,7 +14035,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="168" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A168" s="28" t="s">
         <v>361</v>
       </c>
@@ -14046,7 +14055,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="169" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D169" s="4"/>
       <c r="E169" s="4" t="s">
         <v>147</v>
@@ -14058,7 +14067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="170" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D170" s="9" t="s">
         <v>255</v>
       </c>
@@ -14072,7 +14081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="171" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A171" s="28" t="s">
         <v>429</v>
       </c>
@@ -14087,7 +14096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="172" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A172" s="28" t="s">
         <v>493</v>
       </c>
@@ -14111,7 +14120,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="173" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A173" s="28" t="s">
         <v>388</v>
       </c>
@@ -14132,7 +14141,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="174" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A174" s="28" t="s">
         <v>478</v>
       </c>
@@ -14153,7 +14162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="175" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D175" s="4"/>
       <c r="E175" s="4" t="s">
         <v>152</v>
@@ -14168,7 +14177,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="176" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="176" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D176" s="4"/>
       <c r="E176" s="4" t="s">
         <v>153</v>
@@ -14180,7 +14189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="177" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A177" s="28" t="s">
         <v>272</v>
       </c>
@@ -14195,7 +14204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="178" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D178" s="4"/>
       <c r="E178" s="4" t="s">
         <v>157</v>
@@ -14207,7 +14216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="179" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="179" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A179" s="28" t="s">
         <v>271</v>
       </c>
@@ -14228,7 +14237,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="180" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D180" s="4"/>
       <c r="E180" s="4" t="s">
         <v>160</v>
@@ -14240,7 +14249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="181" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="181" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D181" s="4"/>
       <c r="E181" s="4" t="s">
         <v>161</v>
@@ -14252,7 +14261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="182" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D182" s="4"/>
       <c r="E182" s="4" t="s">
         <v>162</v>
@@ -14264,7 +14273,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="183" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A183" s="28" t="s">
         <v>270</v>
       </c>
@@ -14279,7 +14288,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="184" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="184" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A184" s="28" t="s">
         <v>269</v>
       </c>
@@ -14294,7 +14303,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="185" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="185" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D185" s="4"/>
       <c r="E185" s="4" t="s">
         <v>165</v>
@@ -14306,7 +14315,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="186" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="186" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A186" s="28" t="s">
         <v>311</v>
       </c>
@@ -14327,7 +14336,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="187" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="187" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A187" s="28" t="s">
         <v>265</v>
       </c>
@@ -14348,7 +14357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="188" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="188" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D188" s="4"/>
       <c r="E188" s="4" t="s">
         <v>169</v>
@@ -14360,7 +14369,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="189" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="189" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D189" s="4"/>
       <c r="E189" s="4" t="s">
         <v>170</v>
@@ -14372,7 +14381,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="190" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="190" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D190" s="4"/>
       <c r="E190" s="4" t="s">
         <v>171</v>
@@ -14384,7 +14393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="191" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D191" s="4"/>
       <c r="E191" s="4" t="s">
         <v>172</v>
@@ -14396,7 +14405,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="192" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="192" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D192" s="4"/>
       <c r="E192" s="4" t="s">
         <v>173</v>
@@ -14408,7 +14417,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="193" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="193" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D193" s="4"/>
       <c r="E193" s="4" t="s">
         <v>174</v>
@@ -14420,7 +14429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="194" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D194" s="4"/>
       <c r="E194" s="4" t="s">
         <v>175</v>
@@ -14432,7 +14441,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="195" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="195" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D195" s="4"/>
       <c r="E195" s="4" t="s">
         <v>176</v>
@@ -14444,7 +14453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="196" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="196" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D196" s="4"/>
       <c r="E196" s="4" t="s">
         <v>177</v>
@@ -14456,7 +14465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="197" spans="1:8" s="15" customFormat="1" ht="20.149999999999999" customHeight="1">
+    <row r="197" spans="1:8" s="15" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A197" s="31" t="s">
         <v>431</v>
       </c>
@@ -14471,7 +14480,7 @@
       <c r="G197" s="17"/>
       <c r="H197" s="18"/>
     </row>
-    <row r="198" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="198" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D198" s="4"/>
       <c r="E198" s="4" t="s">
         <v>179</v>
@@ -14483,7 +14492,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="199" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D199" s="4"/>
       <c r="E199" s="4" t="s">
         <v>180</v>
@@ -14495,7 +14504,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="200" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="200" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D200" s="4"/>
       <c r="E200" s="4" t="s">
         <v>181</v>
@@ -14507,7 +14516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="201" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="201" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D201" s="9" t="s">
         <v>256</v>
       </c>
@@ -14521,7 +14530,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="202" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D202" s="9" t="s">
         <v>257</v>
       </c>
@@ -14535,7 +14544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="203" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="203" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D203" s="9" t="s">
         <v>258</v>
       </c>
@@ -14549,7 +14558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="204" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="204" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D204" s="4"/>
       <c r="E204" s="4" t="s">
         <v>185</v>
@@ -14561,7 +14570,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="205" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="205" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D205" s="9" t="s">
         <v>259</v>
       </c>
@@ -14575,7 +14584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="206" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="206" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D206" s="4"/>
       <c r="E206" s="4" t="s">
         <v>186</v>
@@ -14587,7 +14596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="207" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="207" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A207" s="28" t="s">
         <v>328</v>
       </c>
@@ -14605,7 +14614,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="208" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="208" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D208" s="4"/>
       <c r="E208" s="4" t="s">
         <v>189</v>
@@ -14617,7 +14626,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="209" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="209" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D209" s="4"/>
       <c r="E209" s="4" t="s">
         <v>187</v>
@@ -14629,7 +14638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="210" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="210" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A210" s="28" t="s">
         <v>509</v>
       </c>
@@ -14650,7 +14659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="211" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="211" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A211" s="28" t="s">
         <v>408</v>
       </c>
@@ -14673,7 +14682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="212" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="212" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A212" s="28" t="s">
         <v>419</v>
       </c>
@@ -14694,7 +14703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="213" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="213" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A213" s="29" t="s">
         <v>314</v>
       </c>
@@ -14715,7 +14724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="214" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="214" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A214" s="28" t="s">
         <v>315</v>
       </c>
@@ -14736,7 +14745,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="215" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="215" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D215" s="4"/>
       <c r="E215" s="4" t="s">
         <v>194</v>
@@ -14748,7 +14757,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="216" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="216" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D216" s="9" t="s">
         <v>261</v>
       </c>
@@ -14762,7 +14771,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="217" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="217" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A217" s="28" t="s">
         <v>404</v>
       </c>
@@ -14783,7 +14792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="218" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="218" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A218" s="30" t="s">
         <v>432</v>
       </c>
@@ -14798,7 +14807,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="219" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D219" s="4"/>
       <c r="E219" s="4" t="s">
         <v>198</v>
@@ -14810,7 +14819,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="220" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D220" s="4"/>
       <c r="E220" s="4" t="s">
         <v>199</v>
@@ -14822,7 +14831,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="221" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="221" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="D221" s="4"/>
       <c r="E221" s="4" t="s">
         <v>200</v>
@@ -14834,7 +14843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="222" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="222" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A222" s="28" t="s">
         <v>411</v>
       </c>
@@ -14855,7 +14864,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="223" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="223" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A223" s="28" t="s">
         <v>281</v>
       </c>
@@ -14873,7 +14882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="224" spans="1:7" ht="20.149999999999999" customHeight="1">
+    <row r="224" spans="1:7" ht="20.100000000000001" customHeight="1">
       <c r="A224" s="28" t="s">
         <v>280</v>
       </c>
@@ -14894,7 +14903,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="225" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="225" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D225" s="4"/>
       <c r="E225" s="4" t="s">
         <v>203</v>
@@ -14906,7 +14915,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="226" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="226" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D226" s="4"/>
       <c r="E226" s="4" t="s">
         <v>204</v>
@@ -14918,7 +14927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="227" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="227" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A227" s="28" t="s">
         <v>414</v>
       </c>
@@ -14939,7 +14948,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="228" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="228" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A228" s="28" t="s">
         <v>416</v>
       </c>
@@ -14960,7 +14969,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="229" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="229" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A229" s="28" t="s">
         <v>278</v>
       </c>
@@ -14986,7 +14995,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="230" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="230" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A230" s="28" t="s">
         <v>466</v>
       </c>
@@ -15010,7 +15019,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="231" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="231" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D231" s="4"/>
       <c r="E231" s="4" t="s">
         <v>206</v>
@@ -15022,7 +15031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="232" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="232" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D232" s="4"/>
       <c r="E232" s="4" t="s">
         <v>207</v>
@@ -15034,7 +15043,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="233" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="233" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D233" s="9" t="s">
         <v>262</v>
       </c>
@@ -15049,7 +15058,7 @@
       </c>
       <c r="H233"/>
     </row>
-    <row r="234" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="234" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D234" s="9" t="s">
         <v>263</v>
       </c>
@@ -15064,7 +15073,7 @@
       </c>
       <c r="H234"/>
     </row>
-    <row r="235" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="235" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D235" s="4"/>
       <c r="E235" s="4" t="s">
         <v>211</v>
@@ -15077,7 +15086,7 @@
       </c>
       <c r="H235"/>
     </row>
-    <row r="236" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="236" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D236" s="9" t="s">
         <v>264</v>
       </c>
@@ -15092,7 +15101,7 @@
       </c>
       <c r="H236"/>
     </row>
-    <row r="237" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="237" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A237" s="28" t="s">
         <v>296</v>
       </c>
@@ -15114,7 +15123,7 @@
       </c>
       <c r="H237"/>
     </row>
-    <row r="238" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="238" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D238" s="4"/>
       <c r="E238" s="4" t="s">
         <v>214</v>
@@ -15127,7 +15136,7 @@
       </c>
       <c r="H238"/>
     </row>
-    <row r="239" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="239" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D239" s="4"/>
       <c r="E239" s="4" t="s">
         <v>215</v>
@@ -15140,7 +15149,7 @@
       </c>
       <c r="H239"/>
     </row>
-    <row r="240" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="240" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A240" s="28" t="s">
         <v>433</v>
       </c>
@@ -15156,7 +15165,7 @@
       </c>
       <c r="H240"/>
     </row>
-    <row r="241" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="241" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A241" s="28" t="s">
         <v>434</v>
       </c>
@@ -15172,7 +15181,7 @@
       </c>
       <c r="H241"/>
     </row>
-    <row r="242" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="242" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D242" s="4"/>
       <c r="E242" s="4" t="s">
         <v>218</v>
@@ -15185,7 +15194,7 @@
       </c>
       <c r="H242"/>
     </row>
-    <row r="243" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="243" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D243" s="4"/>
       <c r="E243" s="4" t="s">
         <v>219</v>
@@ -15198,7 +15207,7 @@
       </c>
       <c r="H243"/>
     </row>
-    <row r="244" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="244" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A244" s="28" t="s">
         <v>468</v>
       </c>
@@ -15220,7 +15229,7 @@
       </c>
       <c r="H244"/>
     </row>
-    <row r="245" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="245" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D245" s="4"/>
       <c r="E245" s="4" t="s">
         <v>221</v>
@@ -15233,7 +15242,7 @@
       </c>
       <c r="H245"/>
     </row>
-    <row r="246" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="246" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D246" s="4"/>
       <c r="E246" s="4" t="s">
         <v>222</v>
@@ -15246,7 +15255,7 @@
       </c>
       <c r="H246"/>
     </row>
-    <row r="247" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="247" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D247" s="4"/>
       <c r="E247" s="4" t="s">
         <v>224</v>
@@ -15259,7 +15268,7 @@
       </c>
       <c r="H247"/>
     </row>
-    <row r="248" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="248" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D248" s="4"/>
       <c r="E248" s="4" t="s">
         <v>226</v>
@@ -15272,7 +15281,7 @@
       </c>
       <c r="H248"/>
     </row>
-    <row r="249" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="249" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D249" s="4"/>
       <c r="E249" s="4" t="s">
         <v>227</v>
@@ -15285,7 +15294,7 @@
       </c>
       <c r="H249"/>
     </row>
-    <row r="250" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="250" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D250" s="4"/>
       <c r="E250" s="4" t="s">
         <v>229</v>
@@ -15298,7 +15307,7 @@
       </c>
       <c r="H250"/>
     </row>
-    <row r="251" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="251" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="D251" s="4"/>
       <c r="E251" s="4" t="s">
         <v>230</v>
@@ -15311,7 +15320,7 @@
       </c>
       <c r="H251"/>
     </row>
-    <row r="252" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="252" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A252" s="28" t="s">
         <v>582</v>
       </c>
@@ -15331,7 +15340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="253" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="253" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A253" s="28" t="s">
         <v>585</v>
       </c>
@@ -15351,7 +15360,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="254" spans="1:8" ht="20.149999999999999" customHeight="1">
+    <row r="254" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A254" s="28" t="s">
         <v>586</v>
       </c>
@@ -15368,6 +15377,26 @@
         <v>584</v>
       </c>
       <c r="G254" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A255" s="28" t="s">
+        <v>593</v>
+      </c>
+      <c r="B255" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C255" t="s">
+        <v>594</v>
+      </c>
+      <c r="E255" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="F255" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="G255" s="6" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added in graphs data for poultry and pigs
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E6087B-5DDE-4B42-BBC4-7F75DB8E28BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6087C883-C917-4936-A449-A38A0FBEEA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="647">
   <si>
     <t>PyOrator variable</t>
   </si>
@@ -2743,6 +2743,69 @@
   </si>
   <si>
     <t>Manure produced by goats and sheep, crop growth limited by N availability</t>
+  </si>
+  <si>
+    <t>poultry_n_excrete_nlim</t>
+  </si>
+  <si>
+    <t>poultry_eggs_prod_nlim</t>
+  </si>
+  <si>
+    <t>poultry_meat_prod_nlim</t>
+  </si>
+  <si>
+    <t>poultry_manure_prod_nlim</t>
+  </si>
+  <si>
+    <t>N excreted by poultry (N Limited)</t>
+  </si>
+  <si>
+    <t>Eggs produced by poultry (N Limited)</t>
+  </si>
+  <si>
+    <t>Meat produced by poultry (N Limited)</t>
+  </si>
+  <si>
+    <t>Manure produced by poultry (N Limited)</t>
+  </si>
+  <si>
+    <t>Nitrogen excreted by poultry , crop growth limited by N availability</t>
+  </si>
+  <si>
+    <t>Eggs produced by poultry, crop growth limited by N availability</t>
+  </si>
+  <si>
+    <t>Meat produced by  poultry, crop growth limited by N availability</t>
+  </si>
+  <si>
+    <t>Manure produced by poultry, crop growth limited by N availability</t>
+  </si>
+  <si>
+    <t>pigs_n_excrete_nlim</t>
+  </si>
+  <si>
+    <t>N excreted by pigs (N Limited)</t>
+  </si>
+  <si>
+    <t>Meat produced by pigs (N Limited)</t>
+  </si>
+  <si>
+    <t>Manure produced by pigs (N Limited)</t>
+  </si>
+  <si>
+    <t>Nitrogen excreted by pigs, crop growth limited by N availability</t>
+  </si>
+  <si>
+    <t>Meat produced by  pigs, crop growth limited by N availability</t>
+  </si>
+  <si>
+    <t>Manure produced by pigs, crop growth limited by N availability</t>
+  </si>
+  <si>
+    <t>pigs_manure_prod_nlim</t>
+  </si>
+  <si>
+    <t>pigs_meat_prod_nlim</t>
   </si>
 </sst>
 </file>
@@ -11047,11 +11110,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H265"/>
+  <dimension ref="A1:H272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E265" sqref="E265"/>
+      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A272" sqref="A272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -15687,6 +15750,146 @@
         <v>463</v>
       </c>
       <c r="G265" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A266" s="28" t="s">
+        <v>626</v>
+      </c>
+      <c r="B266" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C266" t="s">
+        <v>630</v>
+      </c>
+      <c r="E266" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="F266" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="G266" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A267" s="28" t="s">
+        <v>627</v>
+      </c>
+      <c r="B267" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C267" t="s">
+        <v>631</v>
+      </c>
+      <c r="E267" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="F267" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="G267" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A268" s="28" t="s">
+        <v>628</v>
+      </c>
+      <c r="B268" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C268" t="s">
+        <v>632</v>
+      </c>
+      <c r="E268" t="s">
+        <v>636</v>
+      </c>
+      <c r="F268" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="G268" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A269" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="B269" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C269" t="s">
+        <v>633</v>
+      </c>
+      <c r="E269" t="s">
+        <v>637</v>
+      </c>
+      <c r="F269" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="G269" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A270" s="28" t="s">
+        <v>638</v>
+      </c>
+      <c r="B270" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C270" t="s">
+        <v>639</v>
+      </c>
+      <c r="E270" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="F270" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="G270" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A271" s="28" t="s">
+        <v>646</v>
+      </c>
+      <c r="B271" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C271" t="s">
+        <v>640</v>
+      </c>
+      <c r="E271" t="s">
+        <v>643</v>
+      </c>
+      <c r="F271" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="G271" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A272" s="28" t="s">
+        <v>645</v>
+      </c>
+      <c r="B272" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C272" t="s">
+        <v>641</v>
+      </c>
+      <c r="E272" t="s">
+        <v>644</v>
+      </c>
+      <c r="F272" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="G272" s="6" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All econ calcs now shown as graphs in GUI
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6087C883-C917-4936-A449-A38A0FBEEA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BDBD0F-F407-4B89-92C2-EDB2C4A38844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="658">
   <si>
     <t>PyOrator variable</t>
   </si>
@@ -2806,6 +2806,39 @@
   </si>
   <si>
     <t>pigs_meat_prod_nlim</t>
+  </si>
+  <si>
+    <t>per_capita_consumption_n_lim</t>
+  </si>
+  <si>
+    <t>relative_food_insecurity_n_lim</t>
+  </si>
+  <si>
+    <t>dietary_diversity_n_lim</t>
+  </si>
+  <si>
+    <t>Per Capita Consumption (N Limited))</t>
+  </si>
+  <si>
+    <t>Relative Food Insecutiry (N Limited)</t>
+  </si>
+  <si>
+    <t>Dietary Divertsity (N Limited)</t>
+  </si>
+  <si>
+    <t>ETB/Y</t>
+  </si>
+  <si>
+    <t>Per Capita Consumption, crop production limited by N availability</t>
+  </si>
+  <si>
+    <t>Chance of Relative Food Insecurity, crop production limited by N availability</t>
+  </si>
+  <si>
+    <t>Number of discrete food typesconsumed, crop production limited by N availability</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
 </sst>
 </file>
@@ -11110,16 +11143,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H272"/>
+  <dimension ref="A1:H275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A251" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A272" sqref="A272"/>
+      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D286" sqref="D286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" style="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="25" customWidth="1"/>
     <col min="3" max="3" width="35.140625" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
@@ -15890,6 +15923,66 @@
         <v>463</v>
       </c>
       <c r="G272" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A273" s="28" t="s">
+        <v>647</v>
+      </c>
+      <c r="B273" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C273" t="s">
+        <v>650</v>
+      </c>
+      <c r="E273" t="s">
+        <v>654</v>
+      </c>
+      <c r="F273" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="G273" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A274" s="28" t="s">
+        <v>648</v>
+      </c>
+      <c r="B274" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C274" t="s">
+        <v>651</v>
+      </c>
+      <c r="E274" t="s">
+        <v>655</v>
+      </c>
+      <c r="F274" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="G274" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" ht="20.100000000000001" customHeight="1">
+      <c r="A275" s="28" t="s">
+        <v>649</v>
+      </c>
+      <c r="B275" s="25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C275" t="s">
+        <v>652</v>
+      </c>
+      <c r="E275" t="s">
+        <v>656</v>
+      </c>
+      <c r="F275" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="G275" s="6" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
further cosmetic changes to some modules to improve readability and conformance to PEP 8 standard.
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testPyOra\OratorRun\lookup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BDBD0F-F407-4B89-92C2-EDB2C4A38844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A90F9E8-859B-4FA4-9E34-51ABAE98B7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="630" windowWidth="22560" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="659">
   <si>
     <t>PyOrator variable</t>
   </si>
@@ -2839,6 +2839,9 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>harv_indx</t>
   </si>
 </sst>
 </file>
@@ -3014,7 +3017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3022,7 +3025,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3073,15 +3076,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3091,14 +3085,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3111,61 +3100,12 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -11146,14 +11086,14 @@
   <dimension ref="A1:H275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D286" sqref="D286"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" style="25" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" style="22" customWidth="1"/>
     <col min="3" max="3" width="35.140625" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="120" customWidth="1"/>
@@ -11202,10 +11142,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="28" t="s">
+      <c r="A3" t="s">
         <v>277</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="22" t="s">
         <v>426</v>
       </c>
       <c r="D3" s="4"/>
@@ -11256,10 +11196,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="28" t="s">
+      <c r="A7" t="s">
         <v>470</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C7" t="s">
@@ -11277,10 +11217,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" t="s">
         <v>333</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D8" s="4"/>
@@ -11295,10 +11235,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="28" t="s">
+      <c r="A9" t="s">
         <v>332</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D9" s="4"/>
@@ -11313,10 +11253,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="28" t="s">
+      <c r="A10" t="s">
         <v>334</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D10" s="4"/>
@@ -11331,10 +11271,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="28" t="s">
+      <c r="A11" t="s">
         <v>268</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -11352,10 +11292,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="28" t="s">
+      <c r="A12" t="s">
         <v>329</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D12" s="4"/>
@@ -11370,10 +11310,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="28" t="s">
+      <c r="A13" t="s">
         <v>368</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C13" t="s">
@@ -11393,10 +11333,10 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="28" t="s">
+      <c r="A14" t="s">
         <v>372</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C14" t="s">
@@ -11416,10 +11356,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="28" t="s">
+      <c r="A15" t="s">
         <v>378</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C15" t="s">
@@ -11439,10 +11379,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="28" t="s">
+      <c r="A16" t="s">
         <v>380</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C16" t="s">
@@ -11462,10 +11402,10 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="28" t="s">
+      <c r="A17" t="s">
         <v>267</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -11495,7 +11435,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="28" t="s">
+      <c r="A19" t="s">
         <v>505</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -11513,7 +11453,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="28" t="s">
+      <c r="A20" t="s">
         <v>506</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -11531,15 +11471,15 @@
       </c>
     </row>
     <row r="21" spans="1:8" s="20" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="B21" s="26"/>
+      <c r="B21" s="23"/>
       <c r="D21" s="9"/>
       <c r="E21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="27" t="s">
         <v>462</v>
       </c>
-      <c r="G21" s="34" t="s">
+      <c r="G21" s="28" t="s">
         <v>7</v>
       </c>
       <c r="H21" s="21"/>
@@ -11581,10 +11521,10 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="28" t="s">
+      <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C25" s="4" t="s">
@@ -11602,10 +11542,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="28" t="s">
+      <c r="A26" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -11623,10 +11563,10 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="28" t="s">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -11644,10 +11584,10 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="28" t="s">
+      <c r="A28" t="s">
         <v>318</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -11729,10 +11669,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="28" t="s">
+      <c r="A34" t="s">
         <v>319</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C34" t="s">
@@ -11750,10 +11690,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A35" s="28" t="s">
+      <c r="A35" t="s">
         <v>320</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C35" t="s">
@@ -11771,10 +11711,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="28" t="s">
+      <c r="A36" t="s">
         <v>266</v>
       </c>
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C36" t="s">
@@ -11832,10 +11772,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A40" s="28" t="s">
+      <c r="A40" t="s">
         <v>383</v>
       </c>
-      <c r="B40" s="25" t="s">
+      <c r="B40" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C40" s="4" t="s">
@@ -11853,10 +11793,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A41" s="28" t="s">
+      <c r="A41" t="s">
         <v>448</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C41" t="s">
@@ -11874,10 +11814,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A42" s="28" t="s">
+      <c r="A42" t="s">
         <v>384</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C42" t="s">
@@ -11895,7 +11835,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D43" s="4"/>
@@ -11910,10 +11850,10 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A44" s="28" t="s">
+      <c r="A44" t="s">
         <v>343</v>
       </c>
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C44" s="4" t="s">
@@ -11931,10 +11871,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A45" s="28" t="s">
+      <c r="A45" t="s">
         <v>344</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C45" s="4" t="s">
@@ -11952,10 +11892,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A46" s="28" t="s">
+      <c r="A46" t="s">
         <v>345</v>
       </c>
-      <c r="B46" s="25" t="s">
+      <c r="B46" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C46" s="4" t="s">
@@ -11973,10 +11913,10 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A47" s="28" t="s">
+      <c r="A47" t="s">
         <v>350</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C47" s="4" t="s">
@@ -11994,10 +11934,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A48" s="28" t="s">
+      <c r="A48" t="s">
         <v>323</v>
       </c>
-      <c r="B48" s="25" t="s">
+      <c r="B48" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C48" s="4" t="s">
@@ -12015,10 +11955,10 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A49" s="28" t="s">
+      <c r="A49" t="s">
         <v>514</v>
       </c>
-      <c r="B49" s="25" t="s">
+      <c r="B49" s="22" t="s">
         <v>562</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -12029,7 +11969,7 @@
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="B50" s="25" t="s">
+      <c r="B50" s="22" t="s">
         <v>562</v>
       </c>
       <c r="D50" s="4"/>
@@ -12044,10 +11984,10 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="30" t="s">
         <v>561</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="22" t="s">
         <v>562</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -12065,10 +12005,10 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A52" s="28" t="s">
+      <c r="A52" t="s">
         <v>563</v>
       </c>
-      <c r="B52" s="25" t="s">
+      <c r="B52" s="22" t="s">
         <v>562</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -12104,7 +12044,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A55" s="28" t="s">
+      <c r="A55" t="s">
         <v>451</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -12182,10 +12122,10 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A61" s="28" t="s">
+      <c r="A61" t="s">
         <v>322</v>
       </c>
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -12203,10 +12143,10 @@
       </c>
     </row>
     <row r="62" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A62" s="28" t="s">
+      <c r="A62" t="s">
         <v>321</v>
       </c>
-      <c r="B62" s="25" t="s">
+      <c r="B62" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C62" s="4" t="s">
@@ -12224,6 +12164,9 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="A63" t="s">
+        <v>658</v>
+      </c>
       <c r="D63" s="10" t="s">
         <v>359</v>
       </c>
@@ -12238,24 +12181,24 @@
       </c>
     </row>
     <row r="64" spans="1:8" s="20" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="B64" s="26"/>
+      <c r="B64" s="23"/>
       <c r="D64" s="9"/>
-      <c r="E64" s="22" t="s">
+      <c r="E64" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F64" s="23" t="s">
+      <c r="F64" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G64" s="24" t="s">
+      <c r="G64" s="6" t="s">
         <v>7</v>
       </c>
       <c r="H64" s="21"/>
     </row>
     <row r="65" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A65" s="28" t="s">
+      <c r="A65" t="s">
         <v>445</v>
       </c>
-      <c r="B65" s="25" t="s">
+      <c r="B65" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C65" s="4" t="s">
@@ -12273,7 +12216,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A66" s="28" t="s">
+      <c r="A66" t="s">
         <v>444</v>
       </c>
       <c r="D66" s="4"/>
@@ -12324,10 +12267,10 @@
       </c>
     </row>
     <row r="70" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A70" s="28" t="s">
+      <c r="A70" t="s">
         <v>301</v>
       </c>
-      <c r="B70" s="25" t="s">
+      <c r="B70" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C70" s="11" t="s">
@@ -12348,10 +12291,10 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A71" s="32" t="s">
+      <c r="A71" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="B71" s="25" t="s">
+      <c r="B71" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C71" s="11" t="s">
@@ -12372,10 +12315,10 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A72" s="28" t="s">
+      <c r="A72" t="s">
         <v>297</v>
       </c>
-      <c r="B72" s="25" t="s">
+      <c r="B72" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C72" s="11" t="s">
@@ -12396,7 +12339,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="B73" s="25" t="s">
+      <c r="B73" s="22" t="s">
         <v>562</v>
       </c>
       <c r="D73" s="4"/>
@@ -12411,7 +12354,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="B74" s="25" t="s">
+      <c r="B74" s="22" t="s">
         <v>562</v>
       </c>
       <c r="D74" s="4"/>
@@ -12426,7 +12369,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="B75" s="25" t="s">
+      <c r="B75" s="22" t="s">
         <v>575</v>
       </c>
       <c r="D75" s="9" t="s">
@@ -12446,7 +12389,7 @@
       <c r="A76" t="s">
         <v>569</v>
       </c>
-      <c r="B76" s="25" t="s">
+      <c r="B76" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C76" s="4" t="s">
@@ -12469,7 +12412,7 @@
       <c r="A77" t="s">
         <v>570</v>
       </c>
-      <c r="B77" s="25" t="s">
+      <c r="B77" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C77" s="4" t="s">
@@ -12489,8 +12432,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A78"/>
-      <c r="B78" s="25" t="s">
+      <c r="B78" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C78" s="4"/>
@@ -12511,7 +12453,7 @@
       <c r="A79" t="s">
         <v>567</v>
       </c>
-      <c r="B79" s="25" t="s">
+      <c r="B79" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C79" s="4" t="s">
@@ -12534,7 +12476,7 @@
       <c r="A80" t="s">
         <v>568</v>
       </c>
-      <c r="B80" s="25" t="s">
+      <c r="B80" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C80" s="4" t="s">
@@ -12554,8 +12496,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A81"/>
-      <c r="B81" s="25" t="s">
+      <c r="B81" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C81" s="4"/>
@@ -12574,7 +12515,7 @@
       <c r="A82" t="s">
         <v>565</v>
       </c>
-      <c r="B82" s="25" t="s">
+      <c r="B82" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C82" s="4" t="s">
@@ -12597,7 +12538,7 @@
       <c r="A83" t="s">
         <v>566</v>
       </c>
-      <c r="B83" s="25" t="s">
+      <c r="B83" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C83" s="4" t="s">
@@ -12705,10 +12646,10 @@
       </c>
     </row>
     <row r="91" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A91" s="28" t="s">
+      <c r="A91" t="s">
         <v>282</v>
       </c>
-      <c r="B91" s="25" t="s">
+      <c r="B91" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C91" t="s">
@@ -12726,10 +12667,10 @@
       </c>
     </row>
     <row r="92" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A92" s="28" t="s">
+      <c r="A92" t="s">
         <v>554</v>
       </c>
-      <c r="B92" s="25" t="s">
+      <c r="B92" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C92" s="4" t="s">
@@ -12750,17 +12691,17 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A93" s="28" t="s">
+      <c r="A93" t="s">
         <v>430</v>
       </c>
-      <c r="B93" s="25" t="s">
+      <c r="B93" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>435</v>
       </c>
       <c r="D93" s="4"/>
-      <c r="E93" s="35" t="s">
+      <c r="E93" s="29" t="s">
         <v>482</v>
       </c>
       <c r="F93" s="5" t="s">
@@ -12771,10 +12712,10 @@
       </c>
     </row>
     <row r="94" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A94" s="28" t="s">
+      <c r="A94" t="s">
         <v>481</v>
       </c>
-      <c r="B94" s="25" t="s">
+      <c r="B94" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C94" s="4" t="s">
@@ -12792,10 +12733,10 @@
       </c>
     </row>
     <row r="95" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A95" s="28" t="s">
+      <c r="A95" t="s">
         <v>303</v>
       </c>
-      <c r="B95" s="25" t="s">
+      <c r="B95" s="22" t="s">
         <v>426</v>
       </c>
       <c r="D95" s="4"/>
@@ -12810,10 +12751,10 @@
       </c>
     </row>
     <row r="96" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A96" s="28" t="s">
+      <c r="A96" t="s">
         <v>440</v>
       </c>
-      <c r="B96" s="25" t="s">
+      <c r="B96" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C96" s="4" t="s">
@@ -12834,10 +12775,10 @@
       </c>
     </row>
     <row r="97" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A97" s="28" t="s">
+      <c r="A97" t="s">
         <v>486</v>
       </c>
-      <c r="B97" s="25" t="s">
+      <c r="B97" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C97" s="4" t="s">
@@ -12858,10 +12799,10 @@
       </c>
     </row>
     <row r="98" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A98" s="28" t="s">
+      <c r="A98" t="s">
         <v>441</v>
       </c>
-      <c r="B98" s="25" t="s">
+      <c r="B98" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C98" t="s">
@@ -12882,10 +12823,10 @@
       </c>
     </row>
     <row r="99" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A99" s="28" t="s">
+      <c r="A99" t="s">
         <v>471</v>
       </c>
-      <c r="B99" s="25" t="s">
+      <c r="B99" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C99" t="s">
@@ -12923,7 +12864,7 @@
       <c r="A101" t="s">
         <v>571</v>
       </c>
-      <c r="B101" s="25" t="s">
+      <c r="B101" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C101" s="4" t="s">
@@ -12946,7 +12887,7 @@
       <c r="A102" t="s">
         <v>572</v>
       </c>
-      <c r="B102" s="25" t="s">
+      <c r="B102" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C102" s="4" t="s">
@@ -12966,10 +12907,10 @@
       </c>
     </row>
     <row r="103" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A103" s="28" t="s">
+      <c r="A103" t="s">
         <v>551</v>
       </c>
-      <c r="B103" s="25" t="s">
+      <c r="B103" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C103" t="s">
@@ -12987,10 +12928,10 @@
       </c>
     </row>
     <row r="104" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A104" s="28" t="s">
+      <c r="A104" t="s">
         <v>559</v>
       </c>
-      <c r="B104" s="25" t="s">
+      <c r="B104" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C104" t="s">
@@ -13008,10 +12949,10 @@
       </c>
     </row>
     <row r="105" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A105" s="28" t="s">
+      <c r="A105" t="s">
         <v>560</v>
       </c>
-      <c r="B105" s="25" t="s">
+      <c r="B105" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C105" t="s">
@@ -13029,10 +12970,10 @@
       </c>
     </row>
     <row r="106" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A106" s="28" t="s">
+      <c r="A106" t="s">
         <v>490</v>
       </c>
-      <c r="B106" s="25" t="s">
+      <c r="B106" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C106" s="4" t="s">
@@ -13050,10 +12991,10 @@
       </c>
     </row>
     <row r="107" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A107" s="28" t="s">
+      <c r="A107" t="s">
         <v>284</v>
       </c>
-      <c r="B107" s="25" t="s">
+      <c r="B107" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C107" s="4" t="s">
@@ -13071,10 +13012,10 @@
       </c>
     </row>
     <row r="108" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A108" s="28" t="s">
+      <c r="A108" t="s">
         <v>557</v>
       </c>
-      <c r="B108" s="25" t="s">
+      <c r="B108" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C108" t="s">
@@ -13092,10 +13033,10 @@
       </c>
     </row>
     <row r="109" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A109" s="28" t="s">
+      <c r="A109" t="s">
         <v>457</v>
       </c>
-      <c r="B109" s="25" t="s">
+      <c r="B109" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C109" s="4" t="s">
@@ -13113,10 +13054,10 @@
       </c>
     </row>
     <row r="110" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A110" s="28" t="s">
+      <c r="A110" t="s">
         <v>287</v>
       </c>
-      <c r="B110" s="25" t="s">
+      <c r="B110" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C110" s="4" t="s">
@@ -13136,10 +13077,10 @@
       </c>
     </row>
     <row r="111" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A111" s="28" t="s">
+      <c r="A111" t="s">
         <v>324</v>
       </c>
-      <c r="B111" s="25" t="s">
+      <c r="B111" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C111" t="s">
@@ -13160,10 +13101,10 @@
       </c>
     </row>
     <row r="112" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A112" s="28" t="s">
+      <c r="A112" t="s">
         <v>406</v>
       </c>
-      <c r="B112" s="25" t="s">
+      <c r="B112" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C112" t="s">
@@ -13181,10 +13122,10 @@
       </c>
     </row>
     <row r="113" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A113" s="28" t="s">
+      <c r="A113" t="s">
         <v>410</v>
       </c>
-      <c r="B113" s="25" t="s">
+      <c r="B113" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C113" s="4" t="s">
@@ -13202,10 +13143,10 @@
       </c>
     </row>
     <row r="114" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A114" s="28" t="s">
+      <c r="A114" t="s">
         <v>498</v>
       </c>
-      <c r="B114" s="25" t="s">
+      <c r="B114" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C114" t="s">
@@ -13225,10 +13166,10 @@
       </c>
     </row>
     <row r="115" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A115" s="28" t="s">
+      <c r="A115" t="s">
         <v>325</v>
       </c>
-      <c r="B115" s="25" t="s">
+      <c r="B115" s="22" t="s">
         <v>426</v>
       </c>
       <c r="D115" s="4"/>
@@ -13243,10 +13184,10 @@
       </c>
     </row>
     <row r="116" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A116" s="28" t="s">
+      <c r="A116" t="s">
         <v>288</v>
       </c>
-      <c r="B116" s="25" t="s">
+      <c r="B116" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C116" s="4" t="s">
@@ -13266,10 +13207,10 @@
       </c>
     </row>
     <row r="117" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A117" s="28" t="s">
+      <c r="A117" t="s">
         <v>290</v>
       </c>
-      <c r="B117" s="25" t="s">
+      <c r="B117" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C117" s="4" t="s">
@@ -13287,10 +13228,10 @@
       </c>
     </row>
     <row r="118" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A118" s="28" t="s">
+      <c r="A118" t="s">
         <v>511</v>
       </c>
-      <c r="B118" s="25" t="s">
+      <c r="B118" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C118" s="4" t="s">
@@ -13308,10 +13249,10 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A119" s="28" t="s">
+      <c r="A119" t="s">
         <v>398</v>
       </c>
-      <c r="B119" s="25" t="s">
+      <c r="B119" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C119" s="4" t="s">
@@ -13329,10 +13270,10 @@
       </c>
     </row>
     <row r="120" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A120" s="28" t="s">
+      <c r="A120" t="s">
         <v>399</v>
       </c>
-      <c r="B120" s="25" t="s">
+      <c r="B120" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C120" s="4" t="s">
@@ -13350,10 +13291,10 @@
       </c>
     </row>
     <row r="121" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A121" s="28" t="s">
+      <c r="A121" t="s">
         <v>289</v>
       </c>
-      <c r="B121" s="25" t="s">
+      <c r="B121" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C121" s="4" t="s">
@@ -13374,10 +13315,10 @@
       </c>
     </row>
     <row r="122" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A122" s="28" t="s">
+      <c r="A122" t="s">
         <v>405</v>
       </c>
-      <c r="B122" s="25" t="s">
+      <c r="B122" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C122" s="4" t="s">
@@ -13398,10 +13339,10 @@
       </c>
     </row>
     <row r="123" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A123" s="28" t="s">
+      <c r="A123" t="s">
         <v>472</v>
       </c>
-      <c r="B123" s="25" t="s">
+      <c r="B123" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C123" t="s">
@@ -13419,10 +13360,10 @@
       </c>
     </row>
     <row r="124" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A124" s="28" t="s">
+      <c r="A124" t="s">
         <v>495</v>
       </c>
-      <c r="B124" s="25" t="s">
+      <c r="B124" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C124" s="4" t="s">
@@ -13440,10 +13381,10 @@
       </c>
     </row>
     <row r="125" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A125" s="28" t="s">
+      <c r="A125" t="s">
         <v>491</v>
       </c>
-      <c r="B125" s="25" t="s">
+      <c r="B125" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C125" s="4" t="s">
@@ -13461,10 +13402,10 @@
       </c>
     </row>
     <row r="126" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A126" s="28" t="s">
+      <c r="A126" t="s">
         <v>283</v>
       </c>
-      <c r="B126" s="25" t="s">
+      <c r="B126" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C126" s="4" t="s">
@@ -13482,10 +13423,10 @@
       </c>
     </row>
     <row r="127" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A127" s="28" t="s">
+      <c r="A127" t="s">
         <v>558</v>
       </c>
-      <c r="B127" s="25" t="s">
+      <c r="B127" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C127" t="s">
@@ -13503,10 +13444,10 @@
       </c>
     </row>
     <row r="128" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A128" s="28" t="s">
+      <c r="A128" t="s">
         <v>456</v>
       </c>
-      <c r="B128" s="25" t="s">
+      <c r="B128" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C128" s="4" t="s">
@@ -13524,10 +13465,10 @@
       </c>
     </row>
     <row r="129" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A129" s="28" t="s">
+      <c r="A129" t="s">
         <v>275</v>
       </c>
-      <c r="B129" s="25" t="s">
+      <c r="B129" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C129" s="4" t="s">
@@ -13547,10 +13488,10 @@
       </c>
     </row>
     <row r="130" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A130" s="28" t="s">
+      <c r="A130" t="s">
         <v>327</v>
       </c>
-      <c r="B130" s="25" t="s">
+      <c r="B130" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C130" t="s">
@@ -13571,10 +13512,10 @@
       </c>
     </row>
     <row r="131" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A131" s="28" t="s">
+      <c r="A131" t="s">
         <v>276</v>
       </c>
-      <c r="B131" s="25" t="s">
+      <c r="B131" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C131" s="4" t="s">
@@ -13594,10 +13535,10 @@
       </c>
     </row>
     <row r="132" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A132" s="28" t="s">
+      <c r="A132" t="s">
         <v>389</v>
       </c>
-      <c r="B132" s="25" t="s">
+      <c r="B132" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C132" s="4" t="s">
@@ -13615,10 +13556,10 @@
       </c>
     </row>
     <row r="133" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A133" s="28" t="s">
+      <c r="A133" t="s">
         <v>326</v>
       </c>
-      <c r="B133" s="25" t="s">
+      <c r="B133" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C133" s="4" t="s">
@@ -13636,10 +13577,10 @@
       </c>
     </row>
     <row r="134" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A134" s="28" t="s">
+      <c r="A134" t="s">
         <v>393</v>
       </c>
-      <c r="B134" s="25" t="s">
+      <c r="B134" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C134" s="4" t="s">
@@ -13657,10 +13598,10 @@
       </c>
     </row>
     <row r="135" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A135" s="28" t="s">
+      <c r="A135" t="s">
         <v>325</v>
       </c>
-      <c r="B135" s="25" t="s">
+      <c r="B135" s="22" t="s">
         <v>426</v>
       </c>
       <c r="D135" s="4"/>
@@ -13675,10 +13616,10 @@
       </c>
     </row>
     <row r="136" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A136" s="28" t="s">
+      <c r="A136" t="s">
         <v>274</v>
       </c>
-      <c r="B136" s="25" t="s">
+      <c r="B136" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C136" s="4" t="s">
@@ -13696,10 +13637,10 @@
       </c>
     </row>
     <row r="137" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A137" s="28" t="s">
+      <c r="A137" t="s">
         <v>286</v>
       </c>
-      <c r="B137" s="25" t="s">
+      <c r="B137" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C137" s="4" t="s">
@@ -13717,10 +13658,10 @@
       </c>
     </row>
     <row r="138" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A138" s="28" t="s">
+      <c r="A138" t="s">
         <v>396</v>
       </c>
-      <c r="B138" s="25" t="s">
+      <c r="B138" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C138" s="4" t="s">
@@ -13738,10 +13679,10 @@
       </c>
     </row>
     <row r="139" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A139" s="28" t="s">
+      <c r="A139" t="s">
         <v>285</v>
       </c>
-      <c r="B139" s="25" t="s">
+      <c r="B139" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C139" s="4" t="s">
@@ -13759,10 +13700,10 @@
       </c>
     </row>
     <row r="140" spans="1:8" s="8" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A140" s="30" t="s">
+      <c r="A140" s="8" t="s">
         <v>387</v>
       </c>
-      <c r="B140" s="25" t="s">
+      <c r="B140" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C140" s="8" t="s">
@@ -13781,10 +13722,10 @@
       <c r="H140" s="14"/>
     </row>
     <row r="141" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A141" s="28" t="s">
+      <c r="A141" t="s">
         <v>295</v>
       </c>
-      <c r="B141" s="25" t="s">
+      <c r="B141" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D141" s="4"/>
@@ -13799,7 +13740,7 @@
       </c>
     </row>
     <row r="142" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A142" s="28" t="s">
+      <c r="A142" t="s">
         <v>452</v>
       </c>
       <c r="C142" s="4" t="s">
@@ -13831,7 +13772,7 @@
       </c>
     </row>
     <row r="144" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A144" s="28" t="s">
+      <c r="A144" t="s">
         <v>458</v>
       </c>
       <c r="C144" s="4" t="s">
@@ -13863,7 +13804,7 @@
       </c>
     </row>
     <row r="146" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A146" s="28" t="s">
+      <c r="A146" t="s">
         <v>459</v>
       </c>
       <c r="C146" s="4" t="s">
@@ -13934,10 +13875,10 @@
       <c r="H150"/>
     </row>
     <row r="151" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A151" s="28" t="s">
+      <c r="A151" t="s">
         <v>293</v>
       </c>
-      <c r="B151" s="25" t="s">
+      <c r="B151" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C151" s="4" t="s">
@@ -13956,10 +13897,10 @@
       <c r="H151"/>
     </row>
     <row r="152" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A152" s="28" t="s">
+      <c r="A152" t="s">
         <v>331</v>
       </c>
-      <c r="B152" s="25" t="s">
+      <c r="B152" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D152" s="4"/>
@@ -13975,10 +13916,10 @@
       <c r="H152"/>
     </row>
     <row r="153" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A153" s="28" t="s">
+      <c r="A153" t="s">
         <v>330</v>
       </c>
-      <c r="B153" s="25" t="s">
+      <c r="B153" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D153" s="4"/>
@@ -14020,10 +13961,10 @@
       <c r="H155"/>
     </row>
     <row r="156" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A156" s="28" t="s">
+      <c r="A156" t="s">
         <v>294</v>
       </c>
-      <c r="B156" s="25" t="s">
+      <c r="B156" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D156" s="4"/>
@@ -14039,10 +13980,10 @@
       <c r="H156"/>
     </row>
     <row r="157" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A157" s="28" t="s">
+      <c r="A157" t="s">
         <v>546</v>
       </c>
-      <c r="B157" s="25" t="s">
+      <c r="B157" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D157" s="4"/>
@@ -14089,10 +14030,10 @@
       <c r="H159"/>
     </row>
     <row r="160" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A160" s="28" t="s">
+      <c r="A160" t="s">
         <v>273</v>
       </c>
-      <c r="B160" s="25" t="s">
+      <c r="B160" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C160" s="4" t="s">
@@ -14114,7 +14055,7 @@
       <c r="A161" s="8" t="s">
         <v>442</v>
       </c>
-      <c r="B161" s="25" t="s">
+      <c r="B161" s="22" t="s">
         <v>426</v>
       </c>
       <c r="D161" s="4"/>
@@ -14156,10 +14097,10 @@
       <c r="H163"/>
     </row>
     <row r="164" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A164" s="28" t="s">
+      <c r="A164" t="s">
         <v>308</v>
       </c>
-      <c r="B164" s="25" t="s">
+      <c r="B164" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C164" t="s">
@@ -14192,10 +14133,10 @@
       </c>
     </row>
     <row r="166" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A166" s="28" t="s">
+      <c r="A166" t="s">
         <v>317</v>
       </c>
-      <c r="B166" s="25" t="s">
+      <c r="B166" s="22" t="s">
         <v>426</v>
       </c>
       <c r="D166" s="4"/>
@@ -14222,10 +14163,10 @@
       </c>
     </row>
     <row r="168" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A168" s="28" t="s">
+      <c r="A168" t="s">
         <v>361</v>
       </c>
-      <c r="B168" s="25" t="s">
+      <c r="B168" s="22" t="s">
         <v>427</v>
       </c>
       <c r="D168" s="10" t="s">
@@ -14268,7 +14209,7 @@
       </c>
     </row>
     <row r="171" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A171" s="28" t="s">
+      <c r="A171" t="s">
         <v>429</v>
       </c>
       <c r="D171" s="4"/>
@@ -14283,10 +14224,10 @@
       </c>
     </row>
     <row r="172" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A172" s="28" t="s">
+      <c r="A172" t="s">
         <v>493</v>
       </c>
-      <c r="B172" s="25" t="s">
+      <c r="B172" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C172" t="s">
@@ -14307,10 +14248,10 @@
       </c>
     </row>
     <row r="173" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A173" s="28" t="s">
+      <c r="A173" t="s">
         <v>388</v>
       </c>
-      <c r="B173" s="25" t="s">
+      <c r="B173" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C173" t="s">
@@ -14328,10 +14269,10 @@
       </c>
     </row>
     <row r="174" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A174" s="28" t="s">
+      <c r="A174" t="s">
         <v>478</v>
       </c>
-      <c r="B174" s="25" t="s">
+      <c r="B174" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C174" t="s">
@@ -14376,7 +14317,7 @@
       </c>
     </row>
     <row r="177" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A177" s="28" t="s">
+      <c r="A177" t="s">
         <v>272</v>
       </c>
       <c r="D177" s="4"/>
@@ -14403,10 +14344,10 @@
       </c>
     </row>
     <row r="179" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A179" s="28" t="s">
+      <c r="A179" t="s">
         <v>271</v>
       </c>
-      <c r="B179" s="25" t="s">
+      <c r="B179" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C179" s="4" t="s">
@@ -14460,7 +14401,7 @@
       </c>
     </row>
     <row r="183" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A183" s="28" t="s">
+      <c r="A183" t="s">
         <v>270</v>
       </c>
       <c r="D183" s="4"/>
@@ -14475,7 +14416,7 @@
       </c>
     </row>
     <row r="184" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A184" s="28" t="s">
+      <c r="A184" t="s">
         <v>269</v>
       </c>
       <c r="D184" s="4"/>
@@ -14502,10 +14443,10 @@
       </c>
     </row>
     <row r="186" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A186" s="28" t="s">
+      <c r="A186" t="s">
         <v>311</v>
       </c>
-      <c r="B186" s="25" t="s">
+      <c r="B186" s="22" t="s">
         <v>426</v>
       </c>
       <c r="D186" s="4"/>
@@ -14523,10 +14464,10 @@
       </c>
     </row>
     <row r="187" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A187" s="28" t="s">
+      <c r="A187" t="s">
         <v>265</v>
       </c>
-      <c r="B187" s="25" t="s">
+      <c r="B187" s="22" t="s">
         <v>427</v>
       </c>
       <c r="C187" t="s">
@@ -14652,10 +14593,10 @@
       </c>
     </row>
     <row r="197" spans="1:8" s="15" customFormat="1" ht="20.100000000000001" customHeight="1">
-      <c r="A197" s="31" t="s">
+      <c r="A197" s="15" t="s">
         <v>431</v>
       </c>
-      <c r="B197" s="27"/>
+      <c r="B197" s="24"/>
       <c r="D197" s="19" t="s">
         <v>342</v>
       </c>
@@ -14783,7 +14724,7 @@
       </c>
     </row>
     <row r="207" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A207" s="28" t="s">
+      <c r="A207" t="s">
         <v>328</v>
       </c>
       <c r="C207" t="s">
@@ -14825,10 +14766,10 @@
       </c>
     </row>
     <row r="210" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A210" s="28" t="s">
+      <c r="A210" t="s">
         <v>509</v>
       </c>
-      <c r="B210" s="25" t="s">
+      <c r="B210" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C210" t="s">
@@ -14846,10 +14787,10 @@
       </c>
     </row>
     <row r="211" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A211" s="28" t="s">
+      <c r="A211" t="s">
         <v>408</v>
       </c>
-      <c r="B211" s="25" t="s">
+      <c r="B211" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C211" s="4" t="s">
@@ -14869,10 +14810,10 @@
       </c>
     </row>
     <row r="212" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A212" s="28" t="s">
+      <c r="A212" t="s">
         <v>419</v>
       </c>
-      <c r="B212" s="25" t="s">
+      <c r="B212" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C212" s="4" t="s">
@@ -14890,10 +14831,10 @@
       </c>
     </row>
     <row r="213" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A213" s="29" t="s">
+      <c r="A213" s="25" t="s">
         <v>314</v>
       </c>
-      <c r="B213" s="25" t="s">
+      <c r="B213" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C213" s="4" t="s">
@@ -14911,10 +14852,10 @@
       </c>
     </row>
     <row r="214" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A214" s="28" t="s">
+      <c r="A214" t="s">
         <v>315</v>
       </c>
-      <c r="B214" s="25" t="s">
+      <c r="B214" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C214" s="4" t="s">
@@ -14958,10 +14899,10 @@
       </c>
     </row>
     <row r="217" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A217" s="28" t="s">
+      <c r="A217" t="s">
         <v>404</v>
       </c>
-      <c r="B217" s="25" t="s">
+      <c r="B217" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C217" s="4" t="s">
@@ -14979,7 +14920,7 @@
       </c>
     </row>
     <row r="218" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A218" s="30" t="s">
+      <c r="A218" s="8" t="s">
         <v>432</v>
       </c>
       <c r="D218" s="4"/>
@@ -15030,10 +14971,10 @@
       </c>
     </row>
     <row r="222" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A222" s="28" t="s">
+      <c r="A222" t="s">
         <v>411</v>
       </c>
-      <c r="B222" s="25" t="s">
+      <c r="B222" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C222" s="4" t="s">
@@ -15051,7 +14992,7 @@
       </c>
     </row>
     <row r="223" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A223" s="28" t="s">
+      <c r="A223" t="s">
         <v>281</v>
       </c>
       <c r="C223" s="4" t="s">
@@ -15069,10 +15010,10 @@
       </c>
     </row>
     <row r="224" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A224" s="28" t="s">
+      <c r="A224" t="s">
         <v>280</v>
       </c>
-      <c r="B224" s="25" t="s">
+      <c r="B224" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C224" t="s">
@@ -15114,10 +15055,10 @@
       </c>
     </row>
     <row r="227" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A227" s="28" t="s">
+      <c r="A227" t="s">
         <v>414</v>
       </c>
-      <c r="B227" s="25" t="s">
+      <c r="B227" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C227" s="4" t="s">
@@ -15135,10 +15076,10 @@
       </c>
     </row>
     <row r="228" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A228" s="28" t="s">
+      <c r="A228" t="s">
         <v>416</v>
       </c>
-      <c r="B228" s="25" t="s">
+      <c r="B228" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C228" s="4" t="s">
@@ -15156,10 +15097,10 @@
       </c>
     </row>
     <row r="229" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A229" s="28" t="s">
+      <c r="A229" t="s">
         <v>278</v>
       </c>
-      <c r="B229" s="25" t="s">
+      <c r="B229" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C229" s="4" t="s">
@@ -15182,10 +15123,10 @@
       </c>
     </row>
     <row r="230" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A230" s="28" t="s">
+      <c r="A230" t="s">
         <v>466</v>
       </c>
-      <c r="B230" s="25" t="s">
+      <c r="B230" s="22" t="s">
         <v>428</v>
       </c>
       <c r="C230" t="s">
@@ -15288,10 +15229,10 @@
       <c r="H236"/>
     </row>
     <row r="237" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A237" s="28" t="s">
+      <c r="A237" t="s">
         <v>296</v>
       </c>
-      <c r="B237" s="25" t="s">
+      <c r="B237" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C237" t="s">
@@ -15336,7 +15277,7 @@
       <c r="H239"/>
     </row>
     <row r="240" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A240" s="28" t="s">
+      <c r="A240" t="s">
         <v>433</v>
       </c>
       <c r="D240" s="4"/>
@@ -15352,7 +15293,7 @@
       <c r="H240"/>
     </row>
     <row r="241" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A241" s="28" t="s">
+      <c r="A241" t="s">
         <v>434</v>
       </c>
       <c r="D241" s="4"/>
@@ -15394,10 +15335,10 @@
       <c r="H243"/>
     </row>
     <row r="244" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A244" s="28" t="s">
+      <c r="A244" t="s">
         <v>468</v>
       </c>
-      <c r="B244" s="25" t="s">
+      <c r="B244" s="22" t="s">
         <v>426</v>
       </c>
       <c r="C244" t="s">
@@ -15507,10 +15448,10 @@
       <c r="H251"/>
     </row>
     <row r="252" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A252" s="28" t="s">
+      <c r="A252" t="s">
         <v>582</v>
       </c>
-      <c r="B252" s="25" t="s">
+      <c r="B252" s="22" t="s">
         <v>583</v>
       </c>
       <c r="C252" t="s">
@@ -15527,10 +15468,10 @@
       </c>
     </row>
     <row r="253" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A253" s="28" t="s">
+      <c r="A253" t="s">
         <v>585</v>
       </c>
-      <c r="B253" s="25" t="s">
+      <c r="B253" s="22" t="s">
         <v>583</v>
       </c>
       <c r="C253" t="s">
@@ -15547,10 +15488,10 @@
       </c>
     </row>
     <row r="254" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A254" s="28" t="s">
+      <c r="A254" t="s">
         <v>586</v>
       </c>
-      <c r="B254" s="25" t="s">
+      <c r="B254" s="22" t="s">
         <v>583</v>
       </c>
       <c r="C254" t="s">
@@ -15567,10 +15508,10 @@
       </c>
     </row>
     <row r="255" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A255" s="28" t="s">
+      <c r="A255" t="s">
         <v>593</v>
       </c>
-      <c r="B255" s="25" t="s">
+      <c r="B255" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C255" t="s">
@@ -15587,10 +15528,10 @@
       </c>
     </row>
     <row r="256" spans="1:8" ht="20.100000000000001" customHeight="1">
-      <c r="A256" s="28" t="s">
+      <c r="A256" t="s">
         <v>596</v>
       </c>
-      <c r="B256" s="25" t="s">
+      <c r="B256" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C256" t="s">
@@ -15607,10 +15548,10 @@
       </c>
     </row>
     <row r="257" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A257" s="28" t="s">
+      <c r="A257" t="s">
         <v>597</v>
       </c>
-      <c r="B257" s="25" t="s">
+      <c r="B257" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C257" t="s">
@@ -15627,10 +15568,10 @@
       </c>
     </row>
     <row r="258" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A258" s="28" t="s">
+      <c r="A258" t="s">
         <v>598</v>
       </c>
-      <c r="B258" s="25" t="s">
+      <c r="B258" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C258" t="s">
@@ -15647,10 +15588,10 @@
       </c>
     </row>
     <row r="259" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A259" s="28" t="s">
+      <c r="A259" t="s">
         <v>599</v>
       </c>
-      <c r="B259" s="25" t="s">
+      <c r="B259" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C259" t="s">
@@ -15667,10 +15608,10 @@
       </c>
     </row>
     <row r="260" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A260" s="28" t="s">
+      <c r="A260" t="s">
         <v>600</v>
       </c>
-      <c r="B260" s="25" t="s">
+      <c r="B260" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C260" t="s">
@@ -15687,10 +15628,10 @@
       </c>
     </row>
     <row r="261" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A261" s="28" t="s">
+      <c r="A261" t="s">
         <v>601</v>
       </c>
-      <c r="B261" s="25" t="s">
+      <c r="B261" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C261" t="s">
@@ -15707,10 +15648,10 @@
       </c>
     </row>
     <row r="262" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A262" s="28" t="s">
+      <c r="A262" t="s">
         <v>602</v>
       </c>
-      <c r="B262" s="25" t="s">
+      <c r="B262" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C262" t="s">
@@ -15727,10 +15668,10 @@
       </c>
     </row>
     <row r="263" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A263" s="28" t="s">
+      <c r="A263" t="s">
         <v>603</v>
       </c>
-      <c r="B263" s="25" t="s">
+      <c r="B263" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C263" t="s">
@@ -15747,10 +15688,10 @@
       </c>
     </row>
     <row r="264" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A264" s="28" t="s">
+      <c r="A264" t="s">
         <v>604</v>
       </c>
-      <c r="B264" s="25" t="s">
+      <c r="B264" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C264" t="s">
@@ -15767,10 +15708,10 @@
       </c>
     </row>
     <row r="265" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A265" s="28" t="s">
+      <c r="A265" t="s">
         <v>605</v>
       </c>
-      <c r="B265" s="25" t="s">
+      <c r="B265" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C265" t="s">
@@ -15787,10 +15728,10 @@
       </c>
     </row>
     <row r="266" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A266" s="28" t="s">
+      <c r="A266" t="s">
         <v>626</v>
       </c>
-      <c r="B266" s="25" t="s">
+      <c r="B266" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C266" t="s">
@@ -15807,10 +15748,10 @@
       </c>
     </row>
     <row r="267" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A267" s="28" t="s">
+      <c r="A267" t="s">
         <v>627</v>
       </c>
-      <c r="B267" s="25" t="s">
+      <c r="B267" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C267" t="s">
@@ -15827,10 +15768,10 @@
       </c>
     </row>
     <row r="268" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A268" s="28" t="s">
+      <c r="A268" t="s">
         <v>628</v>
       </c>
-      <c r="B268" s="25" t="s">
+      <c r="B268" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C268" t="s">
@@ -15847,10 +15788,10 @@
       </c>
     </row>
     <row r="269" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A269" s="28" t="s">
+      <c r="A269" t="s">
         <v>629</v>
       </c>
-      <c r="B269" s="25" t="s">
+      <c r="B269" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C269" t="s">
@@ -15867,10 +15808,10 @@
       </c>
     </row>
     <row r="270" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A270" s="28" t="s">
+      <c r="A270" t="s">
         <v>638</v>
       </c>
-      <c r="B270" s="25" t="s">
+      <c r="B270" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C270" t="s">
@@ -15887,10 +15828,10 @@
       </c>
     </row>
     <row r="271" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A271" s="28" t="s">
+      <c r="A271" t="s">
         <v>646</v>
       </c>
-      <c r="B271" s="25" t="s">
+      <c r="B271" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C271" t="s">
@@ -15907,10 +15848,10 @@
       </c>
     </row>
     <row r="272" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A272" s="28" t="s">
+      <c r="A272" t="s">
         <v>645</v>
       </c>
-      <c r="B272" s="25" t="s">
+      <c r="B272" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C272" t="s">
@@ -15927,10 +15868,10 @@
       </c>
     </row>
     <row r="273" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A273" s="28" t="s">
+      <c r="A273" t="s">
         <v>647</v>
       </c>
-      <c r="B273" s="25" t="s">
+      <c r="B273" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C273" t="s">
@@ -15947,10 +15888,10 @@
       </c>
     </row>
     <row r="274" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A274" s="28" t="s">
+      <c r="A274" t="s">
         <v>648</v>
       </c>
-      <c r="B274" s="25" t="s">
+      <c r="B274" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C274" t="s">
@@ -15967,10 +15908,10 @@
       </c>
     </row>
     <row r="275" spans="1:7" ht="20.100000000000001" customHeight="1">
-      <c r="A275" s="28" t="s">
+      <c r="A275" t="s">
         <v>649</v>
       </c>
-      <c r="B275" s="25" t="s">
+      <c r="B275" s="22" t="s">
         <v>575</v>
       </c>
       <c r="C275" t="s">
@@ -15987,73 +15928,33 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J165">
-    <cfRule type="expression" priority="16">
+  <conditionalFormatting sqref="A1:XFD110 A112:XFD125 A126:A129 C126:XFD129 D130:XFD130 A131:A140 C131:XFD140 A197:C197 F197:XFD197 A198:XFD211 A212 A214:XFD229 A230:B230 D230:XFD230 B252:XFD254 A255:XFD1048576">
+    <cfRule type="expression" dxfId="6" priority="15">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D213:XFD213 D130:XFD130 A197:C197 F197:XFD197 A198:XFD211 A126:A129 C126:XFD129 A131:A140 C131:XFD140 A162:XFD163 A165:XFD165 A164 C164:XFD164 A166 C166:XFD166 A167:XFD171 A172 A188:XFD196 A186:A187 C186:XFD187 A212 C212:XFD212 A238:XFD243 A237 C237:XFD237 A160:A161 C160:XFD161 A231:XFD236 A230:B230 D230:XFD230 A244 C244:XFD244 A173:XFD185 C172:XFD172 A214:XFD229 A112:XFD125 B212:B213 A141:XFD159 A245:XFD251 A1:XFD110 B252:XFD254 A255:XFD1048576">
-    <cfRule type="expression" dxfId="13" priority="15">
+  <conditionalFormatting sqref="A141:XFD196">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C213">
-    <cfRule type="expression" dxfId="12" priority="14">
+  <conditionalFormatting sqref="A231:XFD251">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B111">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B126:B140">
-    <cfRule type="expression" dxfId="11" priority="13">
+    <cfRule type="expression" dxfId="2" priority="13">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B160">
-    <cfRule type="expression" dxfId="10" priority="12">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B164">
-    <cfRule type="expression" dxfId="9" priority="11">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B166">
-    <cfRule type="expression" dxfId="8" priority="10">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B172">
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B187">
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B186">
-    <cfRule type="expression" dxfId="5" priority="7">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B237">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B161">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B244">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B111">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="B212:XFD213">
+    <cfRule type="expression" dxfId="1" priority="14">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16062,6 +15963,11 @@
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J165">
+    <cfRule type="expression" priority="16">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
part-way through reordering of crop production model
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A90F9E8-859B-4FA4-9E34-51ABAE98B7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E56E9CE-4759-4B9D-AFB1-B0A0574A4273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5460" yWindow="630" windowWidth="22560" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11086,8 +11086,8 @@
   <dimension ref="A1:H275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
+      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A212" sqref="A212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>

</xml_diff>

<commit_message>
corrected spelling in Orator variables lookup table.xlsx
</commit_message>
<xml_diff>
--- a/OratorRun/lookup/Orator variables lookup table.xlsx
+++ b/OratorRun/lookup/Orator variables lookup table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PyOraDev\testPyOra\OratorRun\lookup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E56E9CE-4759-4B9D-AFB1-B0A0574A4273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED1829C-47DE-4179-90E2-767DF80327E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="630" windowWidth="22560" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29655" yWindow="930" windowWidth="22260" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Appendix A" sheetId="1" r:id="rId1"/>
@@ -2823,9 +2823,6 @@
     <t>Relative Food Insecutiry (N Limited)</t>
   </si>
   <si>
-    <t>Dietary Divertsity (N Limited)</t>
-  </si>
-  <si>
     <t>ETB/Y</t>
   </si>
   <si>
@@ -2842,6 +2839,9 @@
   </si>
   <si>
     <t>harv_indx</t>
+  </si>
+  <si>
+    <t>Dietary Diversity (N Limited)</t>
   </si>
 </sst>
 </file>
@@ -10786,9 +10786,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -10826,7 +10826,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -10932,7 +10932,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -11074,7 +11074,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -11086,8 +11086,8 @@
   <dimension ref="A1:H275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A198" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A212" sqref="A212"/>
+      <pane ySplit="1" topLeftCell="A258" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C281" sqref="C281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -12165,7 +12165,7 @@
     </row>
     <row r="63" spans="1:8" ht="20.100000000000001" customHeight="1">
       <c r="A63" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D63" s="10" t="s">
         <v>359</v>
@@ -15878,10 +15878,10 @@
         <v>650</v>
       </c>
       <c r="E273" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F273" s="5" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G273" s="6" t="s">
         <v>7</v>
@@ -15898,7 +15898,7 @@
         <v>651</v>
       </c>
       <c r="E274" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F274" s="5" t="s">
         <v>228</v>
@@ -15915,13 +15915,13 @@
         <v>575</v>
       </c>
       <c r="C275" t="s">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="E275" t="s">
+        <v>655</v>
+      </c>
+      <c r="F275" s="5" t="s">
         <v>656</v>
-      </c>
-      <c r="F275" s="5" t="s">
-        <v>657</v>
       </c>
       <c r="G275" s="6" t="s">
         <v>7</v>

</xml_diff>